<commit_message>
Fixed bug when using loadPNG instead of loadImage. Added idlekicker functionality to server. Added return to login when kicked. Added return to login screen message for use when logging clients out from the server. Fixed NPE in Start talking event, see comments for clarification.
</commit_message>
<xml_diff>
--- a/Miscellaneous/Packets.xlsx
+++ b/Miscellaneous/Packets.xlsx
@@ -5,11 +5,11 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Rémy Baratté\Documents\Pokemonium\Miscellaneous\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Remy Baratte\Documents\Pokemonium\Miscellaneous\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="16380" windowHeight="8190" tabRatio="947"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="16380" windowHeight="8190" tabRatio="947" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Server TCP" sheetId="1" r:id="rId1"/>
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="957" uniqueCount="533">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="962" uniqueCount="534">
   <si>
     <t>Message ID</t>
   </si>
@@ -1620,6 +1620,9 @@
   </si>
   <si>
     <t>Warp Player to player</t>
+  </si>
+  <si>
+    <t>Return to Login Screen</t>
   </si>
 </sst>
 </file>
@@ -1956,7 +1959,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G67"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A33" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView topLeftCell="A38" zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="F68" sqref="F68"/>
     </sheetView>
   </sheetViews>
@@ -3210,10 +3213,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:AMK121"/>
+  <dimension ref="A1:AMK122"/>
   <sheetViews>
-    <sheetView topLeftCell="A77" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C94" sqref="C94"/>
+    <sheetView tabSelected="1" topLeftCell="A107" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="F122" sqref="F122"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5300,6 +5303,23 @@
         <v>144</v>
       </c>
       <c r="F121" s="2" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="122" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A122" s="3" t="s">
+        <v>527</v>
+      </c>
+      <c r="B122" s="4" t="s">
+        <v>67</v>
+      </c>
+      <c r="C122" s="4" t="s">
+        <v>533</v>
+      </c>
+      <c r="E122" s="4" t="s">
+        <v>144</v>
+      </c>
+      <c r="F122" s="5" t="s">
         <v>15</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Refactored Announcements and Notifications towards clients. Removed old ui test classes. Checked all TODO's and reviewed them with Sadhi and Myth1c. Random cleanup related to TODO's.
</commit_message>
<xml_diff>
--- a/Miscellaneous/Packets.xlsx
+++ b/Miscellaneous/Packets.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="16380" windowHeight="8190" tabRatio="947" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="16380" windowHeight="8190" tabRatio="947"/>
   </bookViews>
   <sheets>
     <sheet name="Server TCP" sheetId="1" r:id="rId1"/>
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="962" uniqueCount="534">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="967" uniqueCount="534">
   <si>
     <t>Message ID</t>
   </si>
@@ -230,9 +230,6 @@
     <t>Ml</t>
   </si>
   <si>
-    <t>Send an Alert</t>
-  </si>
-  <si>
     <t>Implement</t>
   </si>
   <si>
@@ -323,15 +320,6 @@
     <t>Stop Server</t>
   </si>
   <si>
-    <t>Mn</t>
-  </si>
-  <si>
-    <t>Announce Message to Server</t>
-  </si>
-  <si>
-    <t>Announces to Map</t>
-  </si>
-  <si>
     <t>bm</t>
   </si>
   <si>
@@ -1623,6 +1611,18 @@
   </si>
   <si>
     <t>Return to Login Screen</t>
+  </si>
+  <si>
+    <t>Alert Clients</t>
+  </si>
+  <si>
+    <t>52</t>
+  </si>
+  <si>
+    <t>25</t>
+  </si>
+  <si>
+    <t>Notify Clients</t>
   </si>
 </sst>
 </file>
@@ -1957,10 +1957,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G67"/>
+  <dimension ref="A1:G68"/>
   <sheetViews>
-    <sheetView topLeftCell="A38" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="F68" sqref="F68"/>
+    <sheetView tabSelected="1" topLeftCell="A26" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="F45" sqref="F45"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2507,17 +2507,15 @@
     </row>
     <row r="30" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A30" s="2" t="s">
-        <v>67</v>
+        <v>532</v>
       </c>
       <c r="B30" s="2" t="s">
         <v>68</v>
       </c>
       <c r="C30" s="2" t="s">
-        <v>69</v>
-      </c>
-      <c r="D30" s="2" t="s">
-        <v>70</v>
-      </c>
+        <v>533</v>
+      </c>
+      <c r="D30" s="2"/>
       <c r="E30" s="2" t="s">
         <v>8</v>
       </c>
@@ -2530,10 +2528,10 @@
         <v>26</v>
       </c>
       <c r="B31" s="2" t="s">
+        <v>70</v>
+      </c>
+      <c r="C31" s="2" t="s">
         <v>71</v>
-      </c>
-      <c r="C31" s="2" t="s">
-        <v>72</v>
       </c>
       <c r="D31" s="2"/>
       <c r="E31" s="2" t="s">
@@ -2548,10 +2546,10 @@
         <v>27</v>
       </c>
       <c r="B32" s="2" t="s">
+        <v>72</v>
+      </c>
+      <c r="C32" s="2" t="s">
         <v>73</v>
-      </c>
-      <c r="C32" s="2" t="s">
-        <v>74</v>
       </c>
       <c r="D32" s="2"/>
       <c r="E32" s="2" t="s">
@@ -2566,10 +2564,10 @@
         <v>28</v>
       </c>
       <c r="B33" s="2" t="s">
+        <v>74</v>
+      </c>
+      <c r="C33" s="2" t="s">
         <v>75</v>
-      </c>
-      <c r="C33" s="2" t="s">
-        <v>76</v>
       </c>
       <c r="D33" s="2"/>
       <c r="E33" s="2" t="s">
@@ -2584,10 +2582,10 @@
         <v>29</v>
       </c>
       <c r="B34" s="2" t="s">
+        <v>76</v>
+      </c>
+      <c r="C34" s="2" t="s">
         <v>77</v>
-      </c>
-      <c r="C34" s="2" t="s">
-        <v>78</v>
       </c>
       <c r="D34" s="2"/>
       <c r="E34" s="2" t="s">
@@ -2602,10 +2600,10 @@
         <v>30</v>
       </c>
       <c r="B35" s="2" t="s">
+        <v>78</v>
+      </c>
+      <c r="C35" s="2" t="s">
         <v>79</v>
-      </c>
-      <c r="C35" s="2" t="s">
-        <v>80</v>
       </c>
       <c r="D35" s="2"/>
       <c r="E35" s="2" t="s">
@@ -2620,10 +2618,10 @@
         <v>31</v>
       </c>
       <c r="B36" s="2" t="s">
+        <v>80</v>
+      </c>
+      <c r="C36" s="2" t="s">
         <v>81</v>
-      </c>
-      <c r="C36" s="2" t="s">
-        <v>82</v>
       </c>
       <c r="D36" s="2"/>
       <c r="E36" s="2" t="s">
@@ -2638,10 +2636,10 @@
         <v>32</v>
       </c>
       <c r="B37" s="2" t="s">
+        <v>82</v>
+      </c>
+      <c r="C37" s="2" t="s">
         <v>83</v>
-      </c>
-      <c r="C37" s="2" t="s">
-        <v>84</v>
       </c>
       <c r="D37" s="2"/>
       <c r="E37" s="2" t="s">
@@ -2656,13 +2654,13 @@
         <v>32</v>
       </c>
       <c r="B38" s="2" t="s">
+        <v>84</v>
+      </c>
+      <c r="C38" s="2" t="s">
         <v>85</v>
       </c>
-      <c r="C38" s="2" t="s">
+      <c r="D38" s="2" t="s">
         <v>86</v>
-      </c>
-      <c r="D38" s="2" t="s">
-        <v>87</v>
       </c>
       <c r="E38" s="2" t="s">
         <v>8</v>
@@ -2676,13 +2674,13 @@
         <v>32</v>
       </c>
       <c r="B39" s="2" t="s">
+        <v>87</v>
+      </c>
+      <c r="C39" s="2" t="s">
         <v>88</v>
       </c>
-      <c r="C39" s="2" t="s">
+      <c r="D39" s="2" t="s">
         <v>89</v>
-      </c>
-      <c r="D39" s="2" t="s">
-        <v>90</v>
       </c>
       <c r="E39" s="2" t="s">
         <v>8</v>
@@ -2696,13 +2694,13 @@
         <v>32</v>
       </c>
       <c r="B40" s="2" t="s">
+        <v>90</v>
+      </c>
+      <c r="C40" s="2" t="s">
         <v>91</v>
       </c>
-      <c r="C40" s="2" t="s">
+      <c r="D40" s="2" t="s">
         <v>92</v>
-      </c>
-      <c r="D40" s="2" t="s">
-        <v>93</v>
       </c>
       <c r="E40" s="2" t="s">
         <v>8</v>
@@ -2716,10 +2714,10 @@
         <v>32</v>
       </c>
       <c r="B41" s="2" t="s">
+        <v>93</v>
+      </c>
+      <c r="C41" s="2" t="s">
         <v>94</v>
-      </c>
-      <c r="C41" s="2" t="s">
-        <v>95</v>
       </c>
       <c r="D41" s="2"/>
       <c r="E41" s="2" t="s">
@@ -2734,10 +2732,10 @@
         <v>32</v>
       </c>
       <c r="B42" s="2" t="s">
+        <v>95</v>
+      </c>
+      <c r="C42" s="2" t="s">
         <v>96</v>
-      </c>
-      <c r="C42" s="2" t="s">
-        <v>97</v>
       </c>
       <c r="D42" s="2"/>
       <c r="E42" s="2" t="s">
@@ -2752,10 +2750,10 @@
         <v>33</v>
       </c>
       <c r="B43" s="2" t="s">
+        <v>97</v>
+      </c>
+      <c r="C43" s="2" t="s">
         <v>98</v>
-      </c>
-      <c r="C43" s="2" t="s">
-        <v>99</v>
       </c>
       <c r="D43" s="2"/>
       <c r="E43" s="2" t="s">
@@ -2766,17 +2764,17 @@
       </c>
     </row>
     <row r="44" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A44" s="2">
-        <v>34</v>
+      <c r="A44" s="2" t="s">
+        <v>67</v>
       </c>
       <c r="B44" s="2" t="s">
-        <v>100</v>
+        <v>67</v>
       </c>
       <c r="C44" s="2" t="s">
-        <v>101</v>
+        <v>67</v>
       </c>
       <c r="D44" s="2" t="s">
-        <v>102</v>
+        <v>67</v>
       </c>
       <c r="E44" s="2" t="s">
         <v>8</v>
@@ -2790,10 +2788,10 @@
         <v>35</v>
       </c>
       <c r="B45" s="2" t="s">
-        <v>103</v>
+        <v>99</v>
       </c>
       <c r="C45" s="2" t="s">
-        <v>104</v>
+        <v>100</v>
       </c>
       <c r="D45" s="2"/>
       <c r="E45" s="2" t="s">
@@ -2808,10 +2806,10 @@
         <v>36</v>
       </c>
       <c r="B46" s="2" t="s">
-        <v>105</v>
+        <v>101</v>
       </c>
       <c r="C46" s="2" t="s">
-        <v>106</v>
+        <v>102</v>
       </c>
       <c r="D46" s="2"/>
       <c r="E46" s="2" t="s">
@@ -2826,10 +2824,10 @@
         <v>37</v>
       </c>
       <c r="B47" s="2" t="s">
-        <v>107</v>
+        <v>103</v>
       </c>
       <c r="C47" s="2" t="s">
-        <v>108</v>
+        <v>104</v>
       </c>
       <c r="D47" s="2"/>
       <c r="E47" s="2" t="s">
@@ -2844,10 +2842,10 @@
         <v>38</v>
       </c>
       <c r="B48" s="2" t="s">
-        <v>109</v>
+        <v>105</v>
       </c>
       <c r="C48" s="2" t="s">
-        <v>110</v>
+        <v>106</v>
       </c>
       <c r="D48" s="2"/>
       <c r="E48" s="2" t="s">
@@ -2862,10 +2860,10 @@
         <v>39</v>
       </c>
       <c r="B49" s="2" t="s">
-        <v>111</v>
+        <v>107</v>
       </c>
       <c r="C49" s="2" t="s">
-        <v>112</v>
+        <v>108</v>
       </c>
       <c r="D49" s="2"/>
       <c r="E49" s="2" t="s">
@@ -2880,13 +2878,13 @@
         <v>67</v>
       </c>
       <c r="B50" s="2" t="s">
-        <v>113</v>
+        <v>109</v>
       </c>
       <c r="C50" s="2" t="s">
-        <v>114</v>
+        <v>110</v>
       </c>
       <c r="D50" s="2" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="E50" s="2" t="s">
         <v>8</v>
@@ -2900,10 +2898,10 @@
         <v>40</v>
       </c>
       <c r="B51" s="2" t="s">
-        <v>115</v>
+        <v>111</v>
       </c>
       <c r="C51" s="2" t="s">
-        <v>116</v>
+        <v>112</v>
       </c>
       <c r="D51" s="2"/>
       <c r="E51" s="2" t="s">
@@ -2918,10 +2916,10 @@
         <v>51</v>
       </c>
       <c r="B52" s="2" t="s">
-        <v>117</v>
+        <v>113</v>
       </c>
       <c r="C52" s="2" t="s">
-        <v>118</v>
+        <v>114</v>
       </c>
       <c r="D52" s="2"/>
       <c r="E52" s="2" t="s">
@@ -2936,10 +2934,10 @@
         <v>41</v>
       </c>
       <c r="B53" s="2" t="s">
-        <v>119</v>
+        <v>115</v>
       </c>
       <c r="C53" s="2" t="s">
-        <v>120</v>
+        <v>116</v>
       </c>
       <c r="D53" s="2"/>
       <c r="E53" s="2" t="s">
@@ -2954,10 +2952,10 @@
         <v>42</v>
       </c>
       <c r="B54" s="2" t="s">
-        <v>121</v>
+        <v>117</v>
       </c>
       <c r="C54" s="2" t="s">
-        <v>122</v>
+        <v>118</v>
       </c>
       <c r="D54" s="2"/>
       <c r="E54" s="2" t="s">
@@ -2972,10 +2970,10 @@
         <v>43</v>
       </c>
       <c r="B55" s="2" t="s">
-        <v>123</v>
+        <v>119</v>
       </c>
       <c r="C55" s="2" t="s">
-        <v>124</v>
+        <v>120</v>
       </c>
       <c r="D55" s="2"/>
       <c r="E55" s="2" t="s">
@@ -2990,10 +2988,10 @@
         <v>44</v>
       </c>
       <c r="B56" s="2" t="s">
-        <v>125</v>
+        <v>121</v>
       </c>
       <c r="C56" s="2" t="s">
-        <v>126</v>
+        <v>122</v>
       </c>
       <c r="D56" s="2"/>
       <c r="E56" s="2" t="s">
@@ -3008,10 +3006,10 @@
         <v>45</v>
       </c>
       <c r="B57" s="2" t="s">
-        <v>127</v>
+        <v>123</v>
       </c>
       <c r="C57" s="2" t="s">
-        <v>128</v>
+        <v>124</v>
       </c>
       <c r="D57" s="2"/>
       <c r="E57" s="2" t="s">
@@ -3026,13 +3024,13 @@
         <v>46</v>
       </c>
       <c r="B58" s="2" t="s">
-        <v>129</v>
+        <v>125</v>
       </c>
       <c r="C58" s="2" t="s">
-        <v>130</v>
+        <v>126</v>
       </c>
       <c r="D58" s="2" t="s">
-        <v>131</v>
+        <v>127</v>
       </c>
       <c r="E58" s="2" t="s">
         <v>8</v>
@@ -3046,10 +3044,10 @@
         <v>46</v>
       </c>
       <c r="B59" s="2" t="s">
-        <v>132</v>
+        <v>128</v>
       </c>
       <c r="C59" s="2" t="s">
-        <v>133</v>
+        <v>129</v>
       </c>
       <c r="D59" s="2"/>
       <c r="E59" s="2" t="s">
@@ -3064,10 +3062,10 @@
         <v>46</v>
       </c>
       <c r="B60" s="2" t="s">
-        <v>134</v>
+        <v>130</v>
       </c>
       <c r="C60" s="2" t="s">
-        <v>135</v>
+        <v>131</v>
       </c>
       <c r="D60" s="2"/>
       <c r="E60" s="2" t="s">
@@ -3082,10 +3080,10 @@
         <v>47</v>
       </c>
       <c r="B61" s="2" t="s">
-        <v>136</v>
+        <v>132</v>
       </c>
       <c r="C61" s="2" t="s">
-        <v>137</v>
+        <v>133</v>
       </c>
       <c r="D61" s="2"/>
       <c r="E61" s="2" t="s">
@@ -3100,10 +3098,10 @@
         <v>48</v>
       </c>
       <c r="B62" s="2" t="s">
-        <v>138</v>
+        <v>134</v>
       </c>
       <c r="C62" s="2" t="s">
-        <v>139</v>
+        <v>135</v>
       </c>
       <c r="D62" s="2"/>
       <c r="E62" s="2" t="s">
@@ -3118,13 +3116,13 @@
         <v>67</v>
       </c>
       <c r="B63" s="2" t="s">
-        <v>140</v>
+        <v>136</v>
       </c>
       <c r="C63" s="2" t="s">
-        <v>141</v>
+        <v>137</v>
       </c>
       <c r="D63" s="2" t="s">
-        <v>142</v>
+        <v>138</v>
       </c>
       <c r="E63" s="2" t="s">
         <v>8</v>
@@ -3133,33 +3131,33 @@
         <v>15</v>
       </c>
     </row>
-    <row r="64" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A64" s="4" t="s">
-        <v>526</v>
-      </c>
-      <c r="B64" s="4" t="s">
+    <row r="64" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A64" s="2" t="s">
+        <v>531</v>
+      </c>
+      <c r="B64" s="2" t="s">
         <v>67</v>
       </c>
-      <c r="C64" s="4" t="s">
-        <v>355</v>
-      </c>
-      <c r="D64" s="5"/>
-      <c r="E64" s="4" t="s">
+      <c r="C64" s="2" t="s">
+        <v>530</v>
+      </c>
+      <c r="D64" s="2"/>
+      <c r="E64" s="2" t="s">
         <v>8</v>
       </c>
       <c r="F64" s="2" t="s">
-        <v>9</v>
+        <v>15</v>
       </c>
     </row>
     <row r="65" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A65" s="4" t="s">
-        <v>527</v>
+        <v>522</v>
       </c>
       <c r="B65" s="4" t="s">
         <v>67</v>
       </c>
       <c r="C65" s="4" t="s">
-        <v>528</v>
+        <v>351</v>
       </c>
       <c r="D65" s="5"/>
       <c r="E65" s="4" t="s">
@@ -3171,13 +3169,13 @@
     </row>
     <row r="66" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A66" s="4" t="s">
-        <v>529</v>
+        <v>523</v>
       </c>
       <c r="B66" s="4" t="s">
         <v>67</v>
       </c>
       <c r="C66" s="4" t="s">
-        <v>532</v>
+        <v>524</v>
       </c>
       <c r="D66" s="5"/>
       <c r="E66" s="4" t="s">
@@ -3189,19 +3187,37 @@
     </row>
     <row r="67" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A67" s="4" t="s">
-        <v>531</v>
+        <v>525</v>
       </c>
       <c r="B67" s="4" t="s">
         <v>67</v>
       </c>
       <c r="C67" s="4" t="s">
-        <v>530</v>
+        <v>528</v>
       </c>
       <c r="D67" s="5"/>
       <c r="E67" s="4" t="s">
         <v>8</v>
       </c>
       <c r="F67" s="2" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="68" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A68" s="4" t="s">
+        <v>527</v>
+      </c>
+      <c r="B68" s="4" t="s">
+        <v>67</v>
+      </c>
+      <c r="C68" s="4" t="s">
+        <v>526</v>
+      </c>
+      <c r="D68" s="5"/>
+      <c r="E68" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="F68" s="2" t="s">
         <v>9</v>
       </c>
     </row>
@@ -3215,8 +3231,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AMK122"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A107" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="F122" sqref="F122"/>
+    <sheetView topLeftCell="A11" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="C29" sqref="C29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3262,10 +3278,10 @@
         <v>24</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>143</v>
+        <v>139</v>
       </c>
       <c r="E2" s="2" t="s">
-        <v>144</v>
+        <v>140</v>
       </c>
       <c r="F2" s="2" t="s">
         <v>15</v>
@@ -3276,13 +3292,13 @@
         <v>1</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>145</v>
+        <v>141</v>
       </c>
       <c r="C3" s="2" t="s">
-        <v>146</v>
+        <v>142</v>
       </c>
       <c r="E3" s="2" t="s">
-        <v>144</v>
+        <v>140</v>
       </c>
       <c r="F3" s="2" t="s">
         <v>15</v>
@@ -3293,13 +3309,13 @@
         <v>2</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>147</v>
+        <v>143</v>
       </c>
       <c r="C4" s="2" t="s">
         <v>65</v>
       </c>
       <c r="E4" s="2" t="s">
-        <v>144</v>
+        <v>140</v>
       </c>
       <c r="F4" s="2" t="s">
         <v>15</v>
@@ -3310,13 +3326,13 @@
         <v>3</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>148</v>
+        <v>144</v>
       </c>
       <c r="C5" s="2" t="s">
-        <v>149</v>
+        <v>145</v>
       </c>
       <c r="E5" s="2" t="s">
-        <v>144</v>
+        <v>140</v>
       </c>
       <c r="F5" s="2" t="s">
         <v>15</v>
@@ -3327,13 +3343,13 @@
         <v>4</v>
       </c>
       <c r="B6" s="2" t="s">
-        <v>121</v>
+        <v>117</v>
       </c>
       <c r="C6" s="2" t="s">
-        <v>150</v>
+        <v>146</v>
       </c>
       <c r="E6" s="2" t="s">
-        <v>144</v>
+        <v>140</v>
       </c>
       <c r="F6" s="2" t="s">
         <v>15</v>
@@ -3344,13 +3360,13 @@
         <v>5</v>
       </c>
       <c r="B7" s="2" t="s">
-        <v>125</v>
+        <v>121</v>
       </c>
       <c r="C7" s="2" t="s">
-        <v>151</v>
+        <v>147</v>
       </c>
       <c r="E7" s="2" t="s">
-        <v>144</v>
+        <v>140</v>
       </c>
       <c r="F7" s="2" t="s">
         <v>15</v>
@@ -3361,13 +3377,13 @@
         <v>6</v>
       </c>
       <c r="B8" s="2" t="s">
-        <v>152</v>
+        <v>148</v>
       </c>
       <c r="C8" s="2" t="s">
-        <v>153</v>
+        <v>149</v>
       </c>
       <c r="E8" s="2" t="s">
-        <v>144</v>
+        <v>140</v>
       </c>
       <c r="F8" s="2" t="s">
         <v>15</v>
@@ -3378,13 +3394,13 @@
         <v>7</v>
       </c>
       <c r="B9" s="2" t="s">
-        <v>154</v>
+        <v>150</v>
       </c>
       <c r="C9" s="2" t="s">
-        <v>155</v>
+        <v>151</v>
       </c>
       <c r="E9" s="2" t="s">
-        <v>144</v>
+        <v>140</v>
       </c>
       <c r="F9" s="2" t="s">
         <v>15</v>
@@ -3401,7 +3417,7 @@
         <v>35</v>
       </c>
       <c r="E10" s="2" t="s">
-        <v>144</v>
+        <v>140</v>
       </c>
       <c r="F10" s="2" t="s">
         <v>15</v>
@@ -3412,13 +3428,13 @@
         <v>9</v>
       </c>
       <c r="B11" s="2" t="s">
-        <v>156</v>
+        <v>152</v>
       </c>
       <c r="C11" s="2" t="s">
-        <v>157</v>
+        <v>153</v>
       </c>
       <c r="E11" s="2" t="s">
-        <v>144</v>
+        <v>140</v>
       </c>
       <c r="F11" s="2" t="s">
         <v>15</v>
@@ -3429,13 +3445,13 @@
         <v>10</v>
       </c>
       <c r="B12" s="2" t="s">
-        <v>158</v>
+        <v>154</v>
       </c>
       <c r="C12" s="2" t="s">
-        <v>159</v>
+        <v>155</v>
       </c>
       <c r="E12" s="2" t="s">
-        <v>144</v>
+        <v>140</v>
       </c>
       <c r="F12" s="2" t="s">
         <v>15</v>
@@ -3449,10 +3465,10 @@
         <v>42</v>
       </c>
       <c r="C13" s="2" t="s">
-        <v>160</v>
+        <v>156</v>
       </c>
       <c r="E13" s="2" t="s">
-        <v>144</v>
+        <v>140</v>
       </c>
       <c r="F13" s="2" t="s">
         <v>15</v>
@@ -3463,13 +3479,13 @@
         <v>12</v>
       </c>
       <c r="B14" s="2" t="s">
-        <v>161</v>
+        <v>157</v>
       </c>
       <c r="C14" s="2" t="s">
-        <v>162</v>
+        <v>158</v>
       </c>
       <c r="E14" s="2" t="s">
-        <v>144</v>
+        <v>140</v>
       </c>
       <c r="F14" s="2" t="s">
         <v>15</v>
@@ -3480,13 +3496,13 @@
         <v>13</v>
       </c>
       <c r="B15" s="2" t="s">
-        <v>163</v>
+        <v>159</v>
       </c>
       <c r="C15" s="2" t="s">
-        <v>164</v>
+        <v>160</v>
       </c>
       <c r="E15" s="2" t="s">
-        <v>144</v>
+        <v>140</v>
       </c>
       <c r="F15" s="2" t="s">
         <v>15</v>
@@ -3500,10 +3516,10 @@
         <v>38</v>
       </c>
       <c r="C16" s="2" t="s">
-        <v>165</v>
+        <v>161</v>
       </c>
       <c r="E16" s="2" t="s">
-        <v>144</v>
+        <v>140</v>
       </c>
       <c r="F16" s="2" t="s">
         <v>15</v>
@@ -3517,10 +3533,10 @@
         <v>40</v>
       </c>
       <c r="C17" s="2" t="s">
-        <v>166</v>
+        <v>162</v>
       </c>
       <c r="E17" s="2" t="s">
-        <v>144</v>
+        <v>140</v>
       </c>
       <c r="F17" s="2" t="s">
         <v>15</v>
@@ -3531,13 +3547,13 @@
         <v>16</v>
       </c>
       <c r="B18" s="2" t="s">
-        <v>167</v>
+        <v>163</v>
       </c>
       <c r="C18" s="2" t="s">
-        <v>168</v>
+        <v>164</v>
       </c>
       <c r="E18" s="2" t="s">
-        <v>144</v>
+        <v>140</v>
       </c>
       <c r="F18" s="2" t="s">
         <v>15</v>
@@ -3548,13 +3564,13 @@
         <v>17</v>
       </c>
       <c r="B19" s="2" t="s">
-        <v>169</v>
+        <v>165</v>
       </c>
       <c r="C19" s="2" t="s">
-        <v>170</v>
+        <v>166</v>
       </c>
       <c r="E19" s="2" t="s">
-        <v>144</v>
+        <v>140</v>
       </c>
       <c r="F19" s="2" t="s">
         <v>15</v>
@@ -3565,13 +3581,13 @@
         <v>18</v>
       </c>
       <c r="B20" s="2" t="s">
-        <v>171</v>
+        <v>167</v>
       </c>
       <c r="C20" s="2" t="s">
-        <v>172</v>
+        <v>168</v>
       </c>
       <c r="E20" s="2" t="s">
-        <v>144</v>
+        <v>140</v>
       </c>
       <c r="F20" s="2" t="s">
         <v>15</v>
@@ -3582,13 +3598,13 @@
         <v>19</v>
       </c>
       <c r="B21" s="2" t="s">
-        <v>173</v>
+        <v>169</v>
       </c>
       <c r="C21" s="2" t="s">
-        <v>174</v>
+        <v>170</v>
       </c>
       <c r="E21" s="2" t="s">
-        <v>144</v>
+        <v>140</v>
       </c>
       <c r="F21" s="2" t="s">
         <v>15</v>
@@ -3599,13 +3615,13 @@
         <v>20</v>
       </c>
       <c r="B22" s="2" t="s">
-        <v>175</v>
+        <v>171</v>
       </c>
       <c r="C22" s="2" t="s">
-        <v>176</v>
+        <v>172</v>
       </c>
       <c r="E22" s="2" t="s">
-        <v>144</v>
+        <v>140</v>
       </c>
       <c r="F22" s="2" t="s">
         <v>15</v>
@@ -3616,13 +3632,13 @@
         <v>21</v>
       </c>
       <c r="B23" s="2" t="s">
-        <v>177</v>
+        <v>173</v>
       </c>
       <c r="C23" s="2" t="s">
-        <v>178</v>
+        <v>174</v>
       </c>
       <c r="E23" s="2" t="s">
-        <v>144</v>
+        <v>140</v>
       </c>
       <c r="F23" s="2" t="s">
         <v>15</v>
@@ -3633,13 +3649,13 @@
         <v>22</v>
       </c>
       <c r="B24" s="2" t="s">
-        <v>179</v>
+        <v>175</v>
       </c>
       <c r="C24" s="2" t="s">
-        <v>180</v>
+        <v>176</v>
       </c>
       <c r="E24" s="2" t="s">
-        <v>144</v>
+        <v>140</v>
       </c>
       <c r="F24" s="2" t="s">
         <v>15</v>
@@ -3650,13 +3666,13 @@
         <v>23</v>
       </c>
       <c r="B25" s="2" t="s">
-        <v>181</v>
+        <v>177</v>
       </c>
       <c r="C25" s="2" t="s">
-        <v>182</v>
+        <v>178</v>
       </c>
       <c r="E25" s="2" t="s">
-        <v>144</v>
+        <v>140</v>
       </c>
       <c r="F25" s="2" t="s">
         <v>15</v>
@@ -3667,13 +3683,13 @@
         <v>24</v>
       </c>
       <c r="B26" s="4" t="s">
-        <v>183</v>
+        <v>179</v>
       </c>
       <c r="C26" s="2" t="s">
-        <v>184</v>
+        <v>180</v>
       </c>
       <c r="E26" s="2" t="s">
-        <v>144</v>
+        <v>140</v>
       </c>
       <c r="F26" s="2" t="s">
         <v>15</v>
@@ -3684,13 +3700,13 @@
         <v>24</v>
       </c>
       <c r="B27" s="4" t="s">
-        <v>185</v>
+        <v>181</v>
       </c>
       <c r="C27" s="2" t="s">
-        <v>186</v>
+        <v>182</v>
       </c>
       <c r="E27" s="2" t="s">
-        <v>144</v>
+        <v>140</v>
       </c>
       <c r="F27" s="2" t="s">
         <v>15</v>
@@ -3701,13 +3717,13 @@
         <v>24</v>
       </c>
       <c r="B28" s="4" t="s">
-        <v>187</v>
+        <v>183</v>
       </c>
       <c r="C28" s="2" t="s">
-        <v>188</v>
+        <v>184</v>
       </c>
       <c r="E28" s="2" t="s">
-        <v>144</v>
+        <v>140</v>
       </c>
       <c r="F28" s="2" t="s">
         <v>15</v>
@@ -3718,13 +3734,13 @@
         <v>25</v>
       </c>
       <c r="B29" s="2" t="s">
-        <v>189</v>
+        <v>185</v>
       </c>
       <c r="C29" s="2" t="s">
-        <v>190</v>
+        <v>186</v>
       </c>
       <c r="E29" s="2" t="s">
-        <v>144</v>
+        <v>140</v>
       </c>
       <c r="F29" s="2" t="s">
         <v>15</v>
@@ -3735,13 +3751,13 @@
         <v>26</v>
       </c>
       <c r="B30" s="2" t="s">
-        <v>191</v>
+        <v>187</v>
       </c>
       <c r="C30" s="2" t="s">
-        <v>192</v>
+        <v>188</v>
       </c>
       <c r="E30" s="2" t="s">
-        <v>144</v>
+        <v>140</v>
       </c>
       <c r="F30" s="2" t="s">
         <v>15</v>
@@ -3752,13 +3768,13 @@
         <v>27</v>
       </c>
       <c r="B31" s="2" t="s">
-        <v>103</v>
+        <v>99</v>
       </c>
       <c r="C31" s="2" t="s">
-        <v>193</v>
+        <v>189</v>
       </c>
       <c r="E31" s="2" t="s">
-        <v>144</v>
+        <v>140</v>
       </c>
       <c r="F31" s="2" t="s">
         <v>15</v>
@@ -3769,13 +3785,13 @@
         <v>28</v>
       </c>
       <c r="B32" s="2" t="s">
-        <v>194</v>
+        <v>190</v>
       </c>
       <c r="C32" s="2" t="s">
-        <v>195</v>
+        <v>191</v>
       </c>
       <c r="E32" s="2" t="s">
-        <v>144</v>
+        <v>140</v>
       </c>
       <c r="F32" s="2" t="s">
         <v>15</v>
@@ -3786,13 +3802,13 @@
         <v>29</v>
       </c>
       <c r="B33" s="2" t="s">
-        <v>196</v>
+        <v>192</v>
       </c>
       <c r="C33" s="2" t="s">
-        <v>197</v>
+        <v>193</v>
       </c>
       <c r="E33" s="2" t="s">
-        <v>144</v>
+        <v>140</v>
       </c>
       <c r="F33" s="2" t="s">
         <v>15</v>
@@ -3803,13 +3819,13 @@
         <v>30</v>
       </c>
       <c r="B34" s="2" t="s">
-        <v>198</v>
+        <v>194</v>
       </c>
       <c r="C34" s="2" t="s">
-        <v>199</v>
+        <v>195</v>
       </c>
       <c r="E34" s="2" t="s">
-        <v>144</v>
+        <v>140</v>
       </c>
       <c r="F34" s="2" t="s">
         <v>15</v>
@@ -3820,13 +3836,13 @@
         <v>31</v>
       </c>
       <c r="B35" s="2" t="s">
-        <v>105</v>
+        <v>101</v>
       </c>
       <c r="C35" s="2" t="s">
-        <v>200</v>
+        <v>196</v>
       </c>
       <c r="E35" s="2" t="s">
-        <v>144</v>
+        <v>140</v>
       </c>
       <c r="F35" s="2" t="s">
         <v>15</v>
@@ -3837,13 +3853,13 @@
         <v>32</v>
       </c>
       <c r="B36" s="2" t="s">
-        <v>201</v>
+        <v>197</v>
       </c>
       <c r="C36" s="2" t="s">
-        <v>202</v>
+        <v>198</v>
       </c>
       <c r="E36" s="2" t="s">
-        <v>144</v>
+        <v>140</v>
       </c>
       <c r="F36" s="2" t="s">
         <v>15</v>
@@ -3854,13 +3870,13 @@
         <v>33</v>
       </c>
       <c r="B37" s="2" t="s">
-        <v>203</v>
+        <v>199</v>
       </c>
       <c r="C37" s="2" t="s">
-        <v>204</v>
+        <v>200</v>
       </c>
       <c r="E37" s="2" t="s">
-        <v>144</v>
+        <v>140</v>
       </c>
       <c r="F37" s="2" t="s">
         <v>15</v>
@@ -3871,13 +3887,13 @@
         <v>33</v>
       </c>
       <c r="B38" s="2" t="s">
-        <v>205</v>
+        <v>201</v>
       </c>
       <c r="C38" s="2" t="s">
-        <v>206</v>
+        <v>202</v>
       </c>
       <c r="E38" s="2" t="s">
-        <v>144</v>
+        <v>140</v>
       </c>
       <c r="F38" s="2" t="s">
         <v>15</v>
@@ -3888,13 +3904,13 @@
         <v>34</v>
       </c>
       <c r="B39" s="2" t="s">
-        <v>207</v>
+        <v>203</v>
       </c>
       <c r="C39" s="2" t="s">
-        <v>208</v>
+        <v>204</v>
       </c>
       <c r="E39" s="2" t="s">
-        <v>144</v>
+        <v>140</v>
       </c>
       <c r="F39" s="2" t="s">
         <v>15</v>
@@ -3905,13 +3921,13 @@
         <v>34</v>
       </c>
       <c r="B40" s="2" t="s">
-        <v>209</v>
+        <v>205</v>
       </c>
       <c r="C40" s="2" t="s">
-        <v>210</v>
+        <v>206</v>
       </c>
       <c r="E40" s="2" t="s">
-        <v>144</v>
+        <v>140</v>
       </c>
       <c r="F40" s="2" t="s">
         <v>15</v>
@@ -3922,13 +3938,13 @@
         <v>35</v>
       </c>
       <c r="B41" s="2" t="s">
-        <v>211</v>
+        <v>207</v>
       </c>
       <c r="C41" s="2" t="s">
-        <v>212</v>
+        <v>208</v>
       </c>
       <c r="E41" s="2" t="s">
-        <v>144</v>
+        <v>140</v>
       </c>
       <c r="F41" s="2" t="s">
         <v>15</v>
@@ -3939,13 +3955,13 @@
         <v>36</v>
       </c>
       <c r="B42" s="2" t="s">
-        <v>213</v>
+        <v>209</v>
       </c>
       <c r="C42" s="2" t="s">
-        <v>214</v>
+        <v>210</v>
       </c>
       <c r="E42" s="2" t="s">
-        <v>144</v>
+        <v>140</v>
       </c>
       <c r="F42" s="2" t="s">
         <v>15</v>
@@ -3956,13 +3972,13 @@
         <v>37</v>
       </c>
       <c r="B43" s="2" t="s">
-        <v>215</v>
+        <v>211</v>
       </c>
       <c r="C43" s="2" t="s">
-        <v>216</v>
+        <v>212</v>
       </c>
       <c r="E43" s="2" t="s">
-        <v>144</v>
+        <v>140</v>
       </c>
       <c r="F43" s="2" t="s">
         <v>15</v>
@@ -3973,13 +3989,13 @@
         <v>38</v>
       </c>
       <c r="B44" s="2" t="s">
-        <v>217</v>
+        <v>213</v>
       </c>
       <c r="C44" s="2" t="s">
-        <v>218</v>
+        <v>214</v>
       </c>
       <c r="E44" s="2" t="s">
-        <v>144</v>
+        <v>140</v>
       </c>
       <c r="F44" s="2" t="s">
         <v>15</v>
@@ -3990,13 +4006,13 @@
         <v>39</v>
       </c>
       <c r="B45" s="2" t="s">
-        <v>219</v>
+        <v>215</v>
       </c>
       <c r="C45" s="2" t="s">
-        <v>220</v>
+        <v>216</v>
       </c>
       <c r="E45" s="2" t="s">
-        <v>144</v>
+        <v>140</v>
       </c>
       <c r="F45" s="2" t="s">
         <v>15</v>
@@ -4010,10 +4026,10 @@
         <v>26</v>
       </c>
       <c r="C46" s="2" t="s">
-        <v>221</v>
+        <v>217</v>
       </c>
       <c r="E46" s="2" t="s">
-        <v>144</v>
+        <v>140</v>
       </c>
       <c r="F46" s="2" t="s">
         <v>15</v>
@@ -4027,10 +4043,10 @@
         <v>28</v>
       </c>
       <c r="C47" s="2" t="s">
-        <v>222</v>
+        <v>218</v>
       </c>
       <c r="E47" s="2" t="s">
-        <v>144</v>
+        <v>140</v>
       </c>
       <c r="F47" s="2" t="s">
         <v>15</v>
@@ -4041,13 +4057,13 @@
         <v>42</v>
       </c>
       <c r="B48" s="2" t="s">
-        <v>223</v>
+        <v>219</v>
       </c>
       <c r="C48" s="2" t="s">
-        <v>195</v>
+        <v>191</v>
       </c>
       <c r="E48" s="2" t="s">
-        <v>144</v>
+        <v>140</v>
       </c>
       <c r="F48" s="2" t="s">
         <v>15</v>
@@ -4058,13 +4074,13 @@
         <v>43</v>
       </c>
       <c r="B49" s="2" t="s">
-        <v>224</v>
+        <v>220</v>
       </c>
       <c r="C49" s="2" t="s">
-        <v>225</v>
+        <v>221</v>
       </c>
       <c r="E49" s="2" t="s">
-        <v>144</v>
+        <v>140</v>
       </c>
       <c r="F49" s="2" t="s">
         <v>15</v>
@@ -4075,13 +4091,13 @@
         <v>44</v>
       </c>
       <c r="B50" s="2" t="s">
-        <v>226</v>
+        <v>222</v>
       </c>
       <c r="C50" s="2" t="s">
-        <v>227</v>
+        <v>223</v>
       </c>
       <c r="E50" s="2" t="s">
-        <v>144</v>
+        <v>140</v>
       </c>
       <c r="F50" s="2" t="s">
         <v>15</v>
@@ -4092,13 +4108,13 @@
         <v>45</v>
       </c>
       <c r="B51" s="2" t="s">
-        <v>228</v>
+        <v>224</v>
       </c>
       <c r="C51" s="2" t="s">
-        <v>229</v>
+        <v>225</v>
       </c>
       <c r="E51" s="2" t="s">
-        <v>144</v>
+        <v>140</v>
       </c>
       <c r="F51" s="2" t="s">
         <v>15</v>
@@ -4109,13 +4125,13 @@
         <v>46</v>
       </c>
       <c r="B52" s="2" t="s">
-        <v>230</v>
+        <v>226</v>
       </c>
       <c r="C52" s="2" t="s">
-        <v>231</v>
+        <v>227</v>
       </c>
       <c r="E52" s="2" t="s">
-        <v>144</v>
+        <v>140</v>
       </c>
       <c r="F52" s="2" t="s">
         <v>15</v>
@@ -4126,13 +4142,13 @@
         <v>47</v>
       </c>
       <c r="B53" s="2" t="s">
-        <v>232</v>
+        <v>228</v>
       </c>
       <c r="C53" s="2" t="s">
-        <v>233</v>
+        <v>229</v>
       </c>
       <c r="E53" s="2" t="s">
-        <v>144</v>
+        <v>140</v>
       </c>
       <c r="F53" s="2" t="s">
         <v>15</v>
@@ -4143,13 +4159,13 @@
         <v>48</v>
       </c>
       <c r="B54" s="2" t="s">
-        <v>234</v>
+        <v>230</v>
       </c>
       <c r="C54" s="2" t="s">
-        <v>235</v>
+        <v>231</v>
       </c>
       <c r="E54" s="2" t="s">
-        <v>144</v>
+        <v>140</v>
       </c>
       <c r="F54" s="2" t="s">
         <v>15</v>
@@ -4160,13 +4176,13 @@
         <v>49</v>
       </c>
       <c r="B55" s="2" t="s">
-        <v>236</v>
+        <v>232</v>
       </c>
       <c r="C55" s="2" t="s">
-        <v>237</v>
+        <v>233</v>
       </c>
       <c r="E55" s="2" t="s">
-        <v>144</v>
+        <v>140</v>
       </c>
       <c r="F55" s="2" t="s">
         <v>15</v>
@@ -4177,13 +4193,13 @@
         <v>50</v>
       </c>
       <c r="B56" s="2" t="s">
-        <v>238</v>
+        <v>234</v>
       </c>
       <c r="C56" s="2" t="s">
-        <v>239</v>
+        <v>235</v>
       </c>
       <c r="E56" s="2" t="s">
-        <v>144</v>
+        <v>140</v>
       </c>
       <c r="F56" s="2" t="s">
         <v>9</v>
@@ -4194,13 +4210,13 @@
         <v>51</v>
       </c>
       <c r="B57" s="2" t="s">
-        <v>240</v>
+        <v>236</v>
       </c>
       <c r="C57" s="2" t="s">
-        <v>241</v>
+        <v>237</v>
       </c>
       <c r="E57" s="2" t="s">
-        <v>144</v>
+        <v>140</v>
       </c>
       <c r="F57" s="2" t="s">
         <v>15</v>
@@ -4211,13 +4227,13 @@
         <v>52</v>
       </c>
       <c r="B58" s="2" t="s">
-        <v>242</v>
+        <v>238</v>
       </c>
       <c r="C58" s="2" t="s">
-        <v>243</v>
+        <v>239</v>
       </c>
       <c r="E58" s="2" t="s">
-        <v>144</v>
+        <v>140</v>
       </c>
       <c r="F58" s="2" t="s">
         <v>15</v>
@@ -4228,13 +4244,13 @@
         <v>52</v>
       </c>
       <c r="B59" s="2" t="s">
-        <v>244</v>
+        <v>240</v>
       </c>
       <c r="C59" s="2" t="s">
-        <v>245</v>
+        <v>241</v>
       </c>
       <c r="E59" s="2" t="s">
-        <v>144</v>
+        <v>140</v>
       </c>
       <c r="F59" s="2" t="s">
         <v>15</v>
@@ -4245,13 +4261,13 @@
         <v>67</v>
       </c>
       <c r="B60" s="2" t="s">
-        <v>246</v>
+        <v>242</v>
       </c>
       <c r="C60" s="2" t="s">
-        <v>247</v>
+        <v>243</v>
       </c>
       <c r="E60" s="2" t="s">
-        <v>144</v>
+        <v>140</v>
       </c>
       <c r="F60" s="2" t="s">
         <v>15</v>
@@ -4262,13 +4278,13 @@
         <v>67</v>
       </c>
       <c r="B61" s="2" t="s">
-        <v>248</v>
+        <v>244</v>
       </c>
       <c r="C61" s="2" t="s">
-        <v>249</v>
+        <v>245</v>
       </c>
       <c r="E61" s="2" t="s">
-        <v>144</v>
+        <v>140</v>
       </c>
       <c r="F61" s="2" t="s">
         <v>15</v>
@@ -4279,13 +4295,13 @@
         <v>67</v>
       </c>
       <c r="B62" s="2" t="s">
-        <v>250</v>
+        <v>246</v>
       </c>
       <c r="C62" s="2" t="s">
-        <v>251</v>
+        <v>247</v>
       </c>
       <c r="E62" s="2" t="s">
-        <v>144</v>
+        <v>140</v>
       </c>
       <c r="F62" s="2" t="s">
         <v>15</v>
@@ -4296,13 +4312,13 @@
         <v>67</v>
       </c>
       <c r="B63" s="2" t="s">
-        <v>252</v>
+        <v>248</v>
       </c>
       <c r="C63" s="2" t="s">
-        <v>253</v>
+        <v>249</v>
       </c>
       <c r="E63" s="2" t="s">
-        <v>144</v>
+        <v>140</v>
       </c>
       <c r="F63" s="2" t="s">
         <v>15</v>
@@ -4316,10 +4332,10 @@
         <v>67</v>
       </c>
       <c r="C64" s="5" t="s">
-        <v>254</v>
+        <v>250</v>
       </c>
       <c r="E64" s="5" t="s">
-        <v>144</v>
+        <v>140</v>
       </c>
       <c r="F64" s="5" t="s">
         <v>15</v>
@@ -4330,13 +4346,13 @@
         <v>57</v>
       </c>
       <c r="B65" s="2" t="s">
-        <v>255</v>
+        <v>251</v>
       </c>
       <c r="C65" s="2" t="s">
-        <v>256</v>
+        <v>252</v>
       </c>
       <c r="E65" s="2" t="s">
-        <v>144</v>
+        <v>140</v>
       </c>
       <c r="F65" s="2" t="s">
         <v>15</v>
@@ -4347,13 +4363,13 @@
         <v>57</v>
       </c>
       <c r="B66" s="2" t="s">
-        <v>257</v>
+        <v>253</v>
       </c>
       <c r="C66" s="2" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="E66" s="2" t="s">
-        <v>144</v>
+        <v>140</v>
       </c>
       <c r="F66" s="2" t="s">
         <v>15</v>
@@ -4364,13 +4380,13 @@
         <v>57</v>
       </c>
       <c r="B67" s="2" t="s">
-        <v>258</v>
+        <v>254</v>
       </c>
       <c r="C67" s="2" t="s">
-        <v>259</v>
+        <v>255</v>
       </c>
       <c r="E67" s="2" t="s">
-        <v>144</v>
+        <v>140</v>
       </c>
       <c r="F67" s="2" t="s">
         <v>15</v>
@@ -4381,13 +4397,13 @@
         <v>57</v>
       </c>
       <c r="B68" s="2" t="s">
-        <v>260</v>
+        <v>256</v>
       </c>
       <c r="C68" s="2" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="E68" s="2" t="s">
-        <v>144</v>
+        <v>140</v>
       </c>
       <c r="F68" s="2" t="s">
         <v>15</v>
@@ -4398,13 +4414,13 @@
         <v>57</v>
       </c>
       <c r="B69" s="2" t="s">
-        <v>261</v>
+        <v>257</v>
       </c>
       <c r="C69" s="2" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="E69" s="2" t="s">
-        <v>144</v>
+        <v>140</v>
       </c>
       <c r="F69" s="2" t="s">
         <v>15</v>
@@ -4415,13 +4431,13 @@
         <v>58</v>
       </c>
       <c r="B70" s="2" t="s">
-        <v>262</v>
+        <v>258</v>
       </c>
       <c r="C70" s="2" t="s">
-        <v>263</v>
+        <v>259</v>
       </c>
       <c r="E70" s="2" t="s">
-        <v>144</v>
+        <v>140</v>
       </c>
       <c r="F70" s="2" t="s">
         <v>15</v>
@@ -4432,16 +4448,16 @@
         <v>59</v>
       </c>
       <c r="B71" s="2" t="s">
-        <v>264</v>
+        <v>260</v>
       </c>
       <c r="C71" s="2" t="s">
-        <v>265</v>
+        <v>261</v>
       </c>
       <c r="D71" s="2" t="s">
         <v>14</v>
       </c>
       <c r="E71" s="2" t="s">
-        <v>144</v>
+        <v>140</v>
       </c>
       <c r="F71" s="2" t="s">
         <v>15</v>
@@ -4452,16 +4468,16 @@
         <v>60</v>
       </c>
       <c r="B72" s="2" t="s">
-        <v>266</v>
+        <v>262</v>
       </c>
       <c r="C72" s="2" t="s">
-        <v>267</v>
+        <v>263</v>
       </c>
       <c r="D72" s="2" t="s">
         <v>14</v>
       </c>
       <c r="E72" s="2" t="s">
-        <v>144</v>
+        <v>140</v>
       </c>
       <c r="F72" s="2" t="s">
         <v>15</v>
@@ -4472,16 +4488,16 @@
         <v>61</v>
       </c>
       <c r="B73" s="2" t="s">
-        <v>268</v>
+        <v>264</v>
       </c>
       <c r="C73" s="2" t="s">
-        <v>269</v>
+        <v>265</v>
       </c>
       <c r="D73" s="2" t="s">
         <v>14</v>
       </c>
       <c r="E73" s="2" t="s">
-        <v>144</v>
+        <v>140</v>
       </c>
       <c r="F73" s="2" t="s">
         <v>15</v>
@@ -4492,16 +4508,16 @@
         <v>62</v>
       </c>
       <c r="B74" s="2" t="s">
-        <v>270</v>
+        <v>266</v>
       </c>
       <c r="C74" s="2" t="s">
-        <v>271</v>
+        <v>267</v>
       </c>
       <c r="D74" s="2" t="s">
         <v>14</v>
       </c>
       <c r="E74" s="2" t="s">
-        <v>144</v>
+        <v>140</v>
       </c>
       <c r="F74" s="2" t="s">
         <v>15</v>
@@ -4512,13 +4528,13 @@
         <v>63</v>
       </c>
       <c r="B75" s="2" t="s">
-        <v>272</v>
+        <v>268</v>
       </c>
       <c r="C75" s="2" t="s">
-        <v>273</v>
+        <v>269</v>
       </c>
       <c r="E75" s="2" t="s">
-        <v>144</v>
+        <v>140</v>
       </c>
       <c r="F75" s="2" t="s">
         <v>15</v>
@@ -4532,10 +4548,10 @@
         <v>18</v>
       </c>
       <c r="C76" s="2" t="s">
-        <v>274</v>
+        <v>270</v>
       </c>
       <c r="E76" s="2" t="s">
-        <v>144</v>
+        <v>140</v>
       </c>
       <c r="F76" s="2" t="s">
         <v>15</v>
@@ -4546,13 +4562,13 @@
         <v>65</v>
       </c>
       <c r="B77" s="2" t="s">
-        <v>275</v>
+        <v>271</v>
       </c>
       <c r="C77" s="2" t="s">
-        <v>276</v>
+        <v>272</v>
       </c>
       <c r="E77" s="2" t="s">
-        <v>144</v>
+        <v>140</v>
       </c>
       <c r="F77" s="2" t="s">
         <v>15</v>
@@ -4563,13 +4579,13 @@
         <v>66</v>
       </c>
       <c r="B78" s="2" t="s">
-        <v>277</v>
+        <v>273</v>
       </c>
       <c r="C78" s="2" t="s">
-        <v>278</v>
+        <v>274</v>
       </c>
       <c r="E78" s="2" t="s">
-        <v>144</v>
+        <v>140</v>
       </c>
       <c r="F78" s="2" t="s">
         <v>15</v>
@@ -4580,13 +4596,13 @@
         <v>67</v>
       </c>
       <c r="B79" s="2" t="s">
-        <v>279</v>
+        <v>275</v>
       </c>
       <c r="C79" s="2" t="s">
-        <v>280</v>
+        <v>276</v>
       </c>
       <c r="E79" s="2" t="s">
-        <v>144</v>
+        <v>140</v>
       </c>
       <c r="F79" s="2" t="s">
         <v>15</v>
@@ -4597,13 +4613,13 @@
         <v>68</v>
       </c>
       <c r="B80" s="2" t="s">
-        <v>281</v>
+        <v>277</v>
       </c>
       <c r="C80" s="2" t="s">
-        <v>282</v>
+        <v>278</v>
       </c>
       <c r="E80" s="2" t="s">
-        <v>144</v>
+        <v>140</v>
       </c>
       <c r="F80" s="2" t="s">
         <v>15</v>
@@ -4614,13 +4630,13 @@
         <v>69</v>
       </c>
       <c r="B81" s="2" t="s">
-        <v>283</v>
+        <v>279</v>
       </c>
       <c r="C81" s="2" t="s">
-        <v>284</v>
+        <v>280</v>
       </c>
       <c r="E81" s="2" t="s">
-        <v>144</v>
+        <v>140</v>
       </c>
       <c r="F81" s="2" t="s">
         <v>15</v>
@@ -4631,13 +4647,13 @@
         <v>70</v>
       </c>
       <c r="B82" s="2" t="s">
-        <v>285</v>
+        <v>281</v>
       </c>
       <c r="C82" s="2" t="s">
-        <v>286</v>
+        <v>282</v>
       </c>
       <c r="E82" s="2" t="s">
-        <v>144</v>
+        <v>140</v>
       </c>
       <c r="F82" s="2" t="s">
         <v>15</v>
@@ -4648,13 +4664,13 @@
         <v>67</v>
       </c>
       <c r="B83" s="2" t="s">
-        <v>287</v>
+        <v>283</v>
       </c>
       <c r="C83" s="2" t="s">
-        <v>288</v>
+        <v>284</v>
       </c>
       <c r="E83" s="2" t="s">
-        <v>144</v>
+        <v>140</v>
       </c>
       <c r="F83" s="2" t="s">
         <v>15</v>
@@ -4665,13 +4681,13 @@
         <v>67</v>
       </c>
       <c r="B84" s="2" t="s">
-        <v>289</v>
+        <v>285</v>
       </c>
       <c r="C84" s="2" t="s">
-        <v>290</v>
+        <v>286</v>
       </c>
       <c r="E84" s="2" t="s">
-        <v>144</v>
+        <v>140</v>
       </c>
       <c r="F84" s="2" t="s">
         <v>15</v>
@@ -4682,13 +4698,13 @@
         <v>71</v>
       </c>
       <c r="B85" s="2" t="s">
-        <v>291</v>
+        <v>287</v>
       </c>
       <c r="C85" s="2" t="s">
-        <v>292</v>
+        <v>288</v>
       </c>
       <c r="E85" s="2" t="s">
-        <v>144</v>
+        <v>140</v>
       </c>
       <c r="F85" s="2" t="s">
         <v>15</v>
@@ -4699,13 +4715,13 @@
         <v>72</v>
       </c>
       <c r="B86" s="2" t="s">
-        <v>293</v>
+        <v>289</v>
       </c>
       <c r="C86" s="2" t="s">
-        <v>294</v>
+        <v>290</v>
       </c>
       <c r="E86" s="2" t="s">
-        <v>144</v>
+        <v>140</v>
       </c>
       <c r="F86" s="2" t="s">
         <v>15</v>
@@ -4716,13 +4732,13 @@
         <v>73</v>
       </c>
       <c r="B87" s="2" t="s">
-        <v>295</v>
+        <v>291</v>
       </c>
       <c r="C87" s="2" t="s">
-        <v>296</v>
+        <v>292</v>
       </c>
       <c r="E87" s="2" t="s">
-        <v>144</v>
+        <v>140</v>
       </c>
       <c r="F87" s="2" t="s">
         <v>15</v>
@@ -4733,13 +4749,13 @@
         <v>73</v>
       </c>
       <c r="B88" s="2" t="s">
-        <v>297</v>
+        <v>293</v>
       </c>
       <c r="C88" s="2" t="s">
-        <v>298</v>
+        <v>294</v>
       </c>
       <c r="E88" s="2" t="s">
-        <v>144</v>
+        <v>140</v>
       </c>
       <c r="F88" s="2" t="s">
         <v>15</v>
@@ -4750,13 +4766,13 @@
         <v>74</v>
       </c>
       <c r="B89" s="2" t="s">
-        <v>299</v>
+        <v>295</v>
       </c>
       <c r="C89" s="2" t="s">
-        <v>300</v>
+        <v>296</v>
       </c>
       <c r="E89" s="2" t="s">
-        <v>144</v>
+        <v>140</v>
       </c>
       <c r="F89" s="2" t="s">
         <v>15</v>
@@ -4767,13 +4783,13 @@
         <v>75</v>
       </c>
       <c r="B90" s="2" t="s">
-        <v>301</v>
+        <v>297</v>
       </c>
       <c r="C90" s="2" t="s">
-        <v>302</v>
+        <v>298</v>
       </c>
       <c r="E90" s="2" t="s">
-        <v>144</v>
+        <v>140</v>
       </c>
       <c r="F90" s="2" t="s">
         <v>15</v>
@@ -4784,13 +4800,13 @@
         <v>76</v>
       </c>
       <c r="B91" s="2" t="s">
-        <v>303</v>
+        <v>299</v>
       </c>
       <c r="C91" s="2" t="s">
-        <v>304</v>
+        <v>300</v>
       </c>
       <c r="E91" s="2" t="s">
-        <v>144</v>
+        <v>140</v>
       </c>
       <c r="F91" s="2" t="s">
         <v>15</v>
@@ -4801,13 +4817,13 @@
         <v>77</v>
       </c>
       <c r="B92" s="2" t="s">
-        <v>305</v>
+        <v>301</v>
       </c>
       <c r="C92" s="2" t="s">
-        <v>306</v>
+        <v>302</v>
       </c>
       <c r="E92" s="2" t="s">
-        <v>144</v>
+        <v>140</v>
       </c>
       <c r="F92" s="2" t="s">
         <v>15</v>
@@ -4818,13 +4834,13 @@
         <v>78</v>
       </c>
       <c r="B93" s="2" t="s">
-        <v>307</v>
+        <v>303</v>
       </c>
       <c r="C93" s="2" t="s">
-        <v>308</v>
+        <v>304</v>
       </c>
       <c r="E93" s="2" t="s">
-        <v>144</v>
+        <v>140</v>
       </c>
       <c r="F93" s="2" t="s">
         <v>15</v>
@@ -4832,16 +4848,16 @@
     </row>
     <row r="94" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A94" s="6" t="s">
-        <v>309</v>
+        <v>305</v>
       </c>
       <c r="B94" s="2" t="s">
-        <v>310</v>
+        <v>306</v>
       </c>
       <c r="C94" s="2" t="s">
-        <v>311</v>
+        <v>307</v>
       </c>
       <c r="E94" s="2" t="s">
-        <v>144</v>
+        <v>140</v>
       </c>
       <c r="F94" s="2" t="s">
         <v>15</v>
@@ -4852,13 +4868,13 @@
         <v>79</v>
       </c>
       <c r="B95" s="2" t="s">
-        <v>312</v>
+        <v>308</v>
       </c>
       <c r="C95" s="2" t="s">
-        <v>313</v>
+        <v>309</v>
       </c>
       <c r="E95" s="2" t="s">
-        <v>144</v>
+        <v>140</v>
       </c>
       <c r="F95" s="2" t="s">
         <v>15</v>
@@ -4869,13 +4885,13 @@
         <v>80</v>
       </c>
       <c r="B96" s="2" t="s">
-        <v>314</v>
+        <v>310</v>
       </c>
       <c r="C96" s="2" t="s">
-        <v>315</v>
+        <v>311</v>
       </c>
       <c r="E96" s="2" t="s">
-        <v>144</v>
+        <v>140</v>
       </c>
       <c r="F96" s="2" t="s">
         <v>15</v>
@@ -4886,13 +4902,13 @@
         <v>81</v>
       </c>
       <c r="B97" s="2" t="s">
-        <v>316</v>
+        <v>312</v>
       </c>
       <c r="C97" s="2" t="s">
-        <v>317</v>
+        <v>313</v>
       </c>
       <c r="E97" s="2" t="s">
-        <v>144</v>
+        <v>140</v>
       </c>
       <c r="F97" s="2" t="s">
         <v>15</v>
@@ -4903,13 +4919,13 @@
         <v>82</v>
       </c>
       <c r="B98" s="2" t="s">
-        <v>318</v>
+        <v>314</v>
       </c>
       <c r="C98" s="2" t="s">
-        <v>319</v>
+        <v>315</v>
       </c>
       <c r="E98" s="2" t="s">
-        <v>144</v>
+        <v>140</v>
       </c>
       <c r="F98" s="2" t="s">
         <v>15</v>
@@ -4920,13 +4936,13 @@
         <v>82</v>
       </c>
       <c r="B99" s="2" t="s">
-        <v>320</v>
+        <v>316</v>
       </c>
       <c r="C99" s="2" t="s">
-        <v>321</v>
+        <v>317</v>
       </c>
       <c r="E99" s="2" t="s">
-        <v>144</v>
+        <v>140</v>
       </c>
       <c r="F99" s="2" t="s">
         <v>15</v>
@@ -4937,13 +4953,13 @@
         <v>82</v>
       </c>
       <c r="B100" s="2" t="s">
-        <v>322</v>
+        <v>318</v>
       </c>
       <c r="C100" s="2" t="s">
-        <v>323</v>
+        <v>319</v>
       </c>
       <c r="E100" s="2" t="s">
-        <v>144</v>
+        <v>140</v>
       </c>
       <c r="F100" s="2" t="s">
         <v>15</v>
@@ -4954,13 +4970,13 @@
         <v>82</v>
       </c>
       <c r="B101" s="2" t="s">
-        <v>324</v>
+        <v>320</v>
       </c>
       <c r="C101" s="2" t="s">
-        <v>325</v>
+        <v>321</v>
       </c>
       <c r="E101" s="2" t="s">
-        <v>144</v>
+        <v>140</v>
       </c>
       <c r="F101" s="2" t="s">
         <v>15</v>
@@ -4971,13 +4987,13 @@
         <v>82</v>
       </c>
       <c r="B102" s="2" t="s">
-        <v>326</v>
+        <v>322</v>
       </c>
       <c r="C102" s="2" t="s">
-        <v>327</v>
+        <v>323</v>
       </c>
       <c r="E102" s="2" t="s">
-        <v>144</v>
+        <v>140</v>
       </c>
       <c r="F102" s="2" t="s">
         <v>15</v>
@@ -4994,7 +5010,7 @@
         <v>49</v>
       </c>
       <c r="E103" s="2" t="s">
-        <v>144</v>
+        <v>140</v>
       </c>
       <c r="F103" s="2" t="s">
         <v>15</v>
@@ -5011,7 +5027,7 @@
         <v>47</v>
       </c>
       <c r="E104" s="2" t="s">
-        <v>144</v>
+        <v>140</v>
       </c>
       <c r="F104" s="2" t="s">
         <v>15</v>
@@ -5025,10 +5041,10 @@
         <v>52</v>
       </c>
       <c r="C105" s="2" t="s">
-        <v>328</v>
+        <v>324</v>
       </c>
       <c r="E105" s="2" t="s">
-        <v>144</v>
+        <v>140</v>
       </c>
       <c r="F105" s="2" t="s">
         <v>15</v>
@@ -5039,13 +5055,13 @@
         <v>86</v>
       </c>
       <c r="B106" s="2" t="s">
-        <v>329</v>
+        <v>325</v>
       </c>
       <c r="C106" s="2" t="s">
-        <v>330</v>
+        <v>326</v>
       </c>
       <c r="E106" s="2" t="s">
-        <v>144</v>
+        <v>140</v>
       </c>
       <c r="F106" s="2" t="s">
         <v>15</v>
@@ -5056,13 +5072,13 @@
         <v>87</v>
       </c>
       <c r="B107" s="2" t="s">
-        <v>331</v>
+        <v>327</v>
       </c>
       <c r="C107" s="2" t="s">
-        <v>306</v>
+        <v>302</v>
       </c>
       <c r="E107" s="2" t="s">
-        <v>144</v>
+        <v>140</v>
       </c>
       <c r="F107" s="2" t="s">
         <v>15</v>
@@ -5073,13 +5089,13 @@
         <v>87</v>
       </c>
       <c r="B108" s="2" t="s">
-        <v>332</v>
+        <v>328</v>
       </c>
       <c r="C108" s="2" t="s">
-        <v>333</v>
+        <v>329</v>
       </c>
       <c r="E108" s="2" t="s">
-        <v>144</v>
+        <v>140</v>
       </c>
       <c r="F108" s="2" t="s">
         <v>15</v>
@@ -5090,13 +5106,13 @@
         <v>87</v>
       </c>
       <c r="B109" s="2" t="s">
-        <v>334</v>
+        <v>330</v>
       </c>
       <c r="C109" s="2" t="s">
-        <v>335</v>
+        <v>331</v>
       </c>
       <c r="E109" s="2" t="s">
-        <v>144</v>
+        <v>140</v>
       </c>
       <c r="F109" s="2" t="s">
         <v>15</v>
@@ -5107,13 +5123,13 @@
         <v>87</v>
       </c>
       <c r="B110" s="2" t="s">
-        <v>336</v>
+        <v>332</v>
       </c>
       <c r="C110" s="2" t="s">
-        <v>337</v>
+        <v>333</v>
       </c>
       <c r="E110" s="2" t="s">
-        <v>144</v>
+        <v>140</v>
       </c>
       <c r="F110" s="2" t="s">
         <v>15</v>
@@ -5124,13 +5140,13 @@
         <v>87</v>
       </c>
       <c r="B111" s="2" t="s">
-        <v>338</v>
+        <v>334</v>
       </c>
       <c r="C111" s="2" t="s">
-        <v>339</v>
+        <v>335</v>
       </c>
       <c r="E111" s="2" t="s">
-        <v>144</v>
+        <v>140</v>
       </c>
       <c r="F111" s="2" t="s">
         <v>15</v>
@@ -5141,13 +5157,13 @@
         <v>87</v>
       </c>
       <c r="B112" s="2" t="s">
-        <v>340</v>
+        <v>336</v>
       </c>
       <c r="C112" s="2" t="s">
-        <v>341</v>
+        <v>337</v>
       </c>
       <c r="E112" s="2" t="s">
-        <v>144</v>
+        <v>140</v>
       </c>
       <c r="F112" s="2" t="s">
         <v>15</v>
@@ -5158,13 +5174,13 @@
         <v>88</v>
       </c>
       <c r="B113" s="2" t="s">
-        <v>342</v>
+        <v>338</v>
       </c>
       <c r="C113" s="2" t="s">
-        <v>343</v>
+        <v>339</v>
       </c>
       <c r="E113" s="2" t="s">
-        <v>144</v>
+        <v>140</v>
       </c>
       <c r="F113" s="2" t="s">
         <v>15</v>
@@ -5175,13 +5191,13 @@
         <v>89</v>
       </c>
       <c r="B114" s="2" t="s">
-        <v>344</v>
+        <v>340</v>
       </c>
       <c r="C114" s="2" t="s">
-        <v>345</v>
+        <v>341</v>
       </c>
       <c r="E114" s="2" t="s">
-        <v>144</v>
+        <v>140</v>
       </c>
       <c r="F114" s="2" t="s">
         <v>15</v>
@@ -5192,13 +5208,13 @@
         <v>90</v>
       </c>
       <c r="B115" s="2" t="s">
-        <v>346</v>
+        <v>342</v>
       </c>
       <c r="C115" s="2" t="s">
-        <v>347</v>
+        <v>343</v>
       </c>
       <c r="E115" s="2" t="s">
-        <v>144</v>
+        <v>140</v>
       </c>
       <c r="F115" s="2" t="s">
         <v>15</v>
@@ -5209,13 +5225,13 @@
         <v>91</v>
       </c>
       <c r="B116" s="2" t="s">
-        <v>348</v>
+        <v>344</v>
       </c>
       <c r="C116" s="2" t="s">
-        <v>349</v>
+        <v>345</v>
       </c>
       <c r="E116" s="2" t="s">
-        <v>144</v>
+        <v>140</v>
       </c>
       <c r="F116" s="2" t="s">
         <v>15</v>
@@ -5226,13 +5242,13 @@
         <v>92</v>
       </c>
       <c r="B117" s="2" t="s">
-        <v>350</v>
+        <v>346</v>
       </c>
       <c r="C117" s="2" t="s">
-        <v>351</v>
+        <v>347</v>
       </c>
       <c r="E117" s="2" t="s">
-        <v>144</v>
+        <v>140</v>
       </c>
       <c r="F117" s="2" t="s">
         <v>15</v>
@@ -5246,10 +5262,10 @@
         <v>67</v>
       </c>
       <c r="C118" s="5" t="s">
-        <v>352</v>
+        <v>348</v>
       </c>
       <c r="E118" s="2" t="s">
-        <v>144</v>
+        <v>140</v>
       </c>
       <c r="F118" s="2" t="s">
         <v>15</v>
@@ -5263,10 +5279,10 @@
         <v>67</v>
       </c>
       <c r="C119" s="5" t="s">
-        <v>353</v>
+        <v>349</v>
       </c>
       <c r="E119" s="2" t="s">
-        <v>144</v>
+        <v>140</v>
       </c>
       <c r="F119" s="2" t="s">
         <v>15</v>
@@ -5280,10 +5296,10 @@
         <v>67</v>
       </c>
       <c r="C120" s="4" t="s">
-        <v>354</v>
+        <v>350</v>
       </c>
       <c r="E120" s="2" t="s">
-        <v>144</v>
+        <v>140</v>
       </c>
       <c r="F120" s="2" t="s">
         <v>15</v>
@@ -5297,10 +5313,10 @@
         <v>67</v>
       </c>
       <c r="C121" s="4" t="s">
-        <v>355</v>
+        <v>351</v>
       </c>
       <c r="E121" s="2" t="s">
-        <v>144</v>
+        <v>140</v>
       </c>
       <c r="F121" s="2" t="s">
         <v>15</v>
@@ -5308,16 +5324,16 @@
     </row>
     <row r="122" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A122" s="3" t="s">
-        <v>527</v>
+        <v>523</v>
       </c>
       <c r="B122" s="4" t="s">
         <v>67</v>
       </c>
       <c r="C122" s="4" t="s">
-        <v>533</v>
+        <v>529</v>
       </c>
       <c r="E122" s="4" t="s">
-        <v>144</v>
+        <v>140</v>
       </c>
       <c r="F122" s="5" t="s">
         <v>15</v>
@@ -5345,862 +5361,862 @@
   <sheetData>
     <row r="1" spans="1:1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="7" t="s">
-        <v>356</v>
+        <v>352</v>
       </c>
     </row>
     <row r="2" spans="1:1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="7" t="s">
-        <v>357</v>
+        <v>353</v>
       </c>
     </row>
     <row r="3" spans="1:1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="7" t="s">
-        <v>358</v>
+        <v>354</v>
       </c>
     </row>
     <row r="4" spans="1:1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="7" t="s">
-        <v>359</v>
+        <v>355</v>
       </c>
     </row>
     <row r="5" spans="1:1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="7" t="s">
-        <v>360</v>
+        <v>356</v>
       </c>
     </row>
     <row r="6" spans="1:1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="7" t="s">
-        <v>361</v>
+        <v>357</v>
       </c>
     </row>
     <row r="7" spans="1:1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="7" t="s">
-        <v>362</v>
+        <v>358</v>
       </c>
     </row>
     <row r="8" spans="1:1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" s="7" t="s">
-        <v>363</v>
+        <v>359</v>
       </c>
     </row>
     <row r="9" spans="1:1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" s="7" t="s">
-        <v>364</v>
+        <v>360</v>
       </c>
     </row>
     <row r="10" spans="1:1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" s="7" t="s">
-        <v>365</v>
+        <v>361</v>
       </c>
     </row>
     <row r="11" spans="1:1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A11" s="7" t="s">
-        <v>366</v>
+        <v>362</v>
       </c>
     </row>
     <row r="12" spans="1:1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A12" s="7" t="s">
-        <v>367</v>
+        <v>363</v>
       </c>
     </row>
     <row r="13" spans="1:1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A13" s="7" t="s">
-        <v>368</v>
+        <v>364</v>
       </c>
     </row>
     <row r="14" spans="1:1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A14" s="7" t="s">
-        <v>369</v>
+        <v>365</v>
       </c>
     </row>
     <row r="15" spans="1:1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A15" s="7" t="s">
-        <v>370</v>
+        <v>366</v>
       </c>
     </row>
     <row r="16" spans="1:1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A16" s="7" t="s">
-        <v>371</v>
+        <v>367</v>
       </c>
     </row>
     <row r="17" spans="1:1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A17" s="7" t="s">
-        <v>372</v>
+        <v>368</v>
       </c>
     </row>
     <row r="18" spans="1:1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A18" s="7" t="s">
-        <v>373</v>
+        <v>369</v>
       </c>
     </row>
     <row r="19" spans="1:1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A19" s="7" t="s">
-        <v>374</v>
+        <v>370</v>
       </c>
     </row>
     <row r="20" spans="1:1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A20" s="7" t="s">
-        <v>375</v>
+        <v>371</v>
       </c>
     </row>
     <row r="21" spans="1:1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A21" s="7" t="s">
-        <v>376</v>
+        <v>372</v>
       </c>
     </row>
     <row r="22" spans="1:1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A22" s="7" t="s">
-        <v>377</v>
+        <v>373</v>
       </c>
     </row>
     <row r="23" spans="1:1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A23" s="7" t="s">
-        <v>378</v>
+        <v>374</v>
       </c>
     </row>
     <row r="24" spans="1:1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A24" s="7" t="s">
-        <v>379</v>
+        <v>375</v>
       </c>
     </row>
     <row r="25" spans="1:1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A25" s="7" t="s">
-        <v>380</v>
+        <v>376</v>
       </c>
     </row>
     <row r="26" spans="1:1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A26" s="7" t="s">
-        <v>381</v>
+        <v>377</v>
       </c>
     </row>
     <row r="27" spans="1:1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A27" s="7" t="s">
-        <v>382</v>
+        <v>378</v>
       </c>
     </row>
     <row r="28" spans="1:1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A28" s="7" t="s">
-        <v>383</v>
+        <v>379</v>
       </c>
     </row>
     <row r="29" spans="1:1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A29" s="7" t="s">
-        <v>384</v>
+        <v>380</v>
       </c>
     </row>
     <row r="30" spans="1:1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A30" s="7" t="s">
-        <v>385</v>
+        <v>381</v>
       </c>
     </row>
     <row r="31" spans="1:1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A31" s="7" t="s">
-        <v>386</v>
+        <v>382</v>
       </c>
     </row>
     <row r="32" spans="1:1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A32" s="7" t="s">
-        <v>387</v>
+        <v>383</v>
       </c>
     </row>
     <row r="33" spans="1:1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A33" s="7" t="s">
-        <v>388</v>
+        <v>384</v>
       </c>
     </row>
     <row r="34" spans="1:1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A34" s="7" t="s">
-        <v>389</v>
+        <v>385</v>
       </c>
     </row>
     <row r="35" spans="1:1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A35" s="7" t="s">
-        <v>390</v>
+        <v>386</v>
       </c>
     </row>
     <row r="36" spans="1:1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A36" s="7" t="s">
-        <v>391</v>
+        <v>387</v>
       </c>
     </row>
     <row r="37" spans="1:1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A37" s="7" t="s">
-        <v>392</v>
+        <v>388</v>
       </c>
     </row>
     <row r="38" spans="1:1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A38" s="7" t="s">
-        <v>393</v>
+        <v>389</v>
       </c>
     </row>
     <row r="39" spans="1:1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A39" s="7" t="s">
-        <v>394</v>
+        <v>390</v>
       </c>
     </row>
     <row r="40" spans="1:1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A40" s="7" t="s">
-        <v>395</v>
+        <v>391</v>
       </c>
     </row>
     <row r="41" spans="1:1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A41" s="7" t="s">
-        <v>396</v>
+        <v>392</v>
       </c>
     </row>
     <row r="42" spans="1:1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A42" s="7" t="s">
-        <v>397</v>
+        <v>393</v>
       </c>
     </row>
     <row r="43" spans="1:1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A43" s="7" t="s">
-        <v>398</v>
+        <v>394</v>
       </c>
     </row>
     <row r="44" spans="1:1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A44" s="7" t="s">
-        <v>399</v>
+        <v>395</v>
       </c>
     </row>
     <row r="45" spans="1:1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A45" s="7" t="s">
-        <v>400</v>
+        <v>396</v>
       </c>
     </row>
     <row r="46" spans="1:1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A46" s="7" t="s">
-        <v>401</v>
+        <v>397</v>
       </c>
     </row>
     <row r="47" spans="1:1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A47" s="7" t="s">
-        <v>402</v>
+        <v>398</v>
       </c>
     </row>
     <row r="48" spans="1:1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A48" s="7" t="s">
-        <v>403</v>
+        <v>399</v>
       </c>
     </row>
     <row r="49" spans="1:1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A49" s="7" t="s">
-        <v>404</v>
+        <v>400</v>
       </c>
     </row>
     <row r="50" spans="1:1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A50" s="7" t="s">
-        <v>405</v>
+        <v>401</v>
       </c>
     </row>
     <row r="51" spans="1:1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A51" s="7" t="s">
-        <v>406</v>
+        <v>402</v>
       </c>
     </row>
     <row r="52" spans="1:1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A52" s="7" t="s">
-        <v>407</v>
+        <v>403</v>
       </c>
     </row>
     <row r="53" spans="1:1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A53" s="7" t="s">
-        <v>408</v>
+        <v>404</v>
       </c>
     </row>
     <row r="54" spans="1:1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A54" s="7" t="s">
-        <v>409</v>
+        <v>405</v>
       </c>
     </row>
     <row r="55" spans="1:1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A55" s="7" t="s">
-        <v>410</v>
+        <v>406</v>
       </c>
     </row>
     <row r="56" spans="1:1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A56" s="7" t="s">
-        <v>411</v>
+        <v>407</v>
       </c>
     </row>
     <row r="57" spans="1:1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A57" s="7" t="s">
-        <v>412</v>
+        <v>408</v>
       </c>
     </row>
     <row r="58" spans="1:1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A58" s="7" t="s">
-        <v>413</v>
+        <v>409</v>
       </c>
     </row>
     <row r="60" spans="1:1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A60" s="7" t="s">
-        <v>414</v>
+        <v>410</v>
       </c>
     </row>
     <row r="61" spans="1:1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A61" s="7" t="s">
-        <v>415</v>
+        <v>411</v>
       </c>
     </row>
     <row r="62" spans="1:1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A62" s="7" t="s">
-        <v>416</v>
+        <v>412</v>
       </c>
     </row>
     <row r="63" spans="1:1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A63" s="7" t="s">
-        <v>417</v>
+        <v>413</v>
       </c>
     </row>
     <row r="64" spans="1:1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A64" s="7" t="s">
-        <v>418</v>
+        <v>414</v>
       </c>
     </row>
     <row r="65" spans="1:1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A65" s="7" t="s">
-        <v>419</v>
+        <v>415</v>
       </c>
     </row>
     <row r="66" spans="1:1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A66" s="7" t="s">
-        <v>420</v>
+        <v>416</v>
       </c>
     </row>
     <row r="67" spans="1:1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A67" s="7" t="s">
-        <v>421</v>
+        <v>417</v>
       </c>
     </row>
     <row r="68" spans="1:1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A68" s="7" t="s">
-        <v>422</v>
+        <v>418</v>
       </c>
     </row>
     <row r="69" spans="1:1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A69" s="7" t="s">
-        <v>423</v>
+        <v>419</v>
       </c>
     </row>
     <row r="70" spans="1:1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A70" s="7" t="s">
-        <v>424</v>
+        <v>420</v>
       </c>
     </row>
     <row r="71" spans="1:1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A71" s="7" t="s">
-        <v>425</v>
+        <v>421</v>
       </c>
     </row>
     <row r="72" spans="1:1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A72" s="7" t="s">
-        <v>426</v>
+        <v>422</v>
       </c>
     </row>
     <row r="73" spans="1:1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A73" s="7" t="s">
-        <v>427</v>
+        <v>423</v>
       </c>
     </row>
     <row r="74" spans="1:1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A74" s="7" t="s">
-        <v>428</v>
+        <v>424</v>
       </c>
     </row>
     <row r="75" spans="1:1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A75" s="7" t="s">
-        <v>429</v>
+        <v>425</v>
       </c>
     </row>
     <row r="76" spans="1:1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A76" s="7" t="s">
-        <v>430</v>
+        <v>426</v>
       </c>
     </row>
     <row r="77" spans="1:1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A77" s="7" t="s">
-        <v>431</v>
+        <v>427</v>
       </c>
     </row>
     <row r="78" spans="1:1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A78" s="7" t="s">
-        <v>432</v>
+        <v>428</v>
       </c>
     </row>
     <row r="79" spans="1:1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A79" s="7" t="s">
-        <v>433</v>
+        <v>429</v>
       </c>
     </row>
     <row r="80" spans="1:1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A80" s="7" t="s">
-        <v>434</v>
+        <v>430</v>
       </c>
     </row>
     <row r="81" spans="1:1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A81" s="7" t="s">
-        <v>435</v>
+        <v>431</v>
       </c>
     </row>
     <row r="82" spans="1:1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A82" s="7" t="s">
-        <v>436</v>
+        <v>432</v>
       </c>
     </row>
     <row r="83" spans="1:1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A83" s="7" t="s">
-        <v>437</v>
+        <v>433</v>
       </c>
     </row>
     <row r="84" spans="1:1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A84" s="7" t="s">
-        <v>438</v>
+        <v>434</v>
       </c>
     </row>
     <row r="85" spans="1:1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A85" s="7" t="s">
-        <v>439</v>
+        <v>435</v>
       </c>
     </row>
     <row r="86" spans="1:1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A86" s="7" t="s">
-        <v>440</v>
+        <v>436</v>
       </c>
     </row>
     <row r="87" spans="1:1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A87" s="7" t="s">
-        <v>441</v>
+        <v>437</v>
       </c>
     </row>
     <row r="88" spans="1:1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A88" s="7" t="s">
-        <v>442</v>
+        <v>438</v>
       </c>
     </row>
     <row r="89" spans="1:1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A89" s="7" t="s">
-        <v>443</v>
+        <v>439</v>
       </c>
     </row>
     <row r="90" spans="1:1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A90" s="7" t="s">
-        <v>444</v>
+        <v>440</v>
       </c>
     </row>
     <row r="91" spans="1:1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A91" s="7" t="s">
-        <v>445</v>
+        <v>441</v>
       </c>
     </row>
     <row r="92" spans="1:1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A92" s="7" t="s">
-        <v>446</v>
+        <v>442</v>
       </c>
     </row>
     <row r="93" spans="1:1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A93" s="7" t="s">
-        <v>447</v>
+        <v>443</v>
       </c>
     </row>
     <row r="94" spans="1:1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A94" s="7" t="s">
-        <v>448</v>
+        <v>444</v>
       </c>
     </row>
     <row r="95" spans="1:1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A95" s="7" t="s">
-        <v>449</v>
+        <v>445</v>
       </c>
     </row>
     <row r="96" spans="1:1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A96" s="7" t="s">
-        <v>450</v>
+        <v>446</v>
       </c>
     </row>
     <row r="97" spans="1:1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A97" s="7" t="s">
-        <v>451</v>
+        <v>447</v>
       </c>
     </row>
     <row r="98" spans="1:1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A98" s="7" t="s">
-        <v>452</v>
+        <v>448</v>
       </c>
     </row>
     <row r="99" spans="1:1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A99" s="7" t="s">
-        <v>453</v>
+        <v>449</v>
       </c>
     </row>
     <row r="100" spans="1:1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A100" s="7" t="s">
-        <v>454</v>
+        <v>450</v>
       </c>
     </row>
     <row r="101" spans="1:1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A101" s="7" t="s">
-        <v>455</v>
+        <v>451</v>
       </c>
     </row>
     <row r="102" spans="1:1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A102" s="7" t="s">
-        <v>456</v>
+        <v>452</v>
       </c>
     </row>
     <row r="103" spans="1:1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A103" s="7" t="s">
-        <v>457</v>
+        <v>453</v>
       </c>
     </row>
     <row r="104" spans="1:1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A104" s="7" t="s">
-        <v>458</v>
+        <v>454</v>
       </c>
     </row>
     <row r="105" spans="1:1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A105" s="7" t="s">
-        <v>459</v>
+        <v>455</v>
       </c>
     </row>
     <row r="106" spans="1:1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A106" s="7" t="s">
-        <v>460</v>
+        <v>456</v>
       </c>
     </row>
     <row r="107" spans="1:1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A107" s="7" t="s">
-        <v>461</v>
+        <v>457</v>
       </c>
     </row>
     <row r="108" spans="1:1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A108" s="7" t="s">
-        <v>462</v>
+        <v>458</v>
       </c>
     </row>
     <row r="109" spans="1:1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A109" s="7" t="s">
-        <v>463</v>
+        <v>459</v>
       </c>
     </row>
     <row r="110" spans="1:1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A110" s="7" t="s">
-        <v>464</v>
+        <v>460</v>
       </c>
     </row>
     <row r="111" spans="1:1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A111" s="7" t="s">
-        <v>465</v>
+        <v>461</v>
       </c>
     </row>
     <row r="112" spans="1:1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A112" s="7" t="s">
-        <v>466</v>
+        <v>462</v>
       </c>
     </row>
     <row r="113" spans="1:1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A113" s="7" t="s">
-        <v>467</v>
+        <v>463</v>
       </c>
     </row>
     <row r="114" spans="1:1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A114" s="7" t="s">
-        <v>468</v>
+        <v>464</v>
       </c>
     </row>
     <row r="115" spans="1:1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A115" s="7" t="s">
-        <v>469</v>
+        <v>465</v>
       </c>
     </row>
     <row r="116" spans="1:1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A116" s="7" t="s">
-        <v>470</v>
+        <v>466</v>
       </c>
     </row>
     <row r="117" spans="1:1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A117" s="7" t="s">
-        <v>471</v>
+        <v>467</v>
       </c>
     </row>
     <row r="118" spans="1:1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A118" s="7" t="s">
-        <v>472</v>
+        <v>468</v>
       </c>
     </row>
     <row r="119" spans="1:1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A119" s="7" t="s">
-        <v>473</v>
+        <v>469</v>
       </c>
     </row>
     <row r="120" spans="1:1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A120" s="7" t="s">
-        <v>474</v>
+        <v>470</v>
       </c>
     </row>
     <row r="121" spans="1:1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A121" s="7" t="s">
-        <v>475</v>
+        <v>471</v>
       </c>
     </row>
     <row r="122" spans="1:1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A122" s="7" t="s">
-        <v>476</v>
+        <v>472</v>
       </c>
     </row>
     <row r="123" spans="1:1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A123" s="7" t="s">
-        <v>477</v>
+        <v>473</v>
       </c>
     </row>
     <row r="124" spans="1:1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A124" s="7" t="s">
-        <v>478</v>
+        <v>474</v>
       </c>
     </row>
     <row r="125" spans="1:1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A125" s="7" t="s">
-        <v>479</v>
+        <v>475</v>
       </c>
     </row>
     <row r="126" spans="1:1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A126" s="7" t="s">
-        <v>480</v>
+        <v>476</v>
       </c>
     </row>
     <row r="127" spans="1:1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A127" s="7" t="s">
-        <v>481</v>
+        <v>477</v>
       </c>
     </row>
     <row r="128" spans="1:1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A128" s="7" t="s">
-        <v>482</v>
+        <v>478</v>
       </c>
     </row>
     <row r="129" spans="1:1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A129" s="7" t="s">
-        <v>483</v>
+        <v>479</v>
       </c>
     </row>
     <row r="130" spans="1:1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A130" s="7" t="s">
-        <v>484</v>
+        <v>480</v>
       </c>
     </row>
     <row r="131" spans="1:1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A131" s="7" t="s">
-        <v>485</v>
+        <v>481</v>
       </c>
     </row>
     <row r="132" spans="1:1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A132" s="7" t="s">
-        <v>486</v>
+        <v>482</v>
       </c>
     </row>
     <row r="133" spans="1:1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A133" s="7" t="s">
-        <v>487</v>
+        <v>483</v>
       </c>
     </row>
     <row r="134" spans="1:1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A134" s="7" t="s">
-        <v>488</v>
+        <v>484</v>
       </c>
     </row>
     <row r="135" spans="1:1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A135" s="7" t="s">
-        <v>489</v>
+        <v>485</v>
       </c>
     </row>
     <row r="136" spans="1:1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A136" s="7" t="s">
-        <v>490</v>
+        <v>486</v>
       </c>
     </row>
     <row r="137" spans="1:1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A137" s="7" t="s">
-        <v>491</v>
+        <v>487</v>
       </c>
     </row>
     <row r="138" spans="1:1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A138" s="7" t="s">
-        <v>492</v>
+        <v>488</v>
       </c>
     </row>
     <row r="139" spans="1:1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A139" s="7" t="s">
-        <v>493</v>
+        <v>489</v>
       </c>
     </row>
     <row r="140" spans="1:1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A140" s="7" t="s">
-        <v>494</v>
+        <v>490</v>
       </c>
     </row>
     <row r="141" spans="1:1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A141" s="7" t="s">
-        <v>495</v>
+        <v>491</v>
       </c>
     </row>
     <row r="142" spans="1:1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A142" s="7" t="s">
-        <v>496</v>
+        <v>492</v>
       </c>
     </row>
     <row r="143" spans="1:1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A143" s="7" t="s">
-        <v>497</v>
+        <v>493</v>
       </c>
     </row>
     <row r="144" spans="1:1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A144" s="7" t="s">
-        <v>498</v>
+        <v>494</v>
       </c>
     </row>
     <row r="145" spans="1:1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A145" s="7" t="s">
-        <v>499</v>
+        <v>495</v>
       </c>
     </row>
     <row r="146" spans="1:1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A146" s="7" t="s">
-        <v>500</v>
+        <v>496</v>
       </c>
     </row>
     <row r="147" spans="1:1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A147" s="7" t="s">
-        <v>501</v>
+        <v>497</v>
       </c>
     </row>
     <row r="148" spans="1:1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A148" s="7" t="s">
-        <v>502</v>
+        <v>498</v>
       </c>
     </row>
     <row r="149" spans="1:1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A149" s="7" t="s">
-        <v>503</v>
+        <v>499</v>
       </c>
     </row>
     <row r="150" spans="1:1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A150" s="7" t="s">
-        <v>504</v>
+        <v>500</v>
       </c>
     </row>
     <row r="151" spans="1:1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A151" s="7" t="s">
-        <v>505</v>
+        <v>501</v>
       </c>
     </row>
     <row r="152" spans="1:1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A152" s="7" t="s">
-        <v>506</v>
+        <v>502</v>
       </c>
     </row>
     <row r="153" spans="1:1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A153" s="7" t="s">
-        <v>507</v>
+        <v>503</v>
       </c>
     </row>
     <row r="154" spans="1:1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A154" s="7" t="s">
-        <v>508</v>
+        <v>504</v>
       </c>
     </row>
     <row r="155" spans="1:1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A155" s="7" t="s">
-        <v>509</v>
+        <v>505</v>
       </c>
     </row>
     <row r="156" spans="1:1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A156" s="7" t="s">
-        <v>510</v>
+        <v>506</v>
       </c>
     </row>
     <row r="157" spans="1:1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A157" s="7" t="s">
-        <v>511</v>
+        <v>507</v>
       </c>
     </row>
     <row r="158" spans="1:1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A158" s="7" t="s">
-        <v>512</v>
+        <v>508</v>
       </c>
     </row>
     <row r="159" spans="1:1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A159" s="7" t="s">
-        <v>513</v>
+        <v>509</v>
       </c>
     </row>
     <row r="160" spans="1:1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A160" s="7" t="s">
-        <v>514</v>
+        <v>510</v>
       </c>
     </row>
     <row r="161" spans="1:1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A161" s="7" t="s">
-        <v>515</v>
+        <v>511</v>
       </c>
     </row>
     <row r="162" spans="1:1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A162" s="7" t="s">
-        <v>516</v>
+        <v>512</v>
       </c>
     </row>
     <row r="163" spans="1:1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A163" s="7" t="s">
-        <v>517</v>
+        <v>513</v>
       </c>
     </row>
     <row r="164" spans="1:1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A164" s="7" t="s">
-        <v>375</v>
+        <v>371</v>
       </c>
     </row>
     <row r="165" spans="1:1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A165" s="7" t="s">
-        <v>374</v>
+        <v>370</v>
       </c>
     </row>
     <row r="166" spans="1:1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A166" s="7" t="s">
-        <v>518</v>
+        <v>514</v>
       </c>
     </row>
     <row r="167" spans="1:1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A167" s="7" t="s">
-        <v>519</v>
+        <v>515</v>
       </c>
     </row>
     <row r="168" spans="1:1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A168" s="7" t="s">
-        <v>520</v>
+        <v>516</v>
       </c>
     </row>
     <row r="169" spans="1:1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A169" s="7" t="s">
-        <v>521</v>
+        <v>517</v>
       </c>
     </row>
     <row r="170" spans="1:1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A170" s="7" t="s">
-        <v>522</v>
+        <v>518</v>
       </c>
     </row>
     <row r="171" spans="1:1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A171" s="7" t="s">
-        <v>523</v>
+        <v>519</v>
       </c>
     </row>
     <row r="172" spans="1:1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A172" s="7" t="s">
-        <v>524</v>
+        <v>520</v>
       </c>
     </row>
     <row r="173" spans="1:1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A173" s="7" t="s">
-        <v>525</v>
+        <v>521</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Updated Netty for easier server stopping. Updated MySQL/J Connector library. Removed stop command. Fixed server not stopping properly. Fixed NPC's not turning to the player when spoken to. Fixed possible issue with the logoutqueue. Cleanup.
</commit_message>
<xml_diff>
--- a/Miscellaneous/Packets.xlsx
+++ b/Miscellaneous/Packets.xlsx
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="967" uniqueCount="534">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="969" uniqueCount="532">
   <si>
     <t>Message ID</t>
   </si>
@@ -312,12 +312,6 @@
   </si>
   <si>
     <t>Random Weather</t>
-  </si>
-  <si>
-    <t>Ms</t>
-  </si>
-  <si>
-    <t>Stop Server</t>
   </si>
   <si>
     <t>bm</t>
@@ -1960,7 +1954,7 @@
   <dimension ref="A1:G68"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A26" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="F45" sqref="F45"/>
+      <selection activeCell="D43" sqref="D43"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2507,13 +2501,13 @@
     </row>
     <row r="30" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A30" s="2" t="s">
-        <v>532</v>
+        <v>530</v>
       </c>
       <c r="B30" s="2" t="s">
         <v>68</v>
       </c>
       <c r="C30" s="2" t="s">
-        <v>533</v>
+        <v>531</v>
       </c>
       <c r="D30" s="2"/>
       <c r="E30" s="2" t="s">
@@ -2746,16 +2740,18 @@
       </c>
     </row>
     <row r="43" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A43" s="2">
-        <v>33</v>
+      <c r="A43" s="2" t="s">
+        <v>67</v>
       </c>
       <c r="B43" s="2" t="s">
-        <v>97</v>
+        <v>67</v>
       </c>
       <c r="C43" s="2" t="s">
-        <v>98</v>
-      </c>
-      <c r="D43" s="2"/>
+        <v>67</v>
+      </c>
+      <c r="D43" s="2" t="s">
+        <v>67</v>
+      </c>
       <c r="E43" s="2" t="s">
         <v>8</v>
       </c>
@@ -2788,10 +2784,10 @@
         <v>35</v>
       </c>
       <c r="B45" s="2" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
       <c r="C45" s="2" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
       <c r="D45" s="2"/>
       <c r="E45" s="2" t="s">
@@ -2806,10 +2802,10 @@
         <v>36</v>
       </c>
       <c r="B46" s="2" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
       <c r="C46" s="2" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
       <c r="D46" s="2"/>
       <c r="E46" s="2" t="s">
@@ -2824,10 +2820,10 @@
         <v>37</v>
       </c>
       <c r="B47" s="2" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="C47" s="2" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
       <c r="D47" s="2"/>
       <c r="E47" s="2" t="s">
@@ -2842,10 +2838,10 @@
         <v>38</v>
       </c>
       <c r="B48" s="2" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
       <c r="C48" s="2" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
       <c r="D48" s="2"/>
       <c r="E48" s="2" t="s">
@@ -2860,10 +2856,10 @@
         <v>39</v>
       </c>
       <c r="B49" s="2" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
       <c r="C49" s="2" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
       <c r="D49" s="2"/>
       <c r="E49" s="2" t="s">
@@ -2878,10 +2874,10 @@
         <v>67</v>
       </c>
       <c r="B50" s="2" t="s">
-        <v>109</v>
+        <v>107</v>
       </c>
       <c r="C50" s="2" t="s">
-        <v>110</v>
+        <v>108</v>
       </c>
       <c r="D50" s="2" t="s">
         <v>69</v>
@@ -2898,10 +2894,10 @@
         <v>40</v>
       </c>
       <c r="B51" s="2" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
       <c r="C51" s="2" t="s">
-        <v>112</v>
+        <v>110</v>
       </c>
       <c r="D51" s="2"/>
       <c r="E51" s="2" t="s">
@@ -2916,10 +2912,10 @@
         <v>51</v>
       </c>
       <c r="B52" s="2" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
       <c r="C52" s="2" t="s">
-        <v>114</v>
+        <v>112</v>
       </c>
       <c r="D52" s="2"/>
       <c r="E52" s="2" t="s">
@@ -2934,10 +2930,10 @@
         <v>41</v>
       </c>
       <c r="B53" s="2" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
       <c r="C53" s="2" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
       <c r="D53" s="2"/>
       <c r="E53" s="2" t="s">
@@ -2952,10 +2948,10 @@
         <v>42</v>
       </c>
       <c r="B54" s="2" t="s">
-        <v>117</v>
+        <v>115</v>
       </c>
       <c r="C54" s="2" t="s">
-        <v>118</v>
+        <v>116</v>
       </c>
       <c r="D54" s="2"/>
       <c r="E54" s="2" t="s">
@@ -2970,10 +2966,10 @@
         <v>43</v>
       </c>
       <c r="B55" s="2" t="s">
-        <v>119</v>
+        <v>117</v>
       </c>
       <c r="C55" s="2" t="s">
-        <v>120</v>
+        <v>118</v>
       </c>
       <c r="D55" s="2"/>
       <c r="E55" s="2" t="s">
@@ -2988,10 +2984,10 @@
         <v>44</v>
       </c>
       <c r="B56" s="2" t="s">
-        <v>121</v>
+        <v>119</v>
       </c>
       <c r="C56" s="2" t="s">
-        <v>122</v>
+        <v>120</v>
       </c>
       <c r="D56" s="2"/>
       <c r="E56" s="2" t="s">
@@ -3006,10 +3002,10 @@
         <v>45</v>
       </c>
       <c r="B57" s="2" t="s">
-        <v>123</v>
+        <v>121</v>
       </c>
       <c r="C57" s="2" t="s">
-        <v>124</v>
+        <v>122</v>
       </c>
       <c r="D57" s="2"/>
       <c r="E57" s="2" t="s">
@@ -3024,13 +3020,13 @@
         <v>46</v>
       </c>
       <c r="B58" s="2" t="s">
+        <v>123</v>
+      </c>
+      <c r="C58" s="2" t="s">
+        <v>124</v>
+      </c>
+      <c r="D58" s="2" t="s">
         <v>125</v>
-      </c>
-      <c r="C58" s="2" t="s">
-        <v>126</v>
-      </c>
-      <c r="D58" s="2" t="s">
-        <v>127</v>
       </c>
       <c r="E58" s="2" t="s">
         <v>8</v>
@@ -3044,10 +3040,10 @@
         <v>46</v>
       </c>
       <c r="B59" s="2" t="s">
-        <v>128</v>
+        <v>126</v>
       </c>
       <c r="C59" s="2" t="s">
-        <v>129</v>
+        <v>127</v>
       </c>
       <c r="D59" s="2"/>
       <c r="E59" s="2" t="s">
@@ -3062,10 +3058,10 @@
         <v>46</v>
       </c>
       <c r="B60" s="2" t="s">
-        <v>130</v>
+        <v>128</v>
       </c>
       <c r="C60" s="2" t="s">
-        <v>131</v>
+        <v>129</v>
       </c>
       <c r="D60" s="2"/>
       <c r="E60" s="2" t="s">
@@ -3080,10 +3076,10 @@
         <v>47</v>
       </c>
       <c r="B61" s="2" t="s">
-        <v>132</v>
+        <v>130</v>
       </c>
       <c r="C61" s="2" t="s">
-        <v>133</v>
+        <v>131</v>
       </c>
       <c r="D61" s="2"/>
       <c r="E61" s="2" t="s">
@@ -3098,10 +3094,10 @@
         <v>48</v>
       </c>
       <c r="B62" s="2" t="s">
-        <v>134</v>
+        <v>132</v>
       </c>
       <c r="C62" s="2" t="s">
-        <v>135</v>
+        <v>133</v>
       </c>
       <c r="D62" s="2"/>
       <c r="E62" s="2" t="s">
@@ -3116,13 +3112,13 @@
         <v>67</v>
       </c>
       <c r="B63" s="2" t="s">
+        <v>134</v>
+      </c>
+      <c r="C63" s="2" t="s">
+        <v>135</v>
+      </c>
+      <c r="D63" s="2" t="s">
         <v>136</v>
-      </c>
-      <c r="C63" s="2" t="s">
-        <v>137</v>
-      </c>
-      <c r="D63" s="2" t="s">
-        <v>138</v>
       </c>
       <c r="E63" s="2" t="s">
         <v>8</v>
@@ -3133,13 +3129,13 @@
     </row>
     <row r="64" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A64" s="2" t="s">
-        <v>531</v>
+        <v>529</v>
       </c>
       <c r="B64" s="2" t="s">
         <v>67</v>
       </c>
       <c r="C64" s="2" t="s">
-        <v>530</v>
+        <v>528</v>
       </c>
       <c r="D64" s="2"/>
       <c r="E64" s="2" t="s">
@@ -3151,13 +3147,13 @@
     </row>
     <row r="65" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A65" s="4" t="s">
-        <v>522</v>
+        <v>520</v>
       </c>
       <c r="B65" s="4" t="s">
         <v>67</v>
       </c>
       <c r="C65" s="4" t="s">
-        <v>351</v>
+        <v>349</v>
       </c>
       <c r="D65" s="5"/>
       <c r="E65" s="4" t="s">
@@ -3169,13 +3165,13 @@
     </row>
     <row r="66" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A66" s="4" t="s">
-        <v>523</v>
+        <v>521</v>
       </c>
       <c r="B66" s="4" t="s">
         <v>67</v>
       </c>
       <c r="C66" s="4" t="s">
-        <v>524</v>
+        <v>522</v>
       </c>
       <c r="D66" s="5"/>
       <c r="E66" s="4" t="s">
@@ -3187,13 +3183,13 @@
     </row>
     <row r="67" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A67" s="4" t="s">
-        <v>525</v>
+        <v>523</v>
       </c>
       <c r="B67" s="4" t="s">
         <v>67</v>
       </c>
       <c r="C67" s="4" t="s">
-        <v>528</v>
+        <v>526</v>
       </c>
       <c r="D67" s="5"/>
       <c r="E67" s="4" t="s">
@@ -3205,13 +3201,13 @@
     </row>
     <row r="68" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A68" s="4" t="s">
-        <v>527</v>
+        <v>525</v>
       </c>
       <c r="B68" s="4" t="s">
         <v>67</v>
       </c>
       <c r="C68" s="4" t="s">
-        <v>526</v>
+        <v>524</v>
       </c>
       <c r="D68" s="5"/>
       <c r="E68" s="4" t="s">
@@ -3278,10 +3274,10 @@
         <v>24</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>139</v>
+        <v>137</v>
       </c>
       <c r="E2" s="2" t="s">
-        <v>140</v>
+        <v>138</v>
       </c>
       <c r="F2" s="2" t="s">
         <v>15</v>
@@ -3292,13 +3288,13 @@
         <v>1</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>141</v>
+        <v>139</v>
       </c>
       <c r="C3" s="2" t="s">
-        <v>142</v>
+        <v>140</v>
       </c>
       <c r="E3" s="2" t="s">
-        <v>140</v>
+        <v>138</v>
       </c>
       <c r="F3" s="2" t="s">
         <v>15</v>
@@ -3309,13 +3305,13 @@
         <v>2</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>143</v>
+        <v>141</v>
       </c>
       <c r="C4" s="2" t="s">
         <v>65</v>
       </c>
       <c r="E4" s="2" t="s">
-        <v>140</v>
+        <v>138</v>
       </c>
       <c r="F4" s="2" t="s">
         <v>15</v>
@@ -3326,13 +3322,13 @@
         <v>3</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>144</v>
+        <v>142</v>
       </c>
       <c r="C5" s="2" t="s">
-        <v>145</v>
+        <v>143</v>
       </c>
       <c r="E5" s="2" t="s">
-        <v>140</v>
+        <v>138</v>
       </c>
       <c r="F5" s="2" t="s">
         <v>15</v>
@@ -3343,13 +3339,13 @@
         <v>4</v>
       </c>
       <c r="B6" s="2" t="s">
-        <v>117</v>
+        <v>115</v>
       </c>
       <c r="C6" s="2" t="s">
-        <v>146</v>
+        <v>144</v>
       </c>
       <c r="E6" s="2" t="s">
-        <v>140</v>
+        <v>138</v>
       </c>
       <c r="F6" s="2" t="s">
         <v>15</v>
@@ -3360,13 +3356,13 @@
         <v>5</v>
       </c>
       <c r="B7" s="2" t="s">
-        <v>121</v>
+        <v>119</v>
       </c>
       <c r="C7" s="2" t="s">
-        <v>147</v>
+        <v>145</v>
       </c>
       <c r="E7" s="2" t="s">
-        <v>140</v>
+        <v>138</v>
       </c>
       <c r="F7" s="2" t="s">
         <v>15</v>
@@ -3377,13 +3373,13 @@
         <v>6</v>
       </c>
       <c r="B8" s="2" t="s">
-        <v>148</v>
+        <v>146</v>
       </c>
       <c r="C8" s="2" t="s">
-        <v>149</v>
+        <v>147</v>
       </c>
       <c r="E8" s="2" t="s">
-        <v>140</v>
+        <v>138</v>
       </c>
       <c r="F8" s="2" t="s">
         <v>15</v>
@@ -3394,13 +3390,13 @@
         <v>7</v>
       </c>
       <c r="B9" s="2" t="s">
-        <v>150</v>
+        <v>148</v>
       </c>
       <c r="C9" s="2" t="s">
-        <v>151</v>
+        <v>149</v>
       </c>
       <c r="E9" s="2" t="s">
-        <v>140</v>
+        <v>138</v>
       </c>
       <c r="F9" s="2" t="s">
         <v>15</v>
@@ -3417,7 +3413,7 @@
         <v>35</v>
       </c>
       <c r="E10" s="2" t="s">
-        <v>140</v>
+        <v>138</v>
       </c>
       <c r="F10" s="2" t="s">
         <v>15</v>
@@ -3428,13 +3424,13 @@
         <v>9</v>
       </c>
       <c r="B11" s="2" t="s">
-        <v>152</v>
+        <v>150</v>
       </c>
       <c r="C11" s="2" t="s">
-        <v>153</v>
+        <v>151</v>
       </c>
       <c r="E11" s="2" t="s">
-        <v>140</v>
+        <v>138</v>
       </c>
       <c r="F11" s="2" t="s">
         <v>15</v>
@@ -3445,13 +3441,13 @@
         <v>10</v>
       </c>
       <c r="B12" s="2" t="s">
-        <v>154</v>
+        <v>152</v>
       </c>
       <c r="C12" s="2" t="s">
-        <v>155</v>
+        <v>153</v>
       </c>
       <c r="E12" s="2" t="s">
-        <v>140</v>
+        <v>138</v>
       </c>
       <c r="F12" s="2" t="s">
         <v>15</v>
@@ -3465,10 +3461,10 @@
         <v>42</v>
       </c>
       <c r="C13" s="2" t="s">
-        <v>156</v>
+        <v>154</v>
       </c>
       <c r="E13" s="2" t="s">
-        <v>140</v>
+        <v>138</v>
       </c>
       <c r="F13" s="2" t="s">
         <v>15</v>
@@ -3479,13 +3475,13 @@
         <v>12</v>
       </c>
       <c r="B14" s="2" t="s">
-        <v>157</v>
+        <v>155</v>
       </c>
       <c r="C14" s="2" t="s">
-        <v>158</v>
+        <v>156</v>
       </c>
       <c r="E14" s="2" t="s">
-        <v>140</v>
+        <v>138</v>
       </c>
       <c r="F14" s="2" t="s">
         <v>15</v>
@@ -3496,13 +3492,13 @@
         <v>13</v>
       </c>
       <c r="B15" s="2" t="s">
-        <v>159</v>
+        <v>157</v>
       </c>
       <c r="C15" s="2" t="s">
-        <v>160</v>
+        <v>158</v>
       </c>
       <c r="E15" s="2" t="s">
-        <v>140</v>
+        <v>138</v>
       </c>
       <c r="F15" s="2" t="s">
         <v>15</v>
@@ -3516,10 +3512,10 @@
         <v>38</v>
       </c>
       <c r="C16" s="2" t="s">
-        <v>161</v>
+        <v>159</v>
       </c>
       <c r="E16" s="2" t="s">
-        <v>140</v>
+        <v>138</v>
       </c>
       <c r="F16" s="2" t="s">
         <v>15</v>
@@ -3533,10 +3529,10 @@
         <v>40</v>
       </c>
       <c r="C17" s="2" t="s">
-        <v>162</v>
+        <v>160</v>
       </c>
       <c r="E17" s="2" t="s">
-        <v>140</v>
+        <v>138</v>
       </c>
       <c r="F17" s="2" t="s">
         <v>15</v>
@@ -3547,13 +3543,13 @@
         <v>16</v>
       </c>
       <c r="B18" s="2" t="s">
-        <v>163</v>
+        <v>161</v>
       </c>
       <c r="C18" s="2" t="s">
-        <v>164</v>
+        <v>162</v>
       </c>
       <c r="E18" s="2" t="s">
-        <v>140</v>
+        <v>138</v>
       </c>
       <c r="F18" s="2" t="s">
         <v>15</v>
@@ -3564,13 +3560,13 @@
         <v>17</v>
       </c>
       <c r="B19" s="2" t="s">
-        <v>165</v>
+        <v>163</v>
       </c>
       <c r="C19" s="2" t="s">
-        <v>166</v>
+        <v>164</v>
       </c>
       <c r="E19" s="2" t="s">
-        <v>140</v>
+        <v>138</v>
       </c>
       <c r="F19" s="2" t="s">
         <v>15</v>
@@ -3581,13 +3577,13 @@
         <v>18</v>
       </c>
       <c r="B20" s="2" t="s">
-        <v>167</v>
+        <v>165</v>
       </c>
       <c r="C20" s="2" t="s">
-        <v>168</v>
+        <v>166</v>
       </c>
       <c r="E20" s="2" t="s">
-        <v>140</v>
+        <v>138</v>
       </c>
       <c r="F20" s="2" t="s">
         <v>15</v>
@@ -3598,13 +3594,13 @@
         <v>19</v>
       </c>
       <c r="B21" s="2" t="s">
-        <v>169</v>
+        <v>167</v>
       </c>
       <c r="C21" s="2" t="s">
-        <v>170</v>
+        <v>168</v>
       </c>
       <c r="E21" s="2" t="s">
-        <v>140</v>
+        <v>138</v>
       </c>
       <c r="F21" s="2" t="s">
         <v>15</v>
@@ -3615,13 +3611,13 @@
         <v>20</v>
       </c>
       <c r="B22" s="2" t="s">
-        <v>171</v>
+        <v>169</v>
       </c>
       <c r="C22" s="2" t="s">
-        <v>172</v>
+        <v>170</v>
       </c>
       <c r="E22" s="2" t="s">
-        <v>140</v>
+        <v>138</v>
       </c>
       <c r="F22" s="2" t="s">
         <v>15</v>
@@ -3632,13 +3628,13 @@
         <v>21</v>
       </c>
       <c r="B23" s="2" t="s">
-        <v>173</v>
+        <v>171</v>
       </c>
       <c r="C23" s="2" t="s">
-        <v>174</v>
+        <v>172</v>
       </c>
       <c r="E23" s="2" t="s">
-        <v>140</v>
+        <v>138</v>
       </c>
       <c r="F23" s="2" t="s">
         <v>15</v>
@@ -3649,13 +3645,13 @@
         <v>22</v>
       </c>
       <c r="B24" s="2" t="s">
-        <v>175</v>
+        <v>173</v>
       </c>
       <c r="C24" s="2" t="s">
-        <v>176</v>
+        <v>174</v>
       </c>
       <c r="E24" s="2" t="s">
-        <v>140</v>
+        <v>138</v>
       </c>
       <c r="F24" s="2" t="s">
         <v>15</v>
@@ -3666,13 +3662,13 @@
         <v>23</v>
       </c>
       <c r="B25" s="2" t="s">
-        <v>177</v>
+        <v>175</v>
       </c>
       <c r="C25" s="2" t="s">
-        <v>178</v>
+        <v>176</v>
       </c>
       <c r="E25" s="2" t="s">
-        <v>140</v>
+        <v>138</v>
       </c>
       <c r="F25" s="2" t="s">
         <v>15</v>
@@ -3683,13 +3679,13 @@
         <v>24</v>
       </c>
       <c r="B26" s="4" t="s">
-        <v>179</v>
+        <v>177</v>
       </c>
       <c r="C26" s="2" t="s">
-        <v>180</v>
+        <v>178</v>
       </c>
       <c r="E26" s="2" t="s">
-        <v>140</v>
+        <v>138</v>
       </c>
       <c r="F26" s="2" t="s">
         <v>15</v>
@@ -3700,13 +3696,13 @@
         <v>24</v>
       </c>
       <c r="B27" s="4" t="s">
-        <v>181</v>
+        <v>179</v>
       </c>
       <c r="C27" s="2" t="s">
-        <v>182</v>
+        <v>180</v>
       </c>
       <c r="E27" s="2" t="s">
-        <v>140</v>
+        <v>138</v>
       </c>
       <c r="F27" s="2" t="s">
         <v>15</v>
@@ -3717,13 +3713,13 @@
         <v>24</v>
       </c>
       <c r="B28" s="4" t="s">
-        <v>183</v>
+        <v>181</v>
       </c>
       <c r="C28" s="2" t="s">
-        <v>184</v>
+        <v>182</v>
       </c>
       <c r="E28" s="2" t="s">
-        <v>140</v>
+        <v>138</v>
       </c>
       <c r="F28" s="2" t="s">
         <v>15</v>
@@ -3734,13 +3730,13 @@
         <v>25</v>
       </c>
       <c r="B29" s="2" t="s">
-        <v>185</v>
+        <v>183</v>
       </c>
       <c r="C29" s="2" t="s">
-        <v>186</v>
+        <v>184</v>
       </c>
       <c r="E29" s="2" t="s">
-        <v>140</v>
+        <v>138</v>
       </c>
       <c r="F29" s="2" t="s">
         <v>15</v>
@@ -3751,13 +3747,13 @@
         <v>26</v>
       </c>
       <c r="B30" s="2" t="s">
-        <v>187</v>
+        <v>185</v>
       </c>
       <c r="C30" s="2" t="s">
-        <v>188</v>
+        <v>186</v>
       </c>
       <c r="E30" s="2" t="s">
-        <v>140</v>
+        <v>138</v>
       </c>
       <c r="F30" s="2" t="s">
         <v>15</v>
@@ -3768,13 +3764,13 @@
         <v>27</v>
       </c>
       <c r="B31" s="2" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
       <c r="C31" s="2" t="s">
-        <v>189</v>
+        <v>187</v>
       </c>
       <c r="E31" s="2" t="s">
-        <v>140</v>
+        <v>138</v>
       </c>
       <c r="F31" s="2" t="s">
         <v>15</v>
@@ -3785,13 +3781,13 @@
         <v>28</v>
       </c>
       <c r="B32" s="2" t="s">
-        <v>190</v>
+        <v>188</v>
       </c>
       <c r="C32" s="2" t="s">
-        <v>191</v>
+        <v>189</v>
       </c>
       <c r="E32" s="2" t="s">
-        <v>140</v>
+        <v>138</v>
       </c>
       <c r="F32" s="2" t="s">
         <v>15</v>
@@ -3802,13 +3798,13 @@
         <v>29</v>
       </c>
       <c r="B33" s="2" t="s">
-        <v>192</v>
+        <v>190</v>
       </c>
       <c r="C33" s="2" t="s">
-        <v>193</v>
+        <v>191</v>
       </c>
       <c r="E33" s="2" t="s">
-        <v>140</v>
+        <v>138</v>
       </c>
       <c r="F33" s="2" t="s">
         <v>15</v>
@@ -3819,13 +3815,13 @@
         <v>30</v>
       </c>
       <c r="B34" s="2" t="s">
-        <v>194</v>
+        <v>192</v>
       </c>
       <c r="C34" s="2" t="s">
-        <v>195</v>
+        <v>193</v>
       </c>
       <c r="E34" s="2" t="s">
-        <v>140</v>
+        <v>138</v>
       </c>
       <c r="F34" s="2" t="s">
         <v>15</v>
@@ -3836,13 +3832,13 @@
         <v>31</v>
       </c>
       <c r="B35" s="2" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
       <c r="C35" s="2" t="s">
-        <v>196</v>
+        <v>194</v>
       </c>
       <c r="E35" s="2" t="s">
-        <v>140</v>
+        <v>138</v>
       </c>
       <c r="F35" s="2" t="s">
         <v>15</v>
@@ -3853,13 +3849,13 @@
         <v>32</v>
       </c>
       <c r="B36" s="2" t="s">
-        <v>197</v>
+        <v>195</v>
       </c>
       <c r="C36" s="2" t="s">
-        <v>198</v>
+        <v>196</v>
       </c>
       <c r="E36" s="2" t="s">
-        <v>140</v>
+        <v>138</v>
       </c>
       <c r="F36" s="2" t="s">
         <v>15</v>
@@ -3870,13 +3866,13 @@
         <v>33</v>
       </c>
       <c r="B37" s="2" t="s">
-        <v>199</v>
+        <v>197</v>
       </c>
       <c r="C37" s="2" t="s">
-        <v>200</v>
+        <v>198</v>
       </c>
       <c r="E37" s="2" t="s">
-        <v>140</v>
+        <v>138</v>
       </c>
       <c r="F37" s="2" t="s">
         <v>15</v>
@@ -3887,13 +3883,13 @@
         <v>33</v>
       </c>
       <c r="B38" s="2" t="s">
-        <v>201</v>
+        <v>199</v>
       </c>
       <c r="C38" s="2" t="s">
-        <v>202</v>
+        <v>200</v>
       </c>
       <c r="E38" s="2" t="s">
-        <v>140</v>
+        <v>138</v>
       </c>
       <c r="F38" s="2" t="s">
         <v>15</v>
@@ -3904,13 +3900,13 @@
         <v>34</v>
       </c>
       <c r="B39" s="2" t="s">
-        <v>203</v>
+        <v>201</v>
       </c>
       <c r="C39" s="2" t="s">
-        <v>204</v>
+        <v>202</v>
       </c>
       <c r="E39" s="2" t="s">
-        <v>140</v>
+        <v>138</v>
       </c>
       <c r="F39" s="2" t="s">
         <v>15</v>
@@ -3921,13 +3917,13 @@
         <v>34</v>
       </c>
       <c r="B40" s="2" t="s">
-        <v>205</v>
+        <v>203</v>
       </c>
       <c r="C40" s="2" t="s">
-        <v>206</v>
+        <v>204</v>
       </c>
       <c r="E40" s="2" t="s">
-        <v>140</v>
+        <v>138</v>
       </c>
       <c r="F40" s="2" t="s">
         <v>15</v>
@@ -3938,13 +3934,13 @@
         <v>35</v>
       </c>
       <c r="B41" s="2" t="s">
-        <v>207</v>
+        <v>205</v>
       </c>
       <c r="C41" s="2" t="s">
-        <v>208</v>
+        <v>206</v>
       </c>
       <c r="E41" s="2" t="s">
-        <v>140</v>
+        <v>138</v>
       </c>
       <c r="F41" s="2" t="s">
         <v>15</v>
@@ -3955,13 +3951,13 @@
         <v>36</v>
       </c>
       <c r="B42" s="2" t="s">
-        <v>209</v>
+        <v>207</v>
       </c>
       <c r="C42" s="2" t="s">
-        <v>210</v>
+        <v>208</v>
       </c>
       <c r="E42" s="2" t="s">
-        <v>140</v>
+        <v>138</v>
       </c>
       <c r="F42" s="2" t="s">
         <v>15</v>
@@ -3972,13 +3968,13 @@
         <v>37</v>
       </c>
       <c r="B43" s="2" t="s">
-        <v>211</v>
+        <v>209</v>
       </c>
       <c r="C43" s="2" t="s">
-        <v>212</v>
+        <v>210</v>
       </c>
       <c r="E43" s="2" t="s">
-        <v>140</v>
+        <v>138</v>
       </c>
       <c r="F43" s="2" t="s">
         <v>15</v>
@@ -3989,13 +3985,13 @@
         <v>38</v>
       </c>
       <c r="B44" s="2" t="s">
-        <v>213</v>
+        <v>211</v>
       </c>
       <c r="C44" s="2" t="s">
-        <v>214</v>
+        <v>212</v>
       </c>
       <c r="E44" s="2" t="s">
-        <v>140</v>
+        <v>138</v>
       </c>
       <c r="F44" s="2" t="s">
         <v>15</v>
@@ -4006,13 +4002,13 @@
         <v>39</v>
       </c>
       <c r="B45" s="2" t="s">
-        <v>215</v>
+        <v>213</v>
       </c>
       <c r="C45" s="2" t="s">
-        <v>216</v>
+        <v>214</v>
       </c>
       <c r="E45" s="2" t="s">
-        <v>140</v>
+        <v>138</v>
       </c>
       <c r="F45" s="2" t="s">
         <v>15</v>
@@ -4026,10 +4022,10 @@
         <v>26</v>
       </c>
       <c r="C46" s="2" t="s">
-        <v>217</v>
+        <v>215</v>
       </c>
       <c r="E46" s="2" t="s">
-        <v>140</v>
+        <v>138</v>
       </c>
       <c r="F46" s="2" t="s">
         <v>15</v>
@@ -4043,10 +4039,10 @@
         <v>28</v>
       </c>
       <c r="C47" s="2" t="s">
-        <v>218</v>
+        <v>216</v>
       </c>
       <c r="E47" s="2" t="s">
-        <v>140</v>
+        <v>138</v>
       </c>
       <c r="F47" s="2" t="s">
         <v>15</v>
@@ -4057,13 +4053,13 @@
         <v>42</v>
       </c>
       <c r="B48" s="2" t="s">
-        <v>219</v>
+        <v>217</v>
       </c>
       <c r="C48" s="2" t="s">
-        <v>191</v>
+        <v>189</v>
       </c>
       <c r="E48" s="2" t="s">
-        <v>140</v>
+        <v>138</v>
       </c>
       <c r="F48" s="2" t="s">
         <v>15</v>
@@ -4074,13 +4070,13 @@
         <v>43</v>
       </c>
       <c r="B49" s="2" t="s">
-        <v>220</v>
+        <v>218</v>
       </c>
       <c r="C49" s="2" t="s">
-        <v>221</v>
+        <v>219</v>
       </c>
       <c r="E49" s="2" t="s">
-        <v>140</v>
+        <v>138</v>
       </c>
       <c r="F49" s="2" t="s">
         <v>15</v>
@@ -4091,13 +4087,13 @@
         <v>44</v>
       </c>
       <c r="B50" s="2" t="s">
-        <v>222</v>
+        <v>220</v>
       </c>
       <c r="C50" s="2" t="s">
-        <v>223</v>
+        <v>221</v>
       </c>
       <c r="E50" s="2" t="s">
-        <v>140</v>
+        <v>138</v>
       </c>
       <c r="F50" s="2" t="s">
         <v>15</v>
@@ -4108,13 +4104,13 @@
         <v>45</v>
       </c>
       <c r="B51" s="2" t="s">
-        <v>224</v>
+        <v>222</v>
       </c>
       <c r="C51" s="2" t="s">
-        <v>225</v>
+        <v>223</v>
       </c>
       <c r="E51" s="2" t="s">
-        <v>140</v>
+        <v>138</v>
       </c>
       <c r="F51" s="2" t="s">
         <v>15</v>
@@ -4125,13 +4121,13 @@
         <v>46</v>
       </c>
       <c r="B52" s="2" t="s">
-        <v>226</v>
+        <v>224</v>
       </c>
       <c r="C52" s="2" t="s">
-        <v>227</v>
+        <v>225</v>
       </c>
       <c r="E52" s="2" t="s">
-        <v>140</v>
+        <v>138</v>
       </c>
       <c r="F52" s="2" t="s">
         <v>15</v>
@@ -4142,13 +4138,13 @@
         <v>47</v>
       </c>
       <c r="B53" s="2" t="s">
-        <v>228</v>
+        <v>226</v>
       </c>
       <c r="C53" s="2" t="s">
-        <v>229</v>
+        <v>227</v>
       </c>
       <c r="E53" s="2" t="s">
-        <v>140</v>
+        <v>138</v>
       </c>
       <c r="F53" s="2" t="s">
         <v>15</v>
@@ -4159,13 +4155,13 @@
         <v>48</v>
       </c>
       <c r="B54" s="2" t="s">
-        <v>230</v>
+        <v>228</v>
       </c>
       <c r="C54" s="2" t="s">
-        <v>231</v>
+        <v>229</v>
       </c>
       <c r="E54" s="2" t="s">
-        <v>140</v>
+        <v>138</v>
       </c>
       <c r="F54" s="2" t="s">
         <v>15</v>
@@ -4176,13 +4172,13 @@
         <v>49</v>
       </c>
       <c r="B55" s="2" t="s">
-        <v>232</v>
+        <v>230</v>
       </c>
       <c r="C55" s="2" t="s">
-        <v>233</v>
+        <v>231</v>
       </c>
       <c r="E55" s="2" t="s">
-        <v>140</v>
+        <v>138</v>
       </c>
       <c r="F55" s="2" t="s">
         <v>15</v>
@@ -4193,13 +4189,13 @@
         <v>50</v>
       </c>
       <c r="B56" s="2" t="s">
-        <v>234</v>
+        <v>232</v>
       </c>
       <c r="C56" s="2" t="s">
-        <v>235</v>
+        <v>233</v>
       </c>
       <c r="E56" s="2" t="s">
-        <v>140</v>
+        <v>138</v>
       </c>
       <c r="F56" s="2" t="s">
         <v>9</v>
@@ -4210,13 +4206,13 @@
         <v>51</v>
       </c>
       <c r="B57" s="2" t="s">
-        <v>236</v>
+        <v>234</v>
       </c>
       <c r="C57" s="2" t="s">
-        <v>237</v>
+        <v>235</v>
       </c>
       <c r="E57" s="2" t="s">
-        <v>140</v>
+        <v>138</v>
       </c>
       <c r="F57" s="2" t="s">
         <v>15</v>
@@ -4227,13 +4223,13 @@
         <v>52</v>
       </c>
       <c r="B58" s="2" t="s">
-        <v>238</v>
+        <v>236</v>
       </c>
       <c r="C58" s="2" t="s">
-        <v>239</v>
+        <v>237</v>
       </c>
       <c r="E58" s="2" t="s">
-        <v>140</v>
+        <v>138</v>
       </c>
       <c r="F58" s="2" t="s">
         <v>15</v>
@@ -4244,13 +4240,13 @@
         <v>52</v>
       </c>
       <c r="B59" s="2" t="s">
-        <v>240</v>
+        <v>238</v>
       </c>
       <c r="C59" s="2" t="s">
-        <v>241</v>
+        <v>239</v>
       </c>
       <c r="E59" s="2" t="s">
-        <v>140</v>
+        <v>138</v>
       </c>
       <c r="F59" s="2" t="s">
         <v>15</v>
@@ -4261,13 +4257,13 @@
         <v>67</v>
       </c>
       <c r="B60" s="2" t="s">
-        <v>242</v>
+        <v>240</v>
       </c>
       <c r="C60" s="2" t="s">
-        <v>243</v>
+        <v>241</v>
       </c>
       <c r="E60" s="2" t="s">
-        <v>140</v>
+        <v>138</v>
       </c>
       <c r="F60" s="2" t="s">
         <v>15</v>
@@ -4278,13 +4274,13 @@
         <v>67</v>
       </c>
       <c r="B61" s="2" t="s">
-        <v>244</v>
+        <v>242</v>
       </c>
       <c r="C61" s="2" t="s">
-        <v>245</v>
+        <v>243</v>
       </c>
       <c r="E61" s="2" t="s">
-        <v>140</v>
+        <v>138</v>
       </c>
       <c r="F61" s="2" t="s">
         <v>15</v>
@@ -4295,13 +4291,13 @@
         <v>67</v>
       </c>
       <c r="B62" s="2" t="s">
-        <v>246</v>
+        <v>244</v>
       </c>
       <c r="C62" s="2" t="s">
-        <v>247</v>
+        <v>245</v>
       </c>
       <c r="E62" s="2" t="s">
-        <v>140</v>
+        <v>138</v>
       </c>
       <c r="F62" s="2" t="s">
         <v>15</v>
@@ -4312,13 +4308,13 @@
         <v>67</v>
       </c>
       <c r="B63" s="2" t="s">
-        <v>248</v>
+        <v>246</v>
       </c>
       <c r="C63" s="2" t="s">
-        <v>249</v>
+        <v>247</v>
       </c>
       <c r="E63" s="2" t="s">
-        <v>140</v>
+        <v>138</v>
       </c>
       <c r="F63" s="2" t="s">
         <v>15</v>
@@ -4332,10 +4328,10 @@
         <v>67</v>
       </c>
       <c r="C64" s="5" t="s">
-        <v>250</v>
+        <v>248</v>
       </c>
       <c r="E64" s="5" t="s">
-        <v>140</v>
+        <v>138</v>
       </c>
       <c r="F64" s="5" t="s">
         <v>15</v>
@@ -4346,13 +4342,13 @@
         <v>57</v>
       </c>
       <c r="B65" s="2" t="s">
-        <v>251</v>
+        <v>249</v>
       </c>
       <c r="C65" s="2" t="s">
-        <v>252</v>
+        <v>250</v>
       </c>
       <c r="E65" s="2" t="s">
-        <v>140</v>
+        <v>138</v>
       </c>
       <c r="F65" s="2" t="s">
         <v>15</v>
@@ -4363,13 +4359,13 @@
         <v>57</v>
       </c>
       <c r="B66" s="2" t="s">
-        <v>253</v>
+        <v>251</v>
       </c>
       <c r="C66" s="2" t="s">
         <v>85</v>
       </c>
       <c r="E66" s="2" t="s">
-        <v>140</v>
+        <v>138</v>
       </c>
       <c r="F66" s="2" t="s">
         <v>15</v>
@@ -4380,13 +4376,13 @@
         <v>57</v>
       </c>
       <c r="B67" s="2" t="s">
-        <v>254</v>
+        <v>252</v>
       </c>
       <c r="C67" s="2" t="s">
-        <v>255</v>
+        <v>253</v>
       </c>
       <c r="E67" s="2" t="s">
-        <v>140</v>
+        <v>138</v>
       </c>
       <c r="F67" s="2" t="s">
         <v>15</v>
@@ -4397,13 +4393,13 @@
         <v>57</v>
       </c>
       <c r="B68" s="2" t="s">
-        <v>256</v>
+        <v>254</v>
       </c>
       <c r="C68" s="2" t="s">
         <v>91</v>
       </c>
       <c r="E68" s="2" t="s">
-        <v>140</v>
+        <v>138</v>
       </c>
       <c r="F68" s="2" t="s">
         <v>15</v>
@@ -4414,13 +4410,13 @@
         <v>57</v>
       </c>
       <c r="B69" s="2" t="s">
-        <v>257</v>
+        <v>255</v>
       </c>
       <c r="C69" s="2" t="s">
         <v>94</v>
       </c>
       <c r="E69" s="2" t="s">
-        <v>140</v>
+        <v>138</v>
       </c>
       <c r="F69" s="2" t="s">
         <v>15</v>
@@ -4431,13 +4427,13 @@
         <v>58</v>
       </c>
       <c r="B70" s="2" t="s">
-        <v>258</v>
+        <v>256</v>
       </c>
       <c r="C70" s="2" t="s">
-        <v>259</v>
+        <v>257</v>
       </c>
       <c r="E70" s="2" t="s">
-        <v>140</v>
+        <v>138</v>
       </c>
       <c r="F70" s="2" t="s">
         <v>15</v>
@@ -4448,16 +4444,16 @@
         <v>59</v>
       </c>
       <c r="B71" s="2" t="s">
-        <v>260</v>
+        <v>258</v>
       </c>
       <c r="C71" s="2" t="s">
-        <v>261</v>
+        <v>259</v>
       </c>
       <c r="D71" s="2" t="s">
         <v>14</v>
       </c>
       <c r="E71" s="2" t="s">
-        <v>140</v>
+        <v>138</v>
       </c>
       <c r="F71" s="2" t="s">
         <v>15</v>
@@ -4468,16 +4464,16 @@
         <v>60</v>
       </c>
       <c r="B72" s="2" t="s">
-        <v>262</v>
+        <v>260</v>
       </c>
       <c r="C72" s="2" t="s">
-        <v>263</v>
+        <v>261</v>
       </c>
       <c r="D72" s="2" t="s">
         <v>14</v>
       </c>
       <c r="E72" s="2" t="s">
-        <v>140</v>
+        <v>138</v>
       </c>
       <c r="F72" s="2" t="s">
         <v>15</v>
@@ -4488,16 +4484,16 @@
         <v>61</v>
       </c>
       <c r="B73" s="2" t="s">
-        <v>264</v>
+        <v>262</v>
       </c>
       <c r="C73" s="2" t="s">
-        <v>265</v>
+        <v>263</v>
       </c>
       <c r="D73" s="2" t="s">
         <v>14</v>
       </c>
       <c r="E73" s="2" t="s">
-        <v>140</v>
+        <v>138</v>
       </c>
       <c r="F73" s="2" t="s">
         <v>15</v>
@@ -4508,16 +4504,16 @@
         <v>62</v>
       </c>
       <c r="B74" s="2" t="s">
-        <v>266</v>
+        <v>264</v>
       </c>
       <c r="C74" s="2" t="s">
-        <v>267</v>
+        <v>265</v>
       </c>
       <c r="D74" s="2" t="s">
         <v>14</v>
       </c>
       <c r="E74" s="2" t="s">
-        <v>140</v>
+        <v>138</v>
       </c>
       <c r="F74" s="2" t="s">
         <v>15</v>
@@ -4528,13 +4524,13 @@
         <v>63</v>
       </c>
       <c r="B75" s="2" t="s">
-        <v>268</v>
+        <v>266</v>
       </c>
       <c r="C75" s="2" t="s">
-        <v>269</v>
+        <v>267</v>
       </c>
       <c r="E75" s="2" t="s">
-        <v>140</v>
+        <v>138</v>
       </c>
       <c r="F75" s="2" t="s">
         <v>15</v>
@@ -4548,10 +4544,10 @@
         <v>18</v>
       </c>
       <c r="C76" s="2" t="s">
-        <v>270</v>
+        <v>268</v>
       </c>
       <c r="E76" s="2" t="s">
-        <v>140</v>
+        <v>138</v>
       </c>
       <c r="F76" s="2" t="s">
         <v>15</v>
@@ -4562,13 +4558,13 @@
         <v>65</v>
       </c>
       <c r="B77" s="2" t="s">
-        <v>271</v>
+        <v>269</v>
       </c>
       <c r="C77" s="2" t="s">
-        <v>272</v>
+        <v>270</v>
       </c>
       <c r="E77" s="2" t="s">
-        <v>140</v>
+        <v>138</v>
       </c>
       <c r="F77" s="2" t="s">
         <v>15</v>
@@ -4579,13 +4575,13 @@
         <v>66</v>
       </c>
       <c r="B78" s="2" t="s">
-        <v>273</v>
+        <v>271</v>
       </c>
       <c r="C78" s="2" t="s">
-        <v>274</v>
+        <v>272</v>
       </c>
       <c r="E78" s="2" t="s">
-        <v>140</v>
+        <v>138</v>
       </c>
       <c r="F78" s="2" t="s">
         <v>15</v>
@@ -4596,13 +4592,13 @@
         <v>67</v>
       </c>
       <c r="B79" s="2" t="s">
-        <v>275</v>
+        <v>273</v>
       </c>
       <c r="C79" s="2" t="s">
-        <v>276</v>
+        <v>274</v>
       </c>
       <c r="E79" s="2" t="s">
-        <v>140</v>
+        <v>138</v>
       </c>
       <c r="F79" s="2" t="s">
         <v>15</v>
@@ -4613,13 +4609,13 @@
         <v>68</v>
       </c>
       <c r="B80" s="2" t="s">
-        <v>277</v>
+        <v>275</v>
       </c>
       <c r="C80" s="2" t="s">
-        <v>278</v>
+        <v>276</v>
       </c>
       <c r="E80" s="2" t="s">
-        <v>140</v>
+        <v>138</v>
       </c>
       <c r="F80" s="2" t="s">
         <v>15</v>
@@ -4630,13 +4626,13 @@
         <v>69</v>
       </c>
       <c r="B81" s="2" t="s">
-        <v>279</v>
+        <v>277</v>
       </c>
       <c r="C81" s="2" t="s">
-        <v>280</v>
+        <v>278</v>
       </c>
       <c r="E81" s="2" t="s">
-        <v>140</v>
+        <v>138</v>
       </c>
       <c r="F81" s="2" t="s">
         <v>15</v>
@@ -4647,13 +4643,13 @@
         <v>70</v>
       </c>
       <c r="B82" s="2" t="s">
-        <v>281</v>
+        <v>279</v>
       </c>
       <c r="C82" s="2" t="s">
-        <v>282</v>
+        <v>280</v>
       </c>
       <c r="E82" s="2" t="s">
-        <v>140</v>
+        <v>138</v>
       </c>
       <c r="F82" s="2" t="s">
         <v>15</v>
@@ -4664,13 +4660,13 @@
         <v>67</v>
       </c>
       <c r="B83" s="2" t="s">
-        <v>283</v>
+        <v>281</v>
       </c>
       <c r="C83" s="2" t="s">
-        <v>284</v>
+        <v>282</v>
       </c>
       <c r="E83" s="2" t="s">
-        <v>140</v>
+        <v>138</v>
       </c>
       <c r="F83" s="2" t="s">
         <v>15</v>
@@ -4681,13 +4677,13 @@
         <v>67</v>
       </c>
       <c r="B84" s="2" t="s">
-        <v>285</v>
+        <v>283</v>
       </c>
       <c r="C84" s="2" t="s">
-        <v>286</v>
+        <v>284</v>
       </c>
       <c r="E84" s="2" t="s">
-        <v>140</v>
+        <v>138</v>
       </c>
       <c r="F84" s="2" t="s">
         <v>15</v>
@@ -4698,13 +4694,13 @@
         <v>71</v>
       </c>
       <c r="B85" s="2" t="s">
-        <v>287</v>
+        <v>285</v>
       </c>
       <c r="C85" s="2" t="s">
-        <v>288</v>
+        <v>286</v>
       </c>
       <c r="E85" s="2" t="s">
-        <v>140</v>
+        <v>138</v>
       </c>
       <c r="F85" s="2" t="s">
         <v>15</v>
@@ -4715,13 +4711,13 @@
         <v>72</v>
       </c>
       <c r="B86" s="2" t="s">
-        <v>289</v>
+        <v>287</v>
       </c>
       <c r="C86" s="2" t="s">
-        <v>290</v>
+        <v>288</v>
       </c>
       <c r="E86" s="2" t="s">
-        <v>140</v>
+        <v>138</v>
       </c>
       <c r="F86" s="2" t="s">
         <v>15</v>
@@ -4732,13 +4728,13 @@
         <v>73</v>
       </c>
       <c r="B87" s="2" t="s">
-        <v>291</v>
+        <v>289</v>
       </c>
       <c r="C87" s="2" t="s">
-        <v>292</v>
+        <v>290</v>
       </c>
       <c r="E87" s="2" t="s">
-        <v>140</v>
+        <v>138</v>
       </c>
       <c r="F87" s="2" t="s">
         <v>15</v>
@@ -4749,13 +4745,13 @@
         <v>73</v>
       </c>
       <c r="B88" s="2" t="s">
-        <v>293</v>
+        <v>291</v>
       </c>
       <c r="C88" s="2" t="s">
-        <v>294</v>
+        <v>292</v>
       </c>
       <c r="E88" s="2" t="s">
-        <v>140</v>
+        <v>138</v>
       </c>
       <c r="F88" s="2" t="s">
         <v>15</v>
@@ -4766,13 +4762,13 @@
         <v>74</v>
       </c>
       <c r="B89" s="2" t="s">
-        <v>295</v>
+        <v>293</v>
       </c>
       <c r="C89" s="2" t="s">
-        <v>296</v>
+        <v>294</v>
       </c>
       <c r="E89" s="2" t="s">
-        <v>140</v>
+        <v>138</v>
       </c>
       <c r="F89" s="2" t="s">
         <v>15</v>
@@ -4783,13 +4779,13 @@
         <v>75</v>
       </c>
       <c r="B90" s="2" t="s">
-        <v>297</v>
+        <v>295</v>
       </c>
       <c r="C90" s="2" t="s">
-        <v>298</v>
+        <v>296</v>
       </c>
       <c r="E90" s="2" t="s">
-        <v>140</v>
+        <v>138</v>
       </c>
       <c r="F90" s="2" t="s">
         <v>15</v>
@@ -4800,13 +4796,13 @@
         <v>76</v>
       </c>
       <c r="B91" s="2" t="s">
-        <v>299</v>
+        <v>297</v>
       </c>
       <c r="C91" s="2" t="s">
-        <v>300</v>
+        <v>298</v>
       </c>
       <c r="E91" s="2" t="s">
-        <v>140</v>
+        <v>138</v>
       </c>
       <c r="F91" s="2" t="s">
         <v>15</v>
@@ -4817,13 +4813,13 @@
         <v>77</v>
       </c>
       <c r="B92" s="2" t="s">
-        <v>301</v>
+        <v>299</v>
       </c>
       <c r="C92" s="2" t="s">
-        <v>302</v>
+        <v>300</v>
       </c>
       <c r="E92" s="2" t="s">
-        <v>140</v>
+        <v>138</v>
       </c>
       <c r="F92" s="2" t="s">
         <v>15</v>
@@ -4834,13 +4830,13 @@
         <v>78</v>
       </c>
       <c r="B93" s="2" t="s">
-        <v>303</v>
+        <v>301</v>
       </c>
       <c r="C93" s="2" t="s">
-        <v>304</v>
+        <v>302</v>
       </c>
       <c r="E93" s="2" t="s">
-        <v>140</v>
+        <v>138</v>
       </c>
       <c r="F93" s="2" t="s">
         <v>15</v>
@@ -4848,16 +4844,16 @@
     </row>
     <row r="94" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A94" s="6" t="s">
+        <v>303</v>
+      </c>
+      <c r="B94" s="2" t="s">
+        <v>304</v>
+      </c>
+      <c r="C94" s="2" t="s">
         <v>305</v>
       </c>
-      <c r="B94" s="2" t="s">
-        <v>306</v>
-      </c>
-      <c r="C94" s="2" t="s">
-        <v>307</v>
-      </c>
       <c r="E94" s="2" t="s">
-        <v>140</v>
+        <v>138</v>
       </c>
       <c r="F94" s="2" t="s">
         <v>15</v>
@@ -4868,13 +4864,13 @@
         <v>79</v>
       </c>
       <c r="B95" s="2" t="s">
-        <v>308</v>
+        <v>306</v>
       </c>
       <c r="C95" s="2" t="s">
-        <v>309</v>
+        <v>307</v>
       </c>
       <c r="E95" s="2" t="s">
-        <v>140</v>
+        <v>138</v>
       </c>
       <c r="F95" s="2" t="s">
         <v>15</v>
@@ -4885,13 +4881,13 @@
         <v>80</v>
       </c>
       <c r="B96" s="2" t="s">
-        <v>310</v>
+        <v>308</v>
       </c>
       <c r="C96" s="2" t="s">
-        <v>311</v>
+        <v>309</v>
       </c>
       <c r="E96" s="2" t="s">
-        <v>140</v>
+        <v>138</v>
       </c>
       <c r="F96" s="2" t="s">
         <v>15</v>
@@ -4902,13 +4898,13 @@
         <v>81</v>
       </c>
       <c r="B97" s="2" t="s">
-        <v>312</v>
+        <v>310</v>
       </c>
       <c r="C97" s="2" t="s">
-        <v>313</v>
+        <v>311</v>
       </c>
       <c r="E97" s="2" t="s">
-        <v>140</v>
+        <v>138</v>
       </c>
       <c r="F97" s="2" t="s">
         <v>15</v>
@@ -4919,13 +4915,13 @@
         <v>82</v>
       </c>
       <c r="B98" s="2" t="s">
-        <v>314</v>
+        <v>312</v>
       </c>
       <c r="C98" s="2" t="s">
-        <v>315</v>
+        <v>313</v>
       </c>
       <c r="E98" s="2" t="s">
-        <v>140</v>
+        <v>138</v>
       </c>
       <c r="F98" s="2" t="s">
         <v>15</v>
@@ -4936,13 +4932,13 @@
         <v>82</v>
       </c>
       <c r="B99" s="2" t="s">
-        <v>316</v>
+        <v>314</v>
       </c>
       <c r="C99" s="2" t="s">
-        <v>317</v>
+        <v>315</v>
       </c>
       <c r="E99" s="2" t="s">
-        <v>140</v>
+        <v>138</v>
       </c>
       <c r="F99" s="2" t="s">
         <v>15</v>
@@ -4953,13 +4949,13 @@
         <v>82</v>
       </c>
       <c r="B100" s="2" t="s">
-        <v>318</v>
+        <v>316</v>
       </c>
       <c r="C100" s="2" t="s">
-        <v>319</v>
+        <v>317</v>
       </c>
       <c r="E100" s="2" t="s">
-        <v>140</v>
+        <v>138</v>
       </c>
       <c r="F100" s="2" t="s">
         <v>15</v>
@@ -4970,13 +4966,13 @@
         <v>82</v>
       </c>
       <c r="B101" s="2" t="s">
-        <v>320</v>
+        <v>318</v>
       </c>
       <c r="C101" s="2" t="s">
-        <v>321</v>
+        <v>319</v>
       </c>
       <c r="E101" s="2" t="s">
-        <v>140</v>
+        <v>138</v>
       </c>
       <c r="F101" s="2" t="s">
         <v>15</v>
@@ -4987,13 +4983,13 @@
         <v>82</v>
       </c>
       <c r="B102" s="2" t="s">
-        <v>322</v>
+        <v>320</v>
       </c>
       <c r="C102" s="2" t="s">
-        <v>323</v>
+        <v>321</v>
       </c>
       <c r="E102" s="2" t="s">
-        <v>140</v>
+        <v>138</v>
       </c>
       <c r="F102" s="2" t="s">
         <v>15</v>
@@ -5010,7 +5006,7 @@
         <v>49</v>
       </c>
       <c r="E103" s="2" t="s">
-        <v>140</v>
+        <v>138</v>
       </c>
       <c r="F103" s="2" t="s">
         <v>15</v>
@@ -5027,7 +5023,7 @@
         <v>47</v>
       </c>
       <c r="E104" s="2" t="s">
-        <v>140</v>
+        <v>138</v>
       </c>
       <c r="F104" s="2" t="s">
         <v>15</v>
@@ -5041,10 +5037,10 @@
         <v>52</v>
       </c>
       <c r="C105" s="2" t="s">
-        <v>324</v>
+        <v>322</v>
       </c>
       <c r="E105" s="2" t="s">
-        <v>140</v>
+        <v>138</v>
       </c>
       <c r="F105" s="2" t="s">
         <v>15</v>
@@ -5055,13 +5051,13 @@
         <v>86</v>
       </c>
       <c r="B106" s="2" t="s">
-        <v>325</v>
+        <v>323</v>
       </c>
       <c r="C106" s="2" t="s">
-        <v>326</v>
+        <v>324</v>
       </c>
       <c r="E106" s="2" t="s">
-        <v>140</v>
+        <v>138</v>
       </c>
       <c r="F106" s="2" t="s">
         <v>15</v>
@@ -5072,13 +5068,13 @@
         <v>87</v>
       </c>
       <c r="B107" s="2" t="s">
-        <v>327</v>
+        <v>325</v>
       </c>
       <c r="C107" s="2" t="s">
-        <v>302</v>
+        <v>300</v>
       </c>
       <c r="E107" s="2" t="s">
-        <v>140</v>
+        <v>138</v>
       </c>
       <c r="F107" s="2" t="s">
         <v>15</v>
@@ -5089,13 +5085,13 @@
         <v>87</v>
       </c>
       <c r="B108" s="2" t="s">
-        <v>328</v>
+        <v>326</v>
       </c>
       <c r="C108" s="2" t="s">
-        <v>329</v>
+        <v>327</v>
       </c>
       <c r="E108" s="2" t="s">
-        <v>140</v>
+        <v>138</v>
       </c>
       <c r="F108" s="2" t="s">
         <v>15</v>
@@ -5106,13 +5102,13 @@
         <v>87</v>
       </c>
       <c r="B109" s="2" t="s">
-        <v>330</v>
+        <v>328</v>
       </c>
       <c r="C109" s="2" t="s">
-        <v>331</v>
+        <v>329</v>
       </c>
       <c r="E109" s="2" t="s">
-        <v>140</v>
+        <v>138</v>
       </c>
       <c r="F109" s="2" t="s">
         <v>15</v>
@@ -5123,13 +5119,13 @@
         <v>87</v>
       </c>
       <c r="B110" s="2" t="s">
-        <v>332</v>
+        <v>330</v>
       </c>
       <c r="C110" s="2" t="s">
-        <v>333</v>
+        <v>331</v>
       </c>
       <c r="E110" s="2" t="s">
-        <v>140</v>
+        <v>138</v>
       </c>
       <c r="F110" s="2" t="s">
         <v>15</v>
@@ -5140,13 +5136,13 @@
         <v>87</v>
       </c>
       <c r="B111" s="2" t="s">
-        <v>334</v>
+        <v>332</v>
       </c>
       <c r="C111" s="2" t="s">
-        <v>335</v>
+        <v>333</v>
       </c>
       <c r="E111" s="2" t="s">
-        <v>140</v>
+        <v>138</v>
       </c>
       <c r="F111" s="2" t="s">
         <v>15</v>
@@ -5157,13 +5153,13 @@
         <v>87</v>
       </c>
       <c r="B112" s="2" t="s">
-        <v>336</v>
+        <v>334</v>
       </c>
       <c r="C112" s="2" t="s">
-        <v>337</v>
+        <v>335</v>
       </c>
       <c r="E112" s="2" t="s">
-        <v>140</v>
+        <v>138</v>
       </c>
       <c r="F112" s="2" t="s">
         <v>15</v>
@@ -5174,13 +5170,13 @@
         <v>88</v>
       </c>
       <c r="B113" s="2" t="s">
-        <v>338</v>
+        <v>336</v>
       </c>
       <c r="C113" s="2" t="s">
-        <v>339</v>
+        <v>337</v>
       </c>
       <c r="E113" s="2" t="s">
-        <v>140</v>
+        <v>138</v>
       </c>
       <c r="F113" s="2" t="s">
         <v>15</v>
@@ -5191,13 +5187,13 @@
         <v>89</v>
       </c>
       <c r="B114" s="2" t="s">
-        <v>340</v>
+        <v>338</v>
       </c>
       <c r="C114" s="2" t="s">
-        <v>341</v>
+        <v>339</v>
       </c>
       <c r="E114" s="2" t="s">
-        <v>140</v>
+        <v>138</v>
       </c>
       <c r="F114" s="2" t="s">
         <v>15</v>
@@ -5208,13 +5204,13 @@
         <v>90</v>
       </c>
       <c r="B115" s="2" t="s">
-        <v>342</v>
+        <v>340</v>
       </c>
       <c r="C115" s="2" t="s">
-        <v>343</v>
+        <v>341</v>
       </c>
       <c r="E115" s="2" t="s">
-        <v>140</v>
+        <v>138</v>
       </c>
       <c r="F115" s="2" t="s">
         <v>15</v>
@@ -5225,13 +5221,13 @@
         <v>91</v>
       </c>
       <c r="B116" s="2" t="s">
-        <v>344</v>
+        <v>342</v>
       </c>
       <c r="C116" s="2" t="s">
-        <v>345</v>
+        <v>343</v>
       </c>
       <c r="E116" s="2" t="s">
-        <v>140</v>
+        <v>138</v>
       </c>
       <c r="F116" s="2" t="s">
         <v>15</v>
@@ -5242,13 +5238,13 @@
         <v>92</v>
       </c>
       <c r="B117" s="2" t="s">
-        <v>346</v>
+        <v>344</v>
       </c>
       <c r="C117" s="2" t="s">
-        <v>347</v>
+        <v>345</v>
       </c>
       <c r="E117" s="2" t="s">
-        <v>140</v>
+        <v>138</v>
       </c>
       <c r="F117" s="2" t="s">
         <v>15</v>
@@ -5262,10 +5258,10 @@
         <v>67</v>
       </c>
       <c r="C118" s="5" t="s">
-        <v>348</v>
+        <v>346</v>
       </c>
       <c r="E118" s="2" t="s">
-        <v>140</v>
+        <v>138</v>
       </c>
       <c r="F118" s="2" t="s">
         <v>15</v>
@@ -5279,10 +5275,10 @@
         <v>67</v>
       </c>
       <c r="C119" s="5" t="s">
-        <v>349</v>
+        <v>347</v>
       </c>
       <c r="E119" s="2" t="s">
-        <v>140</v>
+        <v>138</v>
       </c>
       <c r="F119" s="2" t="s">
         <v>15</v>
@@ -5296,10 +5292,10 @@
         <v>67</v>
       </c>
       <c r="C120" s="4" t="s">
-        <v>350</v>
+        <v>348</v>
       </c>
       <c r="E120" s="2" t="s">
-        <v>140</v>
+        <v>138</v>
       </c>
       <c r="F120" s="2" t="s">
         <v>15</v>
@@ -5313,10 +5309,10 @@
         <v>67</v>
       </c>
       <c r="C121" s="4" t="s">
-        <v>351</v>
+        <v>349</v>
       </c>
       <c r="E121" s="2" t="s">
-        <v>140</v>
+        <v>138</v>
       </c>
       <c r="F121" s="2" t="s">
         <v>15</v>
@@ -5324,16 +5320,16 @@
     </row>
     <row r="122" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A122" s="3" t="s">
-        <v>523</v>
+        <v>521</v>
       </c>
       <c r="B122" s="4" t="s">
         <v>67</v>
       </c>
       <c r="C122" s="4" t="s">
-        <v>529</v>
+        <v>527</v>
       </c>
       <c r="E122" s="4" t="s">
-        <v>140</v>
+        <v>138</v>
       </c>
       <c r="F122" s="5" t="s">
         <v>15</v>
@@ -5361,862 +5357,862 @@
   <sheetData>
     <row r="1" spans="1:1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="7" t="s">
-        <v>352</v>
+        <v>350</v>
       </c>
     </row>
     <row r="2" spans="1:1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="7" t="s">
-        <v>353</v>
+        <v>351</v>
       </c>
     </row>
     <row r="3" spans="1:1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="7" t="s">
-        <v>354</v>
+        <v>352</v>
       </c>
     </row>
     <row r="4" spans="1:1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="7" t="s">
-        <v>355</v>
+        <v>353</v>
       </c>
     </row>
     <row r="5" spans="1:1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="7" t="s">
-        <v>356</v>
+        <v>354</v>
       </c>
     </row>
     <row r="6" spans="1:1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="7" t="s">
-        <v>357</v>
+        <v>355</v>
       </c>
     </row>
     <row r="7" spans="1:1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="7" t="s">
-        <v>358</v>
+        <v>356</v>
       </c>
     </row>
     <row r="8" spans="1:1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" s="7" t="s">
-        <v>359</v>
+        <v>357</v>
       </c>
     </row>
     <row r="9" spans="1:1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" s="7" t="s">
-        <v>360</v>
+        <v>358</v>
       </c>
     </row>
     <row r="10" spans="1:1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" s="7" t="s">
-        <v>361</v>
+        <v>359</v>
       </c>
     </row>
     <row r="11" spans="1:1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A11" s="7" t="s">
-        <v>362</v>
+        <v>360</v>
       </c>
     </row>
     <row r="12" spans="1:1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A12" s="7" t="s">
-        <v>363</v>
+        <v>361</v>
       </c>
     </row>
     <row r="13" spans="1:1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A13" s="7" t="s">
-        <v>364</v>
+        <v>362</v>
       </c>
     </row>
     <row r="14" spans="1:1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A14" s="7" t="s">
-        <v>365</v>
+        <v>363</v>
       </c>
     </row>
     <row r="15" spans="1:1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A15" s="7" t="s">
-        <v>366</v>
+        <v>364</v>
       </c>
     </row>
     <row r="16" spans="1:1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A16" s="7" t="s">
-        <v>367</v>
+        <v>365</v>
       </c>
     </row>
     <row r="17" spans="1:1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A17" s="7" t="s">
-        <v>368</v>
+        <v>366</v>
       </c>
     </row>
     <row r="18" spans="1:1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A18" s="7" t="s">
-        <v>369</v>
+        <v>367</v>
       </c>
     </row>
     <row r="19" spans="1:1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A19" s="7" t="s">
-        <v>370</v>
+        <v>368</v>
       </c>
     </row>
     <row r="20" spans="1:1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A20" s="7" t="s">
-        <v>371</v>
+        <v>369</v>
       </c>
     </row>
     <row r="21" spans="1:1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A21" s="7" t="s">
-        <v>372</v>
+        <v>370</v>
       </c>
     </row>
     <row r="22" spans="1:1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A22" s="7" t="s">
-        <v>373</v>
+        <v>371</v>
       </c>
     </row>
     <row r="23" spans="1:1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A23" s="7" t="s">
-        <v>374</v>
+        <v>372</v>
       </c>
     </row>
     <row r="24" spans="1:1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A24" s="7" t="s">
-        <v>375</v>
+        <v>373</v>
       </c>
     </row>
     <row r="25" spans="1:1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A25" s="7" t="s">
-        <v>376</v>
+        <v>374</v>
       </c>
     </row>
     <row r="26" spans="1:1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A26" s="7" t="s">
-        <v>377</v>
+        <v>375</v>
       </c>
     </row>
     <row r="27" spans="1:1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A27" s="7" t="s">
-        <v>378</v>
+        <v>376</v>
       </c>
     </row>
     <row r="28" spans="1:1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A28" s="7" t="s">
-        <v>379</v>
+        <v>377</v>
       </c>
     </row>
     <row r="29" spans="1:1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A29" s="7" t="s">
-        <v>380</v>
+        <v>378</v>
       </c>
     </row>
     <row r="30" spans="1:1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A30" s="7" t="s">
-        <v>381</v>
+        <v>379</v>
       </c>
     </row>
     <row r="31" spans="1:1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A31" s="7" t="s">
-        <v>382</v>
+        <v>380</v>
       </c>
     </row>
     <row r="32" spans="1:1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A32" s="7" t="s">
-        <v>383</v>
+        <v>381</v>
       </c>
     </row>
     <row r="33" spans="1:1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A33" s="7" t="s">
-        <v>384</v>
+        <v>382</v>
       </c>
     </row>
     <row r="34" spans="1:1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A34" s="7" t="s">
-        <v>385</v>
+        <v>383</v>
       </c>
     </row>
     <row r="35" spans="1:1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A35" s="7" t="s">
-        <v>386</v>
+        <v>384</v>
       </c>
     </row>
     <row r="36" spans="1:1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A36" s="7" t="s">
-        <v>387</v>
+        <v>385</v>
       </c>
     </row>
     <row r="37" spans="1:1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A37" s="7" t="s">
-        <v>388</v>
+        <v>386</v>
       </c>
     </row>
     <row r="38" spans="1:1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A38" s="7" t="s">
-        <v>389</v>
+        <v>387</v>
       </c>
     </row>
     <row r="39" spans="1:1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A39" s="7" t="s">
-        <v>390</v>
+        <v>388</v>
       </c>
     </row>
     <row r="40" spans="1:1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A40" s="7" t="s">
-        <v>391</v>
+        <v>389</v>
       </c>
     </row>
     <row r="41" spans="1:1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A41" s="7" t="s">
-        <v>392</v>
+        <v>390</v>
       </c>
     </row>
     <row r="42" spans="1:1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A42" s="7" t="s">
-        <v>393</v>
+        <v>391</v>
       </c>
     </row>
     <row r="43" spans="1:1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A43" s="7" t="s">
-        <v>394</v>
+        <v>392</v>
       </c>
     </row>
     <row r="44" spans="1:1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A44" s="7" t="s">
-        <v>395</v>
+        <v>393</v>
       </c>
     </row>
     <row r="45" spans="1:1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A45" s="7" t="s">
-        <v>396</v>
+        <v>394</v>
       </c>
     </row>
     <row r="46" spans="1:1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A46" s="7" t="s">
-        <v>397</v>
+        <v>395</v>
       </c>
     </row>
     <row r="47" spans="1:1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A47" s="7" t="s">
-        <v>398</v>
+        <v>396</v>
       </c>
     </row>
     <row r="48" spans="1:1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A48" s="7" t="s">
-        <v>399</v>
+        <v>397</v>
       </c>
     </row>
     <row r="49" spans="1:1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A49" s="7" t="s">
-        <v>400</v>
+        <v>398</v>
       </c>
     </row>
     <row r="50" spans="1:1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A50" s="7" t="s">
-        <v>401</v>
+        <v>399</v>
       </c>
     </row>
     <row r="51" spans="1:1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A51" s="7" t="s">
-        <v>402</v>
+        <v>400</v>
       </c>
     </row>
     <row r="52" spans="1:1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A52" s="7" t="s">
-        <v>403</v>
+        <v>401</v>
       </c>
     </row>
     <row r="53" spans="1:1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A53" s="7" t="s">
-        <v>404</v>
+        <v>402</v>
       </c>
     </row>
     <row r="54" spans="1:1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A54" s="7" t="s">
-        <v>405</v>
+        <v>403</v>
       </c>
     </row>
     <row r="55" spans="1:1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A55" s="7" t="s">
-        <v>406</v>
+        <v>404</v>
       </c>
     </row>
     <row r="56" spans="1:1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A56" s="7" t="s">
-        <v>407</v>
+        <v>405</v>
       </c>
     </row>
     <row r="57" spans="1:1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A57" s="7" t="s">
-        <v>408</v>
+        <v>406</v>
       </c>
     </row>
     <row r="58" spans="1:1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A58" s="7" t="s">
-        <v>409</v>
+        <v>407</v>
       </c>
     </row>
     <row r="60" spans="1:1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A60" s="7" t="s">
-        <v>410</v>
+        <v>408</v>
       </c>
     </row>
     <row r="61" spans="1:1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A61" s="7" t="s">
-        <v>411</v>
+        <v>409</v>
       </c>
     </row>
     <row r="62" spans="1:1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A62" s="7" t="s">
-        <v>412</v>
+        <v>410</v>
       </c>
     </row>
     <row r="63" spans="1:1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A63" s="7" t="s">
-        <v>413</v>
+        <v>411</v>
       </c>
     </row>
     <row r="64" spans="1:1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A64" s="7" t="s">
-        <v>414</v>
+        <v>412</v>
       </c>
     </row>
     <row r="65" spans="1:1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A65" s="7" t="s">
-        <v>415</v>
+        <v>413</v>
       </c>
     </row>
     <row r="66" spans="1:1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A66" s="7" t="s">
-        <v>416</v>
+        <v>414</v>
       </c>
     </row>
     <row r="67" spans="1:1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A67" s="7" t="s">
-        <v>417</v>
+        <v>415</v>
       </c>
     </row>
     <row r="68" spans="1:1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A68" s="7" t="s">
-        <v>418</v>
+        <v>416</v>
       </c>
     </row>
     <row r="69" spans="1:1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A69" s="7" t="s">
-        <v>419</v>
+        <v>417</v>
       </c>
     </row>
     <row r="70" spans="1:1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A70" s="7" t="s">
-        <v>420</v>
+        <v>418</v>
       </c>
     </row>
     <row r="71" spans="1:1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A71" s="7" t="s">
-        <v>421</v>
+        <v>419</v>
       </c>
     </row>
     <row r="72" spans="1:1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A72" s="7" t="s">
-        <v>422</v>
+        <v>420</v>
       </c>
     </row>
     <row r="73" spans="1:1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A73" s="7" t="s">
-        <v>423</v>
+        <v>421</v>
       </c>
     </row>
     <row r="74" spans="1:1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A74" s="7" t="s">
-        <v>424</v>
+        <v>422</v>
       </c>
     </row>
     <row r="75" spans="1:1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A75" s="7" t="s">
-        <v>425</v>
+        <v>423</v>
       </c>
     </row>
     <row r="76" spans="1:1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A76" s="7" t="s">
-        <v>426</v>
+        <v>424</v>
       </c>
     </row>
     <row r="77" spans="1:1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A77" s="7" t="s">
-        <v>427</v>
+        <v>425</v>
       </c>
     </row>
     <row r="78" spans="1:1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A78" s="7" t="s">
-        <v>428</v>
+        <v>426</v>
       </c>
     </row>
     <row r="79" spans="1:1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A79" s="7" t="s">
-        <v>429</v>
+        <v>427</v>
       </c>
     </row>
     <row r="80" spans="1:1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A80" s="7" t="s">
-        <v>430</v>
+        <v>428</v>
       </c>
     </row>
     <row r="81" spans="1:1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A81" s="7" t="s">
-        <v>431</v>
+        <v>429</v>
       </c>
     </row>
     <row r="82" spans="1:1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A82" s="7" t="s">
-        <v>432</v>
+        <v>430</v>
       </c>
     </row>
     <row r="83" spans="1:1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A83" s="7" t="s">
-        <v>433</v>
+        <v>431</v>
       </c>
     </row>
     <row r="84" spans="1:1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A84" s="7" t="s">
-        <v>434</v>
+        <v>432</v>
       </c>
     </row>
     <row r="85" spans="1:1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A85" s="7" t="s">
-        <v>435</v>
+        <v>433</v>
       </c>
     </row>
     <row r="86" spans="1:1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A86" s="7" t="s">
-        <v>436</v>
+        <v>434</v>
       </c>
     </row>
     <row r="87" spans="1:1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A87" s="7" t="s">
-        <v>437</v>
+        <v>435</v>
       </c>
     </row>
     <row r="88" spans="1:1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A88" s="7" t="s">
-        <v>438</v>
+        <v>436</v>
       </c>
     </row>
     <row r="89" spans="1:1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A89" s="7" t="s">
-        <v>439</v>
+        <v>437</v>
       </c>
     </row>
     <row r="90" spans="1:1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A90" s="7" t="s">
-        <v>440</v>
+        <v>438</v>
       </c>
     </row>
     <row r="91" spans="1:1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A91" s="7" t="s">
-        <v>441</v>
+        <v>439</v>
       </c>
     </row>
     <row r="92" spans="1:1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A92" s="7" t="s">
-        <v>442</v>
+        <v>440</v>
       </c>
     </row>
     <row r="93" spans="1:1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A93" s="7" t="s">
-        <v>443</v>
+        <v>441</v>
       </c>
     </row>
     <row r="94" spans="1:1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A94" s="7" t="s">
-        <v>444</v>
+        <v>442</v>
       </c>
     </row>
     <row r="95" spans="1:1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A95" s="7" t="s">
-        <v>445</v>
+        <v>443</v>
       </c>
     </row>
     <row r="96" spans="1:1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A96" s="7" t="s">
-        <v>446</v>
+        <v>444</v>
       </c>
     </row>
     <row r="97" spans="1:1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A97" s="7" t="s">
-        <v>447</v>
+        <v>445</v>
       </c>
     </row>
     <row r="98" spans="1:1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A98" s="7" t="s">
-        <v>448</v>
+        <v>446</v>
       </c>
     </row>
     <row r="99" spans="1:1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A99" s="7" t="s">
-        <v>449</v>
+        <v>447</v>
       </c>
     </row>
     <row r="100" spans="1:1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A100" s="7" t="s">
-        <v>450</v>
+        <v>448</v>
       </c>
     </row>
     <row r="101" spans="1:1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A101" s="7" t="s">
-        <v>451</v>
+        <v>449</v>
       </c>
     </row>
     <row r="102" spans="1:1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A102" s="7" t="s">
-        <v>452</v>
+        <v>450</v>
       </c>
     </row>
     <row r="103" spans="1:1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A103" s="7" t="s">
-        <v>453</v>
+        <v>451</v>
       </c>
     </row>
     <row r="104" spans="1:1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A104" s="7" t="s">
-        <v>454</v>
+        <v>452</v>
       </c>
     </row>
     <row r="105" spans="1:1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A105" s="7" t="s">
-        <v>455</v>
+        <v>453</v>
       </c>
     </row>
     <row r="106" spans="1:1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A106" s="7" t="s">
-        <v>456</v>
+        <v>454</v>
       </c>
     </row>
     <row r="107" spans="1:1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A107" s="7" t="s">
-        <v>457</v>
+        <v>455</v>
       </c>
     </row>
     <row r="108" spans="1:1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A108" s="7" t="s">
-        <v>458</v>
+        <v>456</v>
       </c>
     </row>
     <row r="109" spans="1:1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A109" s="7" t="s">
-        <v>459</v>
+        <v>457</v>
       </c>
     </row>
     <row r="110" spans="1:1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A110" s="7" t="s">
-        <v>460</v>
+        <v>458</v>
       </c>
     </row>
     <row r="111" spans="1:1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A111" s="7" t="s">
-        <v>461</v>
+        <v>459</v>
       </c>
     </row>
     <row r="112" spans="1:1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A112" s="7" t="s">
-        <v>462</v>
+        <v>460</v>
       </c>
     </row>
     <row r="113" spans="1:1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A113" s="7" t="s">
-        <v>463</v>
+        <v>461</v>
       </c>
     </row>
     <row r="114" spans="1:1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A114" s="7" t="s">
-        <v>464</v>
+        <v>462</v>
       </c>
     </row>
     <row r="115" spans="1:1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A115" s="7" t="s">
-        <v>465</v>
+        <v>463</v>
       </c>
     </row>
     <row r="116" spans="1:1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A116" s="7" t="s">
-        <v>466</v>
+        <v>464</v>
       </c>
     </row>
     <row r="117" spans="1:1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A117" s="7" t="s">
-        <v>467</v>
+        <v>465</v>
       </c>
     </row>
     <row r="118" spans="1:1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A118" s="7" t="s">
-        <v>468</v>
+        <v>466</v>
       </c>
     </row>
     <row r="119" spans="1:1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A119" s="7" t="s">
-        <v>469</v>
+        <v>467</v>
       </c>
     </row>
     <row r="120" spans="1:1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A120" s="7" t="s">
-        <v>470</v>
+        <v>468</v>
       </c>
     </row>
     <row r="121" spans="1:1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A121" s="7" t="s">
-        <v>471</v>
+        <v>469</v>
       </c>
     </row>
     <row r="122" spans="1:1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A122" s="7" t="s">
-        <v>472</v>
+        <v>470</v>
       </c>
     </row>
     <row r="123" spans="1:1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A123" s="7" t="s">
-        <v>473</v>
+        <v>471</v>
       </c>
     </row>
     <row r="124" spans="1:1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A124" s="7" t="s">
-        <v>474</v>
+        <v>472</v>
       </c>
     </row>
     <row r="125" spans="1:1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A125" s="7" t="s">
-        <v>475</v>
+        <v>473</v>
       </c>
     </row>
     <row r="126" spans="1:1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A126" s="7" t="s">
-        <v>476</v>
+        <v>474</v>
       </c>
     </row>
     <row r="127" spans="1:1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A127" s="7" t="s">
-        <v>477</v>
+        <v>475</v>
       </c>
     </row>
     <row r="128" spans="1:1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A128" s="7" t="s">
-        <v>478</v>
+        <v>476</v>
       </c>
     </row>
     <row r="129" spans="1:1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A129" s="7" t="s">
-        <v>479</v>
+        <v>477</v>
       </c>
     </row>
     <row r="130" spans="1:1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A130" s="7" t="s">
-        <v>480</v>
+        <v>478</v>
       </c>
     </row>
     <row r="131" spans="1:1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A131" s="7" t="s">
-        <v>481</v>
+        <v>479</v>
       </c>
     </row>
     <row r="132" spans="1:1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A132" s="7" t="s">
-        <v>482</v>
+        <v>480</v>
       </c>
     </row>
     <row r="133" spans="1:1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A133" s="7" t="s">
-        <v>483</v>
+        <v>481</v>
       </c>
     </row>
     <row r="134" spans="1:1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A134" s="7" t="s">
-        <v>484</v>
+        <v>482</v>
       </c>
     </row>
     <row r="135" spans="1:1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A135" s="7" t="s">
-        <v>485</v>
+        <v>483</v>
       </c>
     </row>
     <row r="136" spans="1:1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A136" s="7" t="s">
-        <v>486</v>
+        <v>484</v>
       </c>
     </row>
     <row r="137" spans="1:1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A137" s="7" t="s">
-        <v>487</v>
+        <v>485</v>
       </c>
     </row>
     <row r="138" spans="1:1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A138" s="7" t="s">
-        <v>488</v>
+        <v>486</v>
       </c>
     </row>
     <row r="139" spans="1:1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A139" s="7" t="s">
-        <v>489</v>
+        <v>487</v>
       </c>
     </row>
     <row r="140" spans="1:1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A140" s="7" t="s">
-        <v>490</v>
+        <v>488</v>
       </c>
     </row>
     <row r="141" spans="1:1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A141" s="7" t="s">
-        <v>491</v>
+        <v>489</v>
       </c>
     </row>
     <row r="142" spans="1:1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A142" s="7" t="s">
-        <v>492</v>
+        <v>490</v>
       </c>
     </row>
     <row r="143" spans="1:1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A143" s="7" t="s">
-        <v>493</v>
+        <v>491</v>
       </c>
     </row>
     <row r="144" spans="1:1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A144" s="7" t="s">
-        <v>494</v>
+        <v>492</v>
       </c>
     </row>
     <row r="145" spans="1:1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A145" s="7" t="s">
-        <v>495</v>
+        <v>493</v>
       </c>
     </row>
     <row r="146" spans="1:1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A146" s="7" t="s">
-        <v>496</v>
+        <v>494</v>
       </c>
     </row>
     <row r="147" spans="1:1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A147" s="7" t="s">
-        <v>497</v>
+        <v>495</v>
       </c>
     </row>
     <row r="148" spans="1:1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A148" s="7" t="s">
-        <v>498</v>
+        <v>496</v>
       </c>
     </row>
     <row r="149" spans="1:1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A149" s="7" t="s">
-        <v>499</v>
+        <v>497</v>
       </c>
     </row>
     <row r="150" spans="1:1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A150" s="7" t="s">
-        <v>500</v>
+        <v>498</v>
       </c>
     </row>
     <row r="151" spans="1:1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A151" s="7" t="s">
-        <v>501</v>
+        <v>499</v>
       </c>
     </row>
     <row r="152" spans="1:1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A152" s="7" t="s">
-        <v>502</v>
+        <v>500</v>
       </c>
     </row>
     <row r="153" spans="1:1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A153" s="7" t="s">
-        <v>503</v>
+        <v>501</v>
       </c>
     </row>
     <row r="154" spans="1:1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A154" s="7" t="s">
-        <v>504</v>
+        <v>502</v>
       </c>
     </row>
     <row r="155" spans="1:1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A155" s="7" t="s">
-        <v>505</v>
+        <v>503</v>
       </c>
     </row>
     <row r="156" spans="1:1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A156" s="7" t="s">
-        <v>506</v>
+        <v>504</v>
       </c>
     </row>
     <row r="157" spans="1:1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A157" s="7" t="s">
-        <v>507</v>
+        <v>505</v>
       </c>
     </row>
     <row r="158" spans="1:1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A158" s="7" t="s">
-        <v>508</v>
+        <v>506</v>
       </c>
     </row>
     <row r="159" spans="1:1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A159" s="7" t="s">
-        <v>509</v>
+        <v>507</v>
       </c>
     </row>
     <row r="160" spans="1:1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A160" s="7" t="s">
-        <v>510</v>
+        <v>508</v>
       </c>
     </row>
     <row r="161" spans="1:1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A161" s="7" t="s">
-        <v>511</v>
+        <v>509</v>
       </c>
     </row>
     <row r="162" spans="1:1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A162" s="7" t="s">
-        <v>512</v>
+        <v>510</v>
       </c>
     </row>
     <row r="163" spans="1:1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A163" s="7" t="s">
-        <v>513</v>
+        <v>511</v>
       </c>
     </row>
     <row r="164" spans="1:1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A164" s="7" t="s">
-        <v>371</v>
+        <v>369</v>
       </c>
     </row>
     <row r="165" spans="1:1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A165" s="7" t="s">
-        <v>370</v>
+        <v>368</v>
       </c>
     </row>
     <row r="166" spans="1:1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A166" s="7" t="s">
-        <v>514</v>
+        <v>512</v>
       </c>
     </row>
     <row r="167" spans="1:1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A167" s="7" t="s">
-        <v>515</v>
+        <v>513</v>
       </c>
     </row>
     <row r="168" spans="1:1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A168" s="7" t="s">
-        <v>516</v>
+        <v>514</v>
       </c>
     </row>
     <row r="169" spans="1:1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A169" s="7" t="s">
-        <v>517</v>
+        <v>515</v>
       </c>
     </row>
     <row r="170" spans="1:1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A170" s="7" t="s">
-        <v>518</v>
+        <v>516</v>
       </c>
     </row>
     <row r="171" spans="1:1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A171" s="7" t="s">
-        <v>519</v>
+        <v>517</v>
       </c>
     </row>
     <row r="172" spans="1:1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A172" s="7" t="s">
-        <v>520</v>
+        <v>518</v>
       </c>
     </row>
     <row r="173" spans="1:1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A173" s="7" t="s">
-        <v>521</v>
+        <v>519</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Updated packet list. Fixed Manifest files. Rewrote Server and ClientPacket. Renamed bat to .bat instead of .exe.bat.
</commit_message>
<xml_diff>
--- a/Miscellaneous/Packets.xlsx
+++ b/Miscellaneous/Packets.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="16380" windowHeight="8190" tabRatio="947"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="16380" windowHeight="8190" tabRatio="947" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Server TCP" sheetId="1" r:id="rId1"/>
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="969" uniqueCount="532">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="979" uniqueCount="536">
   <si>
     <t>Message ID</t>
   </si>
@@ -917,9 +917,6 @@
     <t>le</t>
   </si>
   <si>
-    <t>Error Packet</t>
-  </si>
-  <si>
     <t>l1</t>
   </si>
   <si>
@@ -1617,6 +1614,21 @@
   </si>
   <si>
     <t>Notify Clients</t>
+  </si>
+  <si>
+    <t>98</t>
+  </si>
+  <si>
+    <t>Can't Use Item</t>
+  </si>
+  <si>
+    <t>99</t>
+  </si>
+  <si>
+    <t>BattleFrontier Event</t>
+  </si>
+  <si>
+    <t>Username or Password Wrong</t>
   </si>
 </sst>
 </file>
@@ -1953,8 +1965,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G68"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A26" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="D43" sqref="D43"/>
+    <sheetView topLeftCell="A46" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="D41" sqref="D41"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2501,13 +2513,13 @@
     </row>
     <row r="30" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A30" s="2" t="s">
-        <v>530</v>
+        <v>529</v>
       </c>
       <c r="B30" s="2" t="s">
         <v>68</v>
       </c>
       <c r="C30" s="2" t="s">
-        <v>531</v>
+        <v>530</v>
       </c>
       <c r="D30" s="2"/>
       <c r="E30" s="2" t="s">
@@ -3129,13 +3141,13 @@
     </row>
     <row r="64" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A64" s="2" t="s">
-        <v>529</v>
+        <v>528</v>
       </c>
       <c r="B64" s="2" t="s">
         <v>67</v>
       </c>
       <c r="C64" s="2" t="s">
-        <v>528</v>
+        <v>527</v>
       </c>
       <c r="D64" s="2"/>
       <c r="E64" s="2" t="s">
@@ -3147,13 +3159,13 @@
     </row>
     <row r="65" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A65" s="4" t="s">
-        <v>520</v>
+        <v>519</v>
       </c>
       <c r="B65" s="4" t="s">
         <v>67</v>
       </c>
       <c r="C65" s="4" t="s">
-        <v>349</v>
+        <v>348</v>
       </c>
       <c r="D65" s="5"/>
       <c r="E65" s="4" t="s">
@@ -3165,13 +3177,13 @@
     </row>
     <row r="66" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A66" s="4" t="s">
-        <v>521</v>
+        <v>520</v>
       </c>
       <c r="B66" s="4" t="s">
         <v>67</v>
       </c>
       <c r="C66" s="4" t="s">
-        <v>522</v>
+        <v>521</v>
       </c>
       <c r="D66" s="5"/>
       <c r="E66" s="4" t="s">
@@ -3183,13 +3195,13 @@
     </row>
     <row r="67" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A67" s="4" t="s">
-        <v>523</v>
+        <v>522</v>
       </c>
       <c r="B67" s="4" t="s">
         <v>67</v>
       </c>
       <c r="C67" s="4" t="s">
-        <v>526</v>
+        <v>525</v>
       </c>
       <c r="D67" s="5"/>
       <c r="E67" s="4" t="s">
@@ -3201,13 +3213,13 @@
     </row>
     <row r="68" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A68" s="4" t="s">
-        <v>525</v>
+        <v>524</v>
       </c>
       <c r="B68" s="4" t="s">
         <v>67</v>
       </c>
       <c r="C68" s="4" t="s">
-        <v>524</v>
+        <v>523</v>
       </c>
       <c r="D68" s="5"/>
       <c r="E68" s="4" t="s">
@@ -3225,10 +3237,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:AMK122"/>
+  <dimension ref="A1:AMK124"/>
   <sheetViews>
-    <sheetView topLeftCell="A11" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C29" sqref="C29"/>
+    <sheetView tabSelected="1" topLeftCell="A81" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="C92" sqref="C92"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4338,19 +4350,19 @@
       </c>
     </row>
     <row r="65" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A65" s="6">
-        <v>57</v>
-      </c>
-      <c r="B65" s="2" t="s">
-        <v>249</v>
-      </c>
-      <c r="C65" s="2" t="s">
-        <v>250</v>
-      </c>
-      <c r="E65" s="2" t="s">
-        <v>138</v>
-      </c>
-      <c r="F65" s="2" t="s">
+      <c r="A65" s="3" t="s">
+        <v>520</v>
+      </c>
+      <c r="B65" s="4" t="s">
+        <v>67</v>
+      </c>
+      <c r="C65" s="4" t="s">
+        <v>526</v>
+      </c>
+      <c r="E65" s="4" t="s">
+        <v>138</v>
+      </c>
+      <c r="F65" s="5" t="s">
         <v>15</v>
       </c>
     </row>
@@ -4359,10 +4371,10 @@
         <v>57</v>
       </c>
       <c r="B66" s="2" t="s">
-        <v>251</v>
+        <v>249</v>
       </c>
       <c r="C66" s="2" t="s">
-        <v>85</v>
+        <v>250</v>
       </c>
       <c r="E66" s="2" t="s">
         <v>138</v>
@@ -4376,10 +4388,10 @@
         <v>57</v>
       </c>
       <c r="B67" s="2" t="s">
-        <v>252</v>
+        <v>251</v>
       </c>
       <c r="C67" s="2" t="s">
-        <v>253</v>
+        <v>85</v>
       </c>
       <c r="E67" s="2" t="s">
         <v>138</v>
@@ -4393,10 +4405,10 @@
         <v>57</v>
       </c>
       <c r="B68" s="2" t="s">
-        <v>254</v>
+        <v>252</v>
       </c>
       <c r="C68" s="2" t="s">
-        <v>91</v>
+        <v>253</v>
       </c>
       <c r="E68" s="2" t="s">
         <v>138</v>
@@ -4410,10 +4422,10 @@
         <v>57</v>
       </c>
       <c r="B69" s="2" t="s">
-        <v>255</v>
+        <v>254</v>
       </c>
       <c r="C69" s="2" t="s">
-        <v>94</v>
+        <v>91</v>
       </c>
       <c r="E69" s="2" t="s">
         <v>138</v>
@@ -4424,13 +4436,13 @@
     </row>
     <row r="70" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A70" s="6">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="B70" s="2" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="C70" s="2" t="s">
-        <v>257</v>
+        <v>94</v>
       </c>
       <c r="E70" s="2" t="s">
         <v>138</v>
@@ -4441,16 +4453,13 @@
     </row>
     <row r="71" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A71" s="6">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="B71" s="2" t="s">
-        <v>258</v>
+        <v>256</v>
       </c>
       <c r="C71" s="2" t="s">
-        <v>259</v>
-      </c>
-      <c r="D71" s="2" t="s">
-        <v>14</v>
+        <v>257</v>
       </c>
       <c r="E71" s="2" t="s">
         <v>138</v>
@@ -4461,13 +4470,13 @@
     </row>
     <row r="72" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A72" s="6">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="B72" s="2" t="s">
-        <v>260</v>
+        <v>258</v>
       </c>
       <c r="C72" s="2" t="s">
-        <v>261</v>
+        <v>259</v>
       </c>
       <c r="D72" s="2" t="s">
         <v>14</v>
@@ -4481,13 +4490,13 @@
     </row>
     <row r="73" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A73" s="6">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="B73" s="2" t="s">
-        <v>262</v>
+        <v>260</v>
       </c>
       <c r="C73" s="2" t="s">
-        <v>263</v>
+        <v>261</v>
       </c>
       <c r="D73" s="2" t="s">
         <v>14</v>
@@ -4501,13 +4510,13 @@
     </row>
     <row r="74" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A74" s="6">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="B74" s="2" t="s">
-        <v>264</v>
+        <v>262</v>
       </c>
       <c r="C74" s="2" t="s">
-        <v>265</v>
+        <v>263</v>
       </c>
       <c r="D74" s="2" t="s">
         <v>14</v>
@@ -4521,13 +4530,16 @@
     </row>
     <row r="75" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A75" s="6">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="B75" s="2" t="s">
-        <v>266</v>
+        <v>264</v>
       </c>
       <c r="C75" s="2" t="s">
-        <v>267</v>
+        <v>265</v>
+      </c>
+      <c r="D75" s="2" t="s">
+        <v>14</v>
       </c>
       <c r="E75" s="2" t="s">
         <v>138</v>
@@ -4538,13 +4550,13 @@
     </row>
     <row r="76" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A76" s="6">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="B76" s="2" t="s">
-        <v>18</v>
+        <v>266</v>
       </c>
       <c r="C76" s="2" t="s">
-        <v>268</v>
+        <v>267</v>
       </c>
       <c r="E76" s="2" t="s">
         <v>138</v>
@@ -4555,13 +4567,13 @@
     </row>
     <row r="77" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A77" s="6">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="B77" s="2" t="s">
-        <v>269</v>
+        <v>18</v>
       </c>
       <c r="C77" s="2" t="s">
-        <v>270</v>
+        <v>268</v>
       </c>
       <c r="E77" s="2" t="s">
         <v>138</v>
@@ -4572,13 +4584,13 @@
     </row>
     <row r="78" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A78" s="6">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="B78" s="2" t="s">
-        <v>271</v>
+        <v>269</v>
       </c>
       <c r="C78" s="2" t="s">
-        <v>272</v>
+        <v>270</v>
       </c>
       <c r="E78" s="2" t="s">
         <v>138</v>
@@ -4589,13 +4601,13 @@
     </row>
     <row r="79" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A79" s="6">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="B79" s="2" t="s">
-        <v>273</v>
+        <v>271</v>
       </c>
       <c r="C79" s="2" t="s">
-        <v>274</v>
+        <v>272</v>
       </c>
       <c r="E79" s="2" t="s">
         <v>138</v>
@@ -4606,13 +4618,13 @@
     </row>
     <row r="80" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A80" s="6">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="B80" s="2" t="s">
-        <v>275</v>
+        <v>273</v>
       </c>
       <c r="C80" s="2" t="s">
-        <v>276</v>
+        <v>274</v>
       </c>
       <c r="E80" s="2" t="s">
         <v>138</v>
@@ -4623,13 +4635,13 @@
     </row>
     <row r="81" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A81" s="6">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="B81" s="2" t="s">
-        <v>277</v>
+        <v>275</v>
       </c>
       <c r="C81" s="2" t="s">
-        <v>278</v>
+        <v>276</v>
       </c>
       <c r="E81" s="2" t="s">
         <v>138</v>
@@ -4640,30 +4652,30 @@
     </row>
     <row r="82" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A82" s="6">
+        <v>69</v>
+      </c>
+      <c r="B82" s="2" t="s">
+        <v>277</v>
+      </c>
+      <c r="C82" s="2" t="s">
+        <v>278</v>
+      </c>
+      <c r="E82" s="2" t="s">
+        <v>138</v>
+      </c>
+      <c r="F82" s="2" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="83" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A83" s="6">
         <v>70</v>
       </c>
-      <c r="B82" s="2" t="s">
+      <c r="B83" s="2" t="s">
         <v>279</v>
       </c>
-      <c r="C82" s="2" t="s">
+      <c r="C83" s="2" t="s">
         <v>280</v>
-      </c>
-      <c r="E82" s="2" t="s">
-        <v>138</v>
-      </c>
-      <c r="F82" s="2" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="83" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A83" s="6" t="s">
-        <v>67</v>
-      </c>
-      <c r="B83" s="2" t="s">
-        <v>281</v>
-      </c>
-      <c r="C83" s="2" t="s">
-        <v>282</v>
       </c>
       <c r="E83" s="2" t="s">
         <v>138</v>
@@ -4677,27 +4689,27 @@
         <v>67</v>
       </c>
       <c r="B84" s="2" t="s">
+        <v>281</v>
+      </c>
+      <c r="C84" s="2" t="s">
+        <v>282</v>
+      </c>
+      <c r="E84" s="2" t="s">
+        <v>138</v>
+      </c>
+      <c r="F84" s="2" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="85" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A85" s="6" t="s">
+        <v>67</v>
+      </c>
+      <c r="B85" s="2" t="s">
         <v>283</v>
       </c>
-      <c r="C84" s="2" t="s">
+      <c r="C85" s="2" t="s">
         <v>284</v>
-      </c>
-      <c r="E84" s="2" t="s">
-        <v>138</v>
-      </c>
-      <c r="F84" s="2" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="85" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A85" s="6">
-        <v>71</v>
-      </c>
-      <c r="B85" s="2" t="s">
-        <v>285</v>
-      </c>
-      <c r="C85" s="2" t="s">
-        <v>286</v>
       </c>
       <c r="E85" s="2" t="s">
         <v>138</v>
@@ -4708,13 +4720,13 @@
     </row>
     <row r="86" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A86" s="6">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="B86" s="2" t="s">
-        <v>287</v>
+        <v>285</v>
       </c>
       <c r="C86" s="2" t="s">
-        <v>288</v>
+        <v>286</v>
       </c>
       <c r="E86" s="2" t="s">
         <v>138</v>
@@ -4725,13 +4737,13 @@
     </row>
     <row r="87" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A87" s="6">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="B87" s="2" t="s">
-        <v>289</v>
+        <v>287</v>
       </c>
       <c r="C87" s="2" t="s">
-        <v>290</v>
+        <v>288</v>
       </c>
       <c r="E87" s="2" t="s">
         <v>138</v>
@@ -4745,10 +4757,10 @@
         <v>73</v>
       </c>
       <c r="B88" s="2" t="s">
-        <v>291</v>
+        <v>289</v>
       </c>
       <c r="C88" s="2" t="s">
-        <v>292</v>
+        <v>290</v>
       </c>
       <c r="E88" s="2" t="s">
         <v>138</v>
@@ -4759,13 +4771,13 @@
     </row>
     <row r="89" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A89" s="6">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="B89" s="2" t="s">
-        <v>293</v>
+        <v>291</v>
       </c>
       <c r="C89" s="2" t="s">
-        <v>294</v>
+        <v>292</v>
       </c>
       <c r="E89" s="2" t="s">
         <v>138</v>
@@ -4776,13 +4788,13 @@
     </row>
     <row r="90" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A90" s="6">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="B90" s="2" t="s">
-        <v>295</v>
+        <v>293</v>
       </c>
       <c r="C90" s="2" t="s">
-        <v>296</v>
+        <v>294</v>
       </c>
       <c r="E90" s="2" t="s">
         <v>138</v>
@@ -4793,13 +4805,13 @@
     </row>
     <row r="91" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A91" s="6">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="B91" s="2" t="s">
-        <v>297</v>
+        <v>295</v>
       </c>
       <c r="C91" s="2" t="s">
-        <v>298</v>
+        <v>296</v>
       </c>
       <c r="E91" s="2" t="s">
         <v>138</v>
@@ -4810,13 +4822,13 @@
     </row>
     <row r="92" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A92" s="6">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="B92" s="2" t="s">
-        <v>299</v>
+        <v>297</v>
       </c>
       <c r="C92" s="2" t="s">
-        <v>300</v>
+        <v>535</v>
       </c>
       <c r="E92" s="2" t="s">
         <v>138</v>
@@ -4827,30 +4839,30 @@
     </row>
     <row r="93" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A93" s="6">
+        <v>77</v>
+      </c>
+      <c r="B93" s="2" t="s">
+        <v>298</v>
+      </c>
+      <c r="C93" s="2" t="s">
+        <v>299</v>
+      </c>
+      <c r="E93" s="2" t="s">
+        <v>138</v>
+      </c>
+      <c r="F93" s="2" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="94" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A94" s="6">
         <v>78</v>
       </c>
-      <c r="B93" s="2" t="s">
+      <c r="B94" s="2" t="s">
+        <v>300</v>
+      </c>
+      <c r="C94" s="2" t="s">
         <v>301</v>
-      </c>
-      <c r="C93" s="2" t="s">
-        <v>302</v>
-      </c>
-      <c r="E93" s="2" t="s">
-        <v>138</v>
-      </c>
-      <c r="F93" s="2" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="94" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A94" s="6" t="s">
-        <v>303</v>
-      </c>
-      <c r="B94" s="2" t="s">
-        <v>304</v>
-      </c>
-      <c r="C94" s="2" t="s">
-        <v>305</v>
       </c>
       <c r="E94" s="2" t="s">
         <v>138</v>
@@ -4864,10 +4876,10 @@
         <v>79</v>
       </c>
       <c r="B95" s="2" t="s">
+        <v>305</v>
+      </c>
+      <c r="C95" s="2" t="s">
         <v>306</v>
-      </c>
-      <c r="C95" s="2" t="s">
-        <v>307</v>
       </c>
       <c r="E95" s="2" t="s">
         <v>138</v>
@@ -4881,10 +4893,10 @@
         <v>80</v>
       </c>
       <c r="B96" s="2" t="s">
+        <v>307</v>
+      </c>
+      <c r="C96" s="2" t="s">
         <v>308</v>
-      </c>
-      <c r="C96" s="2" t="s">
-        <v>309</v>
       </c>
       <c r="E96" s="2" t="s">
         <v>138</v>
@@ -4898,10 +4910,10 @@
         <v>81</v>
       </c>
       <c r="B97" s="2" t="s">
+        <v>309</v>
+      </c>
+      <c r="C97" s="2" t="s">
         <v>310</v>
-      </c>
-      <c r="C97" s="2" t="s">
-        <v>311</v>
       </c>
       <c r="E97" s="2" t="s">
         <v>138</v>
@@ -4915,10 +4927,10 @@
         <v>82</v>
       </c>
       <c r="B98" s="2" t="s">
+        <v>311</v>
+      </c>
+      <c r="C98" s="2" t="s">
         <v>312</v>
-      </c>
-      <c r="C98" s="2" t="s">
-        <v>313</v>
       </c>
       <c r="E98" s="2" t="s">
         <v>138</v>
@@ -4932,10 +4944,10 @@
         <v>82</v>
       </c>
       <c r="B99" s="2" t="s">
+        <v>313</v>
+      </c>
+      <c r="C99" s="2" t="s">
         <v>314</v>
-      </c>
-      <c r="C99" s="2" t="s">
-        <v>315</v>
       </c>
       <c r="E99" s="2" t="s">
         <v>138</v>
@@ -4949,10 +4961,10 @@
         <v>82</v>
       </c>
       <c r="B100" s="2" t="s">
+        <v>315</v>
+      </c>
+      <c r="C100" s="2" t="s">
         <v>316</v>
-      </c>
-      <c r="C100" s="2" t="s">
-        <v>317</v>
       </c>
       <c r="E100" s="2" t="s">
         <v>138</v>
@@ -4966,10 +4978,10 @@
         <v>82</v>
       </c>
       <c r="B101" s="2" t="s">
+        <v>317</v>
+      </c>
+      <c r="C101" s="2" t="s">
         <v>318</v>
-      </c>
-      <c r="C101" s="2" t="s">
-        <v>319</v>
       </c>
       <c r="E101" s="2" t="s">
         <v>138</v>
@@ -4983,10 +4995,10 @@
         <v>82</v>
       </c>
       <c r="B102" s="2" t="s">
+        <v>319</v>
+      </c>
+      <c r="C102" s="2" t="s">
         <v>320</v>
-      </c>
-      <c r="C102" s="2" t="s">
-        <v>321</v>
       </c>
       <c r="E102" s="2" t="s">
         <v>138</v>
@@ -5037,7 +5049,7 @@
         <v>52</v>
       </c>
       <c r="C105" s="2" t="s">
-        <v>322</v>
+        <v>321</v>
       </c>
       <c r="E105" s="2" t="s">
         <v>138</v>
@@ -5051,10 +5063,10 @@
         <v>86</v>
       </c>
       <c r="B106" s="2" t="s">
+        <v>322</v>
+      </c>
+      <c r="C106" s="2" t="s">
         <v>323</v>
-      </c>
-      <c r="C106" s="2" t="s">
-        <v>324</v>
       </c>
       <c r="E106" s="2" t="s">
         <v>138</v>
@@ -5068,10 +5080,10 @@
         <v>87</v>
       </c>
       <c r="B107" s="2" t="s">
-        <v>325</v>
+        <v>324</v>
       </c>
       <c r="C107" s="2" t="s">
-        <v>300</v>
+        <v>299</v>
       </c>
       <c r="E107" s="2" t="s">
         <v>138</v>
@@ -5085,10 +5097,10 @@
         <v>87</v>
       </c>
       <c r="B108" s="2" t="s">
+        <v>325</v>
+      </c>
+      <c r="C108" s="2" t="s">
         <v>326</v>
-      </c>
-      <c r="C108" s="2" t="s">
-        <v>327</v>
       </c>
       <c r="E108" s="2" t="s">
         <v>138</v>
@@ -5102,10 +5114,10 @@
         <v>87</v>
       </c>
       <c r="B109" s="2" t="s">
+        <v>327</v>
+      </c>
+      <c r="C109" s="2" t="s">
         <v>328</v>
-      </c>
-      <c r="C109" s="2" t="s">
-        <v>329</v>
       </c>
       <c r="E109" s="2" t="s">
         <v>138</v>
@@ -5119,10 +5131,10 @@
         <v>87</v>
       </c>
       <c r="B110" s="2" t="s">
+        <v>329</v>
+      </c>
+      <c r="C110" s="2" t="s">
         <v>330</v>
-      </c>
-      <c r="C110" s="2" t="s">
-        <v>331</v>
       </c>
       <c r="E110" s="2" t="s">
         <v>138</v>
@@ -5136,10 +5148,10 @@
         <v>87</v>
       </c>
       <c r="B111" s="2" t="s">
+        <v>331</v>
+      </c>
+      <c r="C111" s="2" t="s">
         <v>332</v>
-      </c>
-      <c r="C111" s="2" t="s">
-        <v>333</v>
       </c>
       <c r="E111" s="2" t="s">
         <v>138</v>
@@ -5153,10 +5165,10 @@
         <v>87</v>
       </c>
       <c r="B112" s="2" t="s">
+        <v>333</v>
+      </c>
+      <c r="C112" s="2" t="s">
         <v>334</v>
-      </c>
-      <c r="C112" s="2" t="s">
-        <v>335</v>
       </c>
       <c r="E112" s="2" t="s">
         <v>138</v>
@@ -5170,10 +5182,10 @@
         <v>88</v>
       </c>
       <c r="B113" s="2" t="s">
+        <v>335</v>
+      </c>
+      <c r="C113" s="2" t="s">
         <v>336</v>
-      </c>
-      <c r="C113" s="2" t="s">
-        <v>337</v>
       </c>
       <c r="E113" s="2" t="s">
         <v>138</v>
@@ -5187,10 +5199,10 @@
         <v>89</v>
       </c>
       <c r="B114" s="2" t="s">
+        <v>337</v>
+      </c>
+      <c r="C114" s="2" t="s">
         <v>338</v>
-      </c>
-      <c r="C114" s="2" t="s">
-        <v>339</v>
       </c>
       <c r="E114" s="2" t="s">
         <v>138</v>
@@ -5204,11 +5216,11 @@
         <v>90</v>
       </c>
       <c r="B115" s="2" t="s">
+        <v>339</v>
+      </c>
+      <c r="C115" s="2" t="s">
         <v>340</v>
       </c>
-      <c r="C115" s="2" t="s">
-        <v>341</v>
-      </c>
       <c r="E115" s="2" t="s">
         <v>138</v>
       </c>
@@ -5216,15 +5228,15 @@
         <v>15</v>
       </c>
     </row>
-    <row r="116" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="116" spans="1:6" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A116" s="6">
         <v>91</v>
       </c>
       <c r="B116" s="2" t="s">
+        <v>341</v>
+      </c>
+      <c r="C116" s="2" t="s">
         <v>342</v>
-      </c>
-      <c r="C116" s="2" t="s">
-        <v>343</v>
       </c>
       <c r="E116" s="2" t="s">
         <v>138</v>
@@ -5238,10 +5250,10 @@
         <v>92</v>
       </c>
       <c r="B117" s="2" t="s">
+        <v>343</v>
+      </c>
+      <c r="C117" s="2" t="s">
         <v>344</v>
-      </c>
-      <c r="C117" s="2" t="s">
-        <v>345</v>
       </c>
       <c r="E117" s="2" t="s">
         <v>138</v>
@@ -5258,7 +5270,7 @@
         <v>67</v>
       </c>
       <c r="C118" s="5" t="s">
-        <v>346</v>
+        <v>345</v>
       </c>
       <c r="E118" s="2" t="s">
         <v>138</v>
@@ -5275,7 +5287,7 @@
         <v>67</v>
       </c>
       <c r="C119" s="5" t="s">
-        <v>347</v>
+        <v>346</v>
       </c>
       <c r="E119" s="2" t="s">
         <v>138</v>
@@ -5292,7 +5304,7 @@
         <v>67</v>
       </c>
       <c r="C120" s="4" t="s">
-        <v>348</v>
+        <v>347</v>
       </c>
       <c r="E120" s="2" t="s">
         <v>138</v>
@@ -5301,7 +5313,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="121" spans="1:6" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="121" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A121" s="3">
         <v>96</v>
       </c>
@@ -5309,7 +5321,7 @@
         <v>67</v>
       </c>
       <c r="C121" s="4" t="s">
-        <v>349</v>
+        <v>348</v>
       </c>
       <c r="E121" s="2" t="s">
         <v>138</v>
@@ -5319,19 +5331,53 @@
       </c>
     </row>
     <row r="122" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A122" s="3" t="s">
-        <v>521</v>
-      </c>
-      <c r="B122" s="4" t="s">
+      <c r="A122" s="6" t="s">
+        <v>302</v>
+      </c>
+      <c r="B122" s="2" t="s">
+        <v>303</v>
+      </c>
+      <c r="C122" s="2" t="s">
+        <v>304</v>
+      </c>
+      <c r="E122" s="2" t="s">
+        <v>138</v>
+      </c>
+      <c r="F122" s="2" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="123" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A123" s="3" t="s">
+        <v>531</v>
+      </c>
+      <c r="B123" s="4" t="s">
         <v>67</v>
       </c>
-      <c r="C122" s="4" t="s">
-        <v>527</v>
-      </c>
-      <c r="E122" s="4" t="s">
-        <v>138</v>
-      </c>
-      <c r="F122" s="5" t="s">
+      <c r="C123" s="4" t="s">
+        <v>532</v>
+      </c>
+      <c r="E123" s="4" t="s">
+        <v>138</v>
+      </c>
+      <c r="F123" s="5" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="124" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A124" s="3" t="s">
+        <v>533</v>
+      </c>
+      <c r="B124" s="4" t="s">
+        <v>67</v>
+      </c>
+      <c r="C124" s="4" t="s">
+        <v>534</v>
+      </c>
+      <c r="E124" s="4" t="s">
+        <v>138</v>
+      </c>
+      <c r="F124" s="5" t="s">
         <v>15</v>
       </c>
     </row>
@@ -5357,862 +5403,862 @@
   <sheetData>
     <row r="1" spans="1:1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="7" t="s">
-        <v>350</v>
+        <v>349</v>
       </c>
     </row>
     <row r="2" spans="1:1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="7" t="s">
-        <v>351</v>
+        <v>350</v>
       </c>
     </row>
     <row r="3" spans="1:1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="7" t="s">
-        <v>352</v>
+        <v>351</v>
       </c>
     </row>
     <row r="4" spans="1:1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="7" t="s">
-        <v>353</v>
+        <v>352</v>
       </c>
     </row>
     <row r="5" spans="1:1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="7" t="s">
-        <v>354</v>
+        <v>353</v>
       </c>
     </row>
     <row r="6" spans="1:1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="7" t="s">
-        <v>355</v>
+        <v>354</v>
       </c>
     </row>
     <row r="7" spans="1:1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="7" t="s">
-        <v>356</v>
+        <v>355</v>
       </c>
     </row>
     <row r="8" spans="1:1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" s="7" t="s">
-        <v>357</v>
+        <v>356</v>
       </c>
     </row>
     <row r="9" spans="1:1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" s="7" t="s">
-        <v>358</v>
+        <v>357</v>
       </c>
     </row>
     <row r="10" spans="1:1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" s="7" t="s">
-        <v>359</v>
+        <v>358</v>
       </c>
     </row>
     <row r="11" spans="1:1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A11" s="7" t="s">
-        <v>360</v>
+        <v>359</v>
       </c>
     </row>
     <row r="12" spans="1:1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A12" s="7" t="s">
-        <v>361</v>
+        <v>360</v>
       </c>
     </row>
     <row r="13" spans="1:1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A13" s="7" t="s">
-        <v>362</v>
+        <v>361</v>
       </c>
     </row>
     <row r="14" spans="1:1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A14" s="7" t="s">
-        <v>363</v>
+        <v>362</v>
       </c>
     </row>
     <row r="15" spans="1:1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A15" s="7" t="s">
-        <v>364</v>
+        <v>363</v>
       </c>
     </row>
     <row r="16" spans="1:1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A16" s="7" t="s">
-        <v>365</v>
+        <v>364</v>
       </c>
     </row>
     <row r="17" spans="1:1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A17" s="7" t="s">
-        <v>366</v>
+        <v>365</v>
       </c>
     </row>
     <row r="18" spans="1:1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A18" s="7" t="s">
-        <v>367</v>
+        <v>366</v>
       </c>
     </row>
     <row r="19" spans="1:1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A19" s="7" t="s">
-        <v>368</v>
+        <v>367</v>
       </c>
     </row>
     <row r="20" spans="1:1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A20" s="7" t="s">
-        <v>369</v>
+        <v>368</v>
       </c>
     </row>
     <row r="21" spans="1:1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A21" s="7" t="s">
-        <v>370</v>
+        <v>369</v>
       </c>
     </row>
     <row r="22" spans="1:1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A22" s="7" t="s">
-        <v>371</v>
+        <v>370</v>
       </c>
     </row>
     <row r="23" spans="1:1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A23" s="7" t="s">
-        <v>372</v>
+        <v>371</v>
       </c>
     </row>
     <row r="24" spans="1:1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A24" s="7" t="s">
-        <v>373</v>
+        <v>372</v>
       </c>
     </row>
     <row r="25" spans="1:1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A25" s="7" t="s">
-        <v>374</v>
+        <v>373</v>
       </c>
     </row>
     <row r="26" spans="1:1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A26" s="7" t="s">
-        <v>375</v>
+        <v>374</v>
       </c>
     </row>
     <row r="27" spans="1:1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A27" s="7" t="s">
-        <v>376</v>
+        <v>375</v>
       </c>
     </row>
     <row r="28" spans="1:1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A28" s="7" t="s">
-        <v>377</v>
+        <v>376</v>
       </c>
     </row>
     <row r="29" spans="1:1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A29" s="7" t="s">
-        <v>378</v>
+        <v>377</v>
       </c>
     </row>
     <row r="30" spans="1:1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A30" s="7" t="s">
-        <v>379</v>
+        <v>378</v>
       </c>
     </row>
     <row r="31" spans="1:1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A31" s="7" t="s">
-        <v>380</v>
+        <v>379</v>
       </c>
     </row>
     <row r="32" spans="1:1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A32" s="7" t="s">
-        <v>381</v>
+        <v>380</v>
       </c>
     </row>
     <row r="33" spans="1:1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A33" s="7" t="s">
-        <v>382</v>
+        <v>381</v>
       </c>
     </row>
     <row r="34" spans="1:1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A34" s="7" t="s">
-        <v>383</v>
+        <v>382</v>
       </c>
     </row>
     <row r="35" spans="1:1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A35" s="7" t="s">
-        <v>384</v>
+        <v>383</v>
       </c>
     </row>
     <row r="36" spans="1:1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A36" s="7" t="s">
-        <v>385</v>
+        <v>384</v>
       </c>
     </row>
     <row r="37" spans="1:1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A37" s="7" t="s">
-        <v>386</v>
+        <v>385</v>
       </c>
     </row>
     <row r="38" spans="1:1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A38" s="7" t="s">
-        <v>387</v>
+        <v>386</v>
       </c>
     </row>
     <row r="39" spans="1:1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A39" s="7" t="s">
-        <v>388</v>
+        <v>387</v>
       </c>
     </row>
     <row r="40" spans="1:1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A40" s="7" t="s">
-        <v>389</v>
+        <v>388</v>
       </c>
     </row>
     <row r="41" spans="1:1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A41" s="7" t="s">
-        <v>390</v>
+        <v>389</v>
       </c>
     </row>
     <row r="42" spans="1:1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A42" s="7" t="s">
-        <v>391</v>
+        <v>390</v>
       </c>
     </row>
     <row r="43" spans="1:1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A43" s="7" t="s">
-        <v>392</v>
+        <v>391</v>
       </c>
     </row>
     <row r="44" spans="1:1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A44" s="7" t="s">
-        <v>393</v>
+        <v>392</v>
       </c>
     </row>
     <row r="45" spans="1:1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A45" s="7" t="s">
-        <v>394</v>
+        <v>393</v>
       </c>
     </row>
     <row r="46" spans="1:1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A46" s="7" t="s">
-        <v>395</v>
+        <v>394</v>
       </c>
     </row>
     <row r="47" spans="1:1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A47" s="7" t="s">
-        <v>396</v>
+        <v>395</v>
       </c>
     </row>
     <row r="48" spans="1:1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A48" s="7" t="s">
-        <v>397</v>
+        <v>396</v>
       </c>
     </row>
     <row r="49" spans="1:1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A49" s="7" t="s">
-        <v>398</v>
+        <v>397</v>
       </c>
     </row>
     <row r="50" spans="1:1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A50" s="7" t="s">
-        <v>399</v>
+        <v>398</v>
       </c>
     </row>
     <row r="51" spans="1:1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A51" s="7" t="s">
-        <v>400</v>
+        <v>399</v>
       </c>
     </row>
     <row r="52" spans="1:1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A52" s="7" t="s">
-        <v>401</v>
+        <v>400</v>
       </c>
     </row>
     <row r="53" spans="1:1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A53" s="7" t="s">
-        <v>402</v>
+        <v>401</v>
       </c>
     </row>
     <row r="54" spans="1:1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A54" s="7" t="s">
-        <v>403</v>
+        <v>402</v>
       </c>
     </row>
     <row r="55" spans="1:1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A55" s="7" t="s">
-        <v>404</v>
+        <v>403</v>
       </c>
     </row>
     <row r="56" spans="1:1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A56" s="7" t="s">
-        <v>405</v>
+        <v>404</v>
       </c>
     </row>
     <row r="57" spans="1:1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A57" s="7" t="s">
-        <v>406</v>
+        <v>405</v>
       </c>
     </row>
     <row r="58" spans="1:1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A58" s="7" t="s">
-        <v>407</v>
+        <v>406</v>
       </c>
     </row>
     <row r="60" spans="1:1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A60" s="7" t="s">
-        <v>408</v>
+        <v>407</v>
       </c>
     </row>
     <row r="61" spans="1:1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A61" s="7" t="s">
-        <v>409</v>
+        <v>408</v>
       </c>
     </row>
     <row r="62" spans="1:1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A62" s="7" t="s">
-        <v>410</v>
+        <v>409</v>
       </c>
     </row>
     <row r="63" spans="1:1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A63" s="7" t="s">
-        <v>411</v>
+        <v>410</v>
       </c>
     </row>
     <row r="64" spans="1:1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A64" s="7" t="s">
-        <v>412</v>
+        <v>411</v>
       </c>
     </row>
     <row r="65" spans="1:1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A65" s="7" t="s">
-        <v>413</v>
+        <v>412</v>
       </c>
     </row>
     <row r="66" spans="1:1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A66" s="7" t="s">
-        <v>414</v>
+        <v>413</v>
       </c>
     </row>
     <row r="67" spans="1:1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A67" s="7" t="s">
-        <v>415</v>
+        <v>414</v>
       </c>
     </row>
     <row r="68" spans="1:1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A68" s="7" t="s">
-        <v>416</v>
+        <v>415</v>
       </c>
     </row>
     <row r="69" spans="1:1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A69" s="7" t="s">
-        <v>417</v>
+        <v>416</v>
       </c>
     </row>
     <row r="70" spans="1:1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A70" s="7" t="s">
-        <v>418</v>
+        <v>417</v>
       </c>
     </row>
     <row r="71" spans="1:1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A71" s="7" t="s">
-        <v>419</v>
+        <v>418</v>
       </c>
     </row>
     <row r="72" spans="1:1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A72" s="7" t="s">
-        <v>420</v>
+        <v>419</v>
       </c>
     </row>
     <row r="73" spans="1:1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A73" s="7" t="s">
-        <v>421</v>
+        <v>420</v>
       </c>
     </row>
     <row r="74" spans="1:1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A74" s="7" t="s">
-        <v>422</v>
+        <v>421</v>
       </c>
     </row>
     <row r="75" spans="1:1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A75" s="7" t="s">
-        <v>423</v>
+        <v>422</v>
       </c>
     </row>
     <row r="76" spans="1:1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A76" s="7" t="s">
-        <v>424</v>
+        <v>423</v>
       </c>
     </row>
     <row r="77" spans="1:1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A77" s="7" t="s">
-        <v>425</v>
+        <v>424</v>
       </c>
     </row>
     <row r="78" spans="1:1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A78" s="7" t="s">
-        <v>426</v>
+        <v>425</v>
       </c>
     </row>
     <row r="79" spans="1:1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A79" s="7" t="s">
-        <v>427</v>
+        <v>426</v>
       </c>
     </row>
     <row r="80" spans="1:1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A80" s="7" t="s">
-        <v>428</v>
+        <v>427</v>
       </c>
     </row>
     <row r="81" spans="1:1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A81" s="7" t="s">
-        <v>429</v>
+        <v>428</v>
       </c>
     </row>
     <row r="82" spans="1:1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A82" s="7" t="s">
-        <v>430</v>
+        <v>429</v>
       </c>
     </row>
     <row r="83" spans="1:1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A83" s="7" t="s">
-        <v>431</v>
+        <v>430</v>
       </c>
     </row>
     <row r="84" spans="1:1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A84" s="7" t="s">
-        <v>432</v>
+        <v>431</v>
       </c>
     </row>
     <row r="85" spans="1:1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A85" s="7" t="s">
-        <v>433</v>
+        <v>432</v>
       </c>
     </row>
     <row r="86" spans="1:1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A86" s="7" t="s">
-        <v>434</v>
+        <v>433</v>
       </c>
     </row>
     <row r="87" spans="1:1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A87" s="7" t="s">
-        <v>435</v>
+        <v>434</v>
       </c>
     </row>
     <row r="88" spans="1:1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A88" s="7" t="s">
-        <v>436</v>
+        <v>435</v>
       </c>
     </row>
     <row r="89" spans="1:1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A89" s="7" t="s">
-        <v>437</v>
+        <v>436</v>
       </c>
     </row>
     <row r="90" spans="1:1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A90" s="7" t="s">
-        <v>438</v>
+        <v>437</v>
       </c>
     </row>
     <row r="91" spans="1:1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A91" s="7" t="s">
-        <v>439</v>
+        <v>438</v>
       </c>
     </row>
     <row r="92" spans="1:1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A92" s="7" t="s">
-        <v>440</v>
+        <v>439</v>
       </c>
     </row>
     <row r="93" spans="1:1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A93" s="7" t="s">
-        <v>441</v>
+        <v>440</v>
       </c>
     </row>
     <row r="94" spans="1:1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A94" s="7" t="s">
-        <v>442</v>
+        <v>441</v>
       </c>
     </row>
     <row r="95" spans="1:1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A95" s="7" t="s">
-        <v>443</v>
+        <v>442</v>
       </c>
     </row>
     <row r="96" spans="1:1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A96" s="7" t="s">
-        <v>444</v>
+        <v>443</v>
       </c>
     </row>
     <row r="97" spans="1:1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A97" s="7" t="s">
-        <v>445</v>
+        <v>444</v>
       </c>
     </row>
     <row r="98" spans="1:1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A98" s="7" t="s">
-        <v>446</v>
+        <v>445</v>
       </c>
     </row>
     <row r="99" spans="1:1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A99" s="7" t="s">
-        <v>447</v>
+        <v>446</v>
       </c>
     </row>
     <row r="100" spans="1:1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A100" s="7" t="s">
-        <v>448</v>
+        <v>447</v>
       </c>
     </row>
     <row r="101" spans="1:1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A101" s="7" t="s">
-        <v>449</v>
+        <v>448</v>
       </c>
     </row>
     <row r="102" spans="1:1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A102" s="7" t="s">
-        <v>450</v>
+        <v>449</v>
       </c>
     </row>
     <row r="103" spans="1:1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A103" s="7" t="s">
-        <v>451</v>
+        <v>450</v>
       </c>
     </row>
     <row r="104" spans="1:1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A104" s="7" t="s">
-        <v>452</v>
+        <v>451</v>
       </c>
     </row>
     <row r="105" spans="1:1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A105" s="7" t="s">
-        <v>453</v>
+        <v>452</v>
       </c>
     </row>
     <row r="106" spans="1:1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A106" s="7" t="s">
-        <v>454</v>
+        <v>453</v>
       </c>
     </row>
     <row r="107" spans="1:1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A107" s="7" t="s">
-        <v>455</v>
+        <v>454</v>
       </c>
     </row>
     <row r="108" spans="1:1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A108" s="7" t="s">
-        <v>456</v>
+        <v>455</v>
       </c>
     </row>
     <row r="109" spans="1:1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A109" s="7" t="s">
-        <v>457</v>
+        <v>456</v>
       </c>
     </row>
     <row r="110" spans="1:1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A110" s="7" t="s">
-        <v>458</v>
+        <v>457</v>
       </c>
     </row>
     <row r="111" spans="1:1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A111" s="7" t="s">
-        <v>459</v>
+        <v>458</v>
       </c>
     </row>
     <row r="112" spans="1:1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A112" s="7" t="s">
-        <v>460</v>
+        <v>459</v>
       </c>
     </row>
     <row r="113" spans="1:1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A113" s="7" t="s">
-        <v>461</v>
+        <v>460</v>
       </c>
     </row>
     <row r="114" spans="1:1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A114" s="7" t="s">
-        <v>462</v>
+        <v>461</v>
       </c>
     </row>
     <row r="115" spans="1:1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A115" s="7" t="s">
-        <v>463</v>
+        <v>462</v>
       </c>
     </row>
     <row r="116" spans="1:1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A116" s="7" t="s">
-        <v>464</v>
+        <v>463</v>
       </c>
     </row>
     <row r="117" spans="1:1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A117" s="7" t="s">
-        <v>465</v>
+        <v>464</v>
       </c>
     </row>
     <row r="118" spans="1:1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A118" s="7" t="s">
-        <v>466</v>
+        <v>465</v>
       </c>
     </row>
     <row r="119" spans="1:1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A119" s="7" t="s">
-        <v>467</v>
+        <v>466</v>
       </c>
     </row>
     <row r="120" spans="1:1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A120" s="7" t="s">
-        <v>468</v>
+        <v>467</v>
       </c>
     </row>
     <row r="121" spans="1:1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A121" s="7" t="s">
-        <v>469</v>
+        <v>468</v>
       </c>
     </row>
     <row r="122" spans="1:1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A122" s="7" t="s">
-        <v>470</v>
+        <v>469</v>
       </c>
     </row>
     <row r="123" spans="1:1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A123" s="7" t="s">
-        <v>471</v>
+        <v>470</v>
       </c>
     </row>
     <row r="124" spans="1:1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A124" s="7" t="s">
-        <v>472</v>
+        <v>471</v>
       </c>
     </row>
     <row r="125" spans="1:1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A125" s="7" t="s">
-        <v>473</v>
+        <v>472</v>
       </c>
     </row>
     <row r="126" spans="1:1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A126" s="7" t="s">
-        <v>474</v>
+        <v>473</v>
       </c>
     </row>
     <row r="127" spans="1:1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A127" s="7" t="s">
-        <v>475</v>
+        <v>474</v>
       </c>
     </row>
     <row r="128" spans="1:1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A128" s="7" t="s">
-        <v>476</v>
+        <v>475</v>
       </c>
     </row>
     <row r="129" spans="1:1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A129" s="7" t="s">
-        <v>477</v>
+        <v>476</v>
       </c>
     </row>
     <row r="130" spans="1:1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A130" s="7" t="s">
-        <v>478</v>
+        <v>477</v>
       </c>
     </row>
     <row r="131" spans="1:1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A131" s="7" t="s">
-        <v>479</v>
+        <v>478</v>
       </c>
     </row>
     <row r="132" spans="1:1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A132" s="7" t="s">
-        <v>480</v>
+        <v>479</v>
       </c>
     </row>
     <row r="133" spans="1:1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A133" s="7" t="s">
-        <v>481</v>
+        <v>480</v>
       </c>
     </row>
     <row r="134" spans="1:1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A134" s="7" t="s">
-        <v>482</v>
+        <v>481</v>
       </c>
     </row>
     <row r="135" spans="1:1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A135" s="7" t="s">
-        <v>483</v>
+        <v>482</v>
       </c>
     </row>
     <row r="136" spans="1:1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A136" s="7" t="s">
-        <v>484</v>
+        <v>483</v>
       </c>
     </row>
     <row r="137" spans="1:1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A137" s="7" t="s">
-        <v>485</v>
+        <v>484</v>
       </c>
     </row>
     <row r="138" spans="1:1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A138" s="7" t="s">
-        <v>486</v>
+        <v>485</v>
       </c>
     </row>
     <row r="139" spans="1:1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A139" s="7" t="s">
-        <v>487</v>
+        <v>486</v>
       </c>
     </row>
     <row r="140" spans="1:1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A140" s="7" t="s">
-        <v>488</v>
+        <v>487</v>
       </c>
     </row>
     <row r="141" spans="1:1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A141" s="7" t="s">
-        <v>489</v>
+        <v>488</v>
       </c>
     </row>
     <row r="142" spans="1:1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A142" s="7" t="s">
-        <v>490</v>
+        <v>489</v>
       </c>
     </row>
     <row r="143" spans="1:1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A143" s="7" t="s">
-        <v>491</v>
+        <v>490</v>
       </c>
     </row>
     <row r="144" spans="1:1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A144" s="7" t="s">
-        <v>492</v>
+        <v>491</v>
       </c>
     </row>
     <row r="145" spans="1:1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A145" s="7" t="s">
-        <v>493</v>
+        <v>492</v>
       </c>
     </row>
     <row r="146" spans="1:1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A146" s="7" t="s">
-        <v>494</v>
+        <v>493</v>
       </c>
     </row>
     <row r="147" spans="1:1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A147" s="7" t="s">
-        <v>495</v>
+        <v>494</v>
       </c>
     </row>
     <row r="148" spans="1:1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A148" s="7" t="s">
-        <v>496</v>
+        <v>495</v>
       </c>
     </row>
     <row r="149" spans="1:1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A149" s="7" t="s">
-        <v>497</v>
+        <v>496</v>
       </c>
     </row>
     <row r="150" spans="1:1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A150" s="7" t="s">
-        <v>498</v>
+        <v>497</v>
       </c>
     </row>
     <row r="151" spans="1:1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A151" s="7" t="s">
-        <v>499</v>
+        <v>498</v>
       </c>
     </row>
     <row r="152" spans="1:1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A152" s="7" t="s">
-        <v>500</v>
+        <v>499</v>
       </c>
     </row>
     <row r="153" spans="1:1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A153" s="7" t="s">
-        <v>501</v>
+        <v>500</v>
       </c>
     </row>
     <row r="154" spans="1:1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A154" s="7" t="s">
-        <v>502</v>
+        <v>501</v>
       </c>
     </row>
     <row r="155" spans="1:1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A155" s="7" t="s">
-        <v>503</v>
+        <v>502</v>
       </c>
     </row>
     <row r="156" spans="1:1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A156" s="7" t="s">
-        <v>504</v>
+        <v>503</v>
       </c>
     </row>
     <row r="157" spans="1:1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A157" s="7" t="s">
-        <v>505</v>
+        <v>504</v>
       </c>
     </row>
     <row r="158" spans="1:1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A158" s="7" t="s">
-        <v>506</v>
+        <v>505</v>
       </c>
     </row>
     <row r="159" spans="1:1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A159" s="7" t="s">
-        <v>507</v>
+        <v>506</v>
       </c>
     </row>
     <row r="160" spans="1:1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A160" s="7" t="s">
-        <v>508</v>
+        <v>507</v>
       </c>
     </row>
     <row r="161" spans="1:1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A161" s="7" t="s">
-        <v>509</v>
+        <v>508</v>
       </c>
     </row>
     <row r="162" spans="1:1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A162" s="7" t="s">
-        <v>510</v>
+        <v>509</v>
       </c>
     </row>
     <row r="163" spans="1:1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A163" s="7" t="s">
-        <v>511</v>
+        <v>510</v>
       </c>
     </row>
     <row r="164" spans="1:1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A164" s="7" t="s">
-        <v>369</v>
+        <v>368</v>
       </c>
     </row>
     <row r="165" spans="1:1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A165" s="7" t="s">
-        <v>368</v>
+        <v>367</v>
       </c>
     </row>
     <row r="166" spans="1:1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A166" s="7" t="s">
-        <v>512</v>
+        <v>511</v>
       </c>
     </row>
     <row r="167" spans="1:1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A167" s="7" t="s">
-        <v>513</v>
+        <v>512</v>
       </c>
     </row>
     <row r="168" spans="1:1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A168" s="7" t="s">
-        <v>514</v>
+        <v>513</v>
       </c>
     </row>
     <row r="169" spans="1:1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A169" s="7" t="s">
-        <v>515</v>
+        <v>514</v>
       </c>
     </row>
     <row r="170" spans="1:1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A170" s="7" t="s">
-        <v>516</v>
+        <v>515</v>
       </c>
     </row>
     <row r="171" spans="1:1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A171" s="7" t="s">
-        <v>517</v>
+        <v>516</v>
       </c>
     </row>
     <row r="172" spans="1:1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A172" s="7" t="s">
-        <v>518</v>
+        <v>517</v>
       </c>
     </row>
     <row r="173" spans="1:1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A173" s="7" t="s">
-        <v>519</v>
+        <v>518</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Added feedback for client commands. Cleanup and TODO's.
</commit_message>
<xml_diff>
--- a/Miscellaneous/Packets.xlsx
+++ b/Miscellaneous/Packets.xlsx
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="979" uniqueCount="536">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="980" uniqueCount="537">
   <si>
     <t>Message ID</t>
   </si>
@@ -1629,6 +1629,9 @@
   </si>
   <si>
     <t>Username or Password Wrong</t>
+  </si>
+  <si>
+    <t>100</t>
   </si>
 </sst>
 </file>
@@ -3239,8 +3242,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AMK124"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A81" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C92" sqref="C92"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3279,8 +3282,8 @@
       </c>
     </row>
     <row r="2" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="6">
-        <v>0</v>
+      <c r="A2" s="6" t="s">
+        <v>536</v>
       </c>
       <c r="B2" s="2" t="s">
         <v>24</v>

</xml_diff>